<commit_message>
Add login test case
</commit_message>
<xml_diff>
--- a/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\OneDrive - Hanoi University of Science and Technology\BaiGiang\Quantriduan\DemoTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Subject\Ky1Nam5\IT4240\Btl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4F35652-5374-4CF0-A1FB-F90841B8B095}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="16" r:id="rId1"/>
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$102</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="H28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="J28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="A29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="H30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="I30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="J30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="A31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="H32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="I32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="A33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -311,9 +310,6 @@
     <t>1.</t>
   </si>
   <si>
-    <t>Test với tham số mặc định</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
@@ -335,16 +331,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Không có tham số dòng lệnh
-</t>
-  </si>
-  <si>
-    <t>1. Gõ duy nhất tên chương trình, không có tham số dòng lệnh</t>
-  </si>
-  <si>
-    <t>Chạy được</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -357,9 +343,6 @@
     <t>Repairer</t>
   </si>
   <si>
-    <t>1.1-1</t>
-  </si>
-  <si>
     <t>DinhPX</t>
   </si>
   <si>
@@ -378,21 +361,6 @@
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
-    <t>Không có tham số dòng lệnh, nhưng nhập từ Task Manager</t>
-  </si>
-  <si>
-    <t>BUG21312</t>
-  </si>
-  <si>
-    <t>1.2.1-1</t>
-  </si>
-  <si>
-    <t>AnhDV</t>
-  </si>
-  <si>
-    <t>TienND</t>
-  </si>
-  <si>
     <t>23/08/2008</t>
   </si>
   <si>
@@ -408,38 +376,64 @@
     <t xml:space="preserve">Test với tham số chỉ định \ Test với tham số -r </t>
   </si>
   <si>
-    <t>File Mpeg có thời lượng 3s</t>
-  </si>
-  <si>
-    <t>1. Add film mpeg
-2. Mo VLC
-3. Gõ địa chỉ 192.168.0.5</t>
-  </si>
-  <si>
-    <t>Xem được phim</t>
-  </si>
-  <si>
-    <t>1.2.2-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Mpeg
-</t>
-  </si>
-  <si>
-    <t>BUG213</t>
-  </si>
-  <si>
-    <t>1.1-2</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Đăng nhập vào hệ thống</t>
+  </si>
+  <si>
+    <t>Đăng nhập với tên và mật khẩu chính xác</t>
+  </si>
+  <si>
+    <t>Hệ thống chuyển sang trang chủ</t>
+  </si>
+  <si>
+    <t>NgaPT</t>
+  </si>
+  <si>
+    <t>DangNhap_01</t>
+  </si>
+  <si>
+    <t>DangNhap_02</t>
+  </si>
+  <si>
+    <t>Đăng nhập sai tên người dùng</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị màn hình đăng nhập với thông báo "Tên đăng nhập hoặc mật khẩu không đúng"
+Focus tới trường "Tên đăng nhập"</t>
+  </si>
+  <si>
+    <t>DangNhap_03</t>
+  </si>
+  <si>
+    <t>Đăng nhập sai mật khẩu</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị màn hình đăng nhập với thông báo "Tên đăng nhập hoặc mật khẩu không đúng"
+Focus tới trường "Mật khẩu"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -618,6 +612,12 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -940,7 +940,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1217,25 +1217,16 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1245,14 +1236,68 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1272,68 +1317,71 @@
     <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1388,7 +1436,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1512,23 +1560,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1564,23 +1595,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1756,14 +1770,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor indexed="46"/>
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1889,13 +1903,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="127" t="s">
+      <c r="O6" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
+      <c r="P6" s="124"/>
+      <c r="Q6" s="124"/>
+      <c r="R6" s="124"/>
+      <c r="S6" s="124"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1905,11 +1919,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="Q7" s="127"/>
-      <c r="R7" s="127"/>
-      <c r="S7" s="127"/>
+      <c r="O7" s="124"/>
+      <c r="P7" s="124"/>
+      <c r="Q7" s="124"/>
+      <c r="R7" s="124"/>
+      <c r="S7" s="124"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -1964,12 +1978,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="128">
+      <c r="E11" s="125">
         <f ca="1">TODAY()</f>
         <v>43430</v>
       </c>
-      <c r="F11" s="128"/>
-      <c r="G11" s="128"/>
+      <c r="F11" s="125"/>
+      <c r="G11" s="125"/>
       <c r="H11" s="72"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -2823,14 +2837,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2861,8 +2875,8 @@
         <v>22</v>
       </c>
       <c r="I1" s="101">
-        <f>COUNTIF(H1:H786,"OK")</f>
-        <v>1</v>
+        <f>COUNTIF(H1:H792,"OK")</f>
+        <v>2</v>
       </c>
       <c r="J1" s="82" t="s">
         <v>23</v>
@@ -2885,7 +2899,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="102">
-        <f>COUNTIF(H2:H787,"Not OK")</f>
+        <f>COUNTIF(H2:H793,"Not OK")</f>
         <v>4</v>
       </c>
       <c r="J2" s="89" t="s">
@@ -2909,7 +2923,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="103">
-        <f>COUNTIF(H2:H787,"Untested")</f>
+        <f>COUNTIF(H2:H793,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="89" t="s">
@@ -2929,8 +2943,8 @@
       </c>
       <c r="H4" s="85"/>
       <c r="I4" s="102">
-        <f>COUNTIF(H3:H788,"Result")</f>
-        <v>5</v>
+        <f>COUNTIF(H3:H794,"Result")</f>
+        <v>6</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="90"/>
@@ -2965,775 +2979,855 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="156" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="156"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="156"/>
-      <c r="J7" s="156"/>
-      <c r="K7" s="156"/>
+      <c r="B7" s="126" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="129" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="129" t="s">
-        <v>36</v>
       </c>
       <c r="C8" s="130"/>
       <c r="D8" s="129" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="130"/>
       <c r="F8" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="130"/>
+      <c r="H8" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="130"/>
-      <c r="H8" s="157" t="s">
+      <c r="I8" s="128"/>
+      <c r="J8" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="157"/>
-      <c r="J8" s="118" t="s">
+      <c r="K8" s="47" t="s">
         <v>40</v>
-      </c>
-      <c r="K8" s="47" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="132" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="133"/>
-      <c r="D9" s="141" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="142"/>
-      <c r="F9" s="120" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="121"/>
-      <c r="H9" s="147" t="s">
+      <c r="B9" s="162" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="163"/>
+      <c r="D9" s="168" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="169"/>
+      <c r="F9" s="156" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="157"/>
+      <c r="H9" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="148"/>
+      <c r="I9" s="138"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="151"/>
+      <c r="K9" s="134"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="134"/>
-      <c r="C10" s="135"/>
-      <c r="D10" s="143"/>
-      <c r="E10" s="144"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="123"/>
+        <v>41</v>
+      </c>
+      <c r="B10" s="164"/>
+      <c r="C10" s="165"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="171"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="159"/>
       <c r="H10" s="117" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I10" s="117" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J10" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="152"/>
+        <v>44</v>
+      </c>
+      <c r="K10" s="135"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="134"/>
-      <c r="C11" s="135"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="144"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="123"/>
+        <v>56</v>
+      </c>
+      <c r="B11" s="164"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="170"/>
+      <c r="E11" s="171"/>
+      <c r="F11" s="158"/>
+      <c r="G11" s="159"/>
       <c r="H11" s="50" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="152"/>
+      <c r="K11" s="135"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="134"/>
-      <c r="C12" s="135"/>
-      <c r="D12" s="143"/>
-      <c r="E12" s="144"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="123"/>
+        <v>46</v>
+      </c>
+      <c r="B12" s="164"/>
+      <c r="C12" s="165"/>
+      <c r="D12" s="170"/>
+      <c r="E12" s="171"/>
+      <c r="F12" s="158"/>
+      <c r="G12" s="159"/>
       <c r="H12" s="117" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I12" s="117" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J12" s="117"/>
-      <c r="K12" s="152"/>
+      <c r="K12" s="135"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
-        <v>981</v>
-      </c>
-      <c r="B13" s="136"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="145"/>
-      <c r="E13" s="146"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="125"/>
-      <c r="H13" s="53" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="B13" s="166"/>
+      <c r="C13" s="167"/>
+      <c r="D13" s="172"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="161"/>
+      <c r="H13" s="53">
+        <v>43434</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="153"/>
+      <c r="K13" s="136"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="139" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="140"/>
-      <c r="D14" s="139" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="132" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="133"/>
+      <c r="D14" s="132" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="133"/>
+      <c r="F14" s="132" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="140"/>
-      <c r="F14" s="139" t="s">
+      <c r="G14" s="133"/>
+      <c r="H14" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="140"/>
-      <c r="H14" s="138" t="s">
+      <c r="I14" s="133"/>
+      <c r="J14" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="138"/>
-      <c r="J14" s="126" t="s">
+      <c r="K14" s="56" t="s">
         <v>40</v>
-      </c>
-      <c r="K14" s="56" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="132" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="133"/>
-      <c r="D15" s="141" t="s">
+      <c r="B15" s="162" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="163"/>
+      <c r="D15" s="168" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="169"/>
+      <c r="F15" s="168" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="169"/>
+      <c r="H15" s="137" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="138"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="134"/>
+    </row>
+    <row r="16" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A16" s="122" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="164"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="170"/>
+      <c r="E16" s="171"/>
+      <c r="F16" s="170"/>
+      <c r="G16" s="171"/>
+      <c r="H16" s="122" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="142"/>
-      <c r="F15" s="120" t="s">
+      <c r="J16" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="121"/>
-      <c r="H15" s="149" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="150"/>
-      <c r="J15" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="151"/>
-    </row>
-    <row r="16" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A16" s="126" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="134"/>
-      <c r="C16" s="135"/>
-      <c r="D16" s="143"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="126" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="126" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="152"/>
+      <c r="K16" s="135"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="134"/>
-      <c r="C17" s="135"/>
-      <c r="D17" s="143"/>
-      <c r="E17" s="144"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="123"/>
+        <v>57</v>
+      </c>
+      <c r="B17" s="164"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="170"/>
+      <c r="E17" s="171"/>
+      <c r="F17" s="170"/>
+      <c r="G17" s="171"/>
       <c r="H17" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="K17" s="152"/>
+        <v>64</v>
+      </c>
+      <c r="I17" s="50"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="135"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="126" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="134"/>
-      <c r="C18" s="135"/>
-      <c r="D18" s="143"/>
-      <c r="E18" s="144"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="126" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="126" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="126"/>
-      <c r="K18" s="152"/>
+      <c r="A18" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="164"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="170"/>
+      <c r="E18" s="171"/>
+      <c r="F18" s="170"/>
+      <c r="G18" s="171"/>
+      <c r="H18" s="122" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="122" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="122"/>
+      <c r="K18" s="135"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
-        <v>921</v>
-      </c>
-      <c r="B19" s="136"/>
-      <c r="C19" s="137"/>
-      <c r="D19" s="145"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="166"/>
+      <c r="C19" s="167"/>
+      <c r="D19" s="172"/>
+      <c r="E19" s="173"/>
+      <c r="F19" s="172"/>
+      <c r="G19" s="173"/>
+      <c r="H19" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I19" s="50"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="135"/>
+    </row>
+    <row r="20" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A20" s="121" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="130"/>
+      <c r="D20" s="129" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="130"/>
+      <c r="F20" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="130"/>
+      <c r="H20" s="128" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="128"/>
+      <c r="J20" s="123" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A21" s="48">
+        <v>3</v>
+      </c>
+      <c r="B21" s="162" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="163"/>
+      <c r="D21" s="168" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="169"/>
+      <c r="F21" s="174" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="157"/>
+      <c r="H21" s="137" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="138"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="134"/>
+    </row>
+    <row r="22" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A22" s="121" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="164"/>
+      <c r="C22" s="165"/>
+      <c r="D22" s="170"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="159"/>
+      <c r="H22" s="121" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="121" t="s">
+        <v>44</v>
+      </c>
+      <c r="K22" s="135"/>
+    </row>
+    <row r="23" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A23" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="164"/>
+      <c r="C23" s="165"/>
+      <c r="D23" s="170"/>
+      <c r="E23" s="171"/>
+      <c r="F23" s="158"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="50"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="135"/>
+    </row>
+    <row r="24" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A24" s="121" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="164"/>
+      <c r="C24" s="165"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="158"/>
+      <c r="G24" s="159"/>
+      <c r="H24" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="121" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="121"/>
+      <c r="K24" s="135"/>
+    </row>
+    <row r="25" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A25" s="51">
+        <v>3</v>
+      </c>
+      <c r="B25" s="166"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="172"/>
+      <c r="E25" s="173"/>
+      <c r="F25" s="160"/>
+      <c r="G25" s="161"/>
+      <c r="H25" s="53">
+        <v>43434</v>
+      </c>
+      <c r="I25" s="53"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="136"/>
+    </row>
+    <row r="26" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A26" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="131"/>
+      <c r="D26" s="126"/>
+      <c r="E26" s="126"/>
+      <c r="F26" s="126"/>
+      <c r="G26" s="126"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="126"/>
+      <c r="K26" s="126"/>
+    </row>
+    <row r="27" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A27" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" s="48"/>
-      <c r="K19" s="152"/>
-    </row>
-    <row r="20" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A20" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="158" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="158"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="156"/>
-      <c r="F20" s="156"/>
-      <c r="G20" s="156"/>
-      <c r="H20" s="156"/>
-      <c r="I20" s="156"/>
-      <c r="J20" s="156"/>
-      <c r="K20" s="156"/>
-    </row>
-    <row r="21" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A21" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="154" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="154"/>
-      <c r="D21" s="155"/>
-      <c r="E21" s="155"/>
-      <c r="F21" s="155"/>
-      <c r="G21" s="155"/>
-      <c r="H21" s="155"/>
-      <c r="I21" s="155"/>
-      <c r="J21" s="155"/>
-      <c r="K21" s="155"/>
-    </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A22" s="126" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="139" t="s">
+      <c r="B27" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="140"/>
-      <c r="D22" s="139" t="s">
+      <c r="C27" s="153"/>
+      <c r="D27" s="154"/>
+      <c r="E27" s="154"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="154"/>
+      <c r="H27" s="154"/>
+      <c r="I27" s="154"/>
+      <c r="J27" s="154"/>
+      <c r="K27" s="154"/>
+    </row>
+    <row r="28" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A28" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="132" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="133"/>
+      <c r="D28" s="132" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="133"/>
+      <c r="F28" s="132" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="140"/>
-      <c r="F22" s="139" t="s">
+      <c r="G28" s="133"/>
+      <c r="H28" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="140"/>
-      <c r="H22" s="138" t="s">
+      <c r="I28" s="155"/>
+      <c r="J28" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="138"/>
-      <c r="J22" s="126" t="s">
+      <c r="K28" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="K22" s="126" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A23" s="48">
+    </row>
+    <row r="29" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A29" s="48">
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B23" s="132" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="133"/>
-      <c r="D23" s="141" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="142"/>
-      <c r="F23" s="141" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="142"/>
-      <c r="H23" s="147" t="s">
+      <c r="B29" s="147"/>
+      <c r="C29" s="148"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="148"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="151"/>
-    </row>
-    <row r="24" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A24" s="126" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="134"/>
-      <c r="C24" s="135"/>
-      <c r="D24" s="143"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="143"/>
-      <c r="G24" s="144"/>
-      <c r="H24" s="126" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="126" t="s">
-        <v>47</v>
-      </c>
-      <c r="J24" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="K24" s="152"/>
-    </row>
-    <row r="25" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A25" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="134"/>
-      <c r="C25" s="135"/>
-      <c r="D25" s="143"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="144"/>
-      <c r="H25" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="50"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="152"/>
-    </row>
-    <row r="26" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A26" s="126" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="134"/>
-      <c r="C26" s="135"/>
-      <c r="D26" s="143"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="143"/>
-      <c r="G26" s="144"/>
-      <c r="H26" s="126" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="152"/>
-    </row>
-    <row r="27" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A27" s="51">
-        <v>922</v>
-      </c>
-      <c r="B27" s="136"/>
-      <c r="C27" s="137"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="146"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="146"/>
-      <c r="H27" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="153"/>
-    </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A28" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="129" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="130"/>
-      <c r="D28" s="129" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="130"/>
-      <c r="F28" s="129" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="130"/>
-      <c r="H28" s="131" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="131"/>
-      <c r="J28" s="117" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="119" t="s">
+      <c r="I29" s="138"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="134"/>
+    </row>
+    <row r="30" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A30" s="120" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A29" s="48">
-        <v>4</v>
-      </c>
-      <c r="B29" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="133"/>
-      <c r="D29" s="141" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="142"/>
-      <c r="F29" s="141" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="142"/>
-      <c r="H29" s="149" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="150"/>
-      <c r="J29" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="K29" s="151"/>
-    </row>
-    <row r="30" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A30" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="134"/>
-      <c r="C30" s="135"/>
-      <c r="D30" s="143"/>
-      <c r="E30" s="144"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="144"/>
-      <c r="H30" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="J30" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="K30" s="152"/>
+      <c r="B30" s="149"/>
+      <c r="C30" s="150"/>
+      <c r="D30" s="141"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="141"/>
+      <c r="G30" s="142"/>
+      <c r="H30" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" s="120" t="s">
+        <v>44</v>
+      </c>
+      <c r="K30" s="135"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="134"/>
-      <c r="C31" s="135"/>
-      <c r="D31" s="143"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="143"/>
-      <c r="G31" s="144"/>
+        <v>58</v>
+      </c>
+      <c r="B31" s="149"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="141"/>
+      <c r="G31" s="142"/>
       <c r="H31" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="J31" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="K31" s="152"/>
+        <v>45</v>
+      </c>
+      <c r="I31" s="50"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="135"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A32" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="134"/>
-      <c r="C32" s="135"/>
-      <c r="D32" s="143"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="143"/>
-      <c r="G32" s="144"/>
-      <c r="H32" s="117" t="s">
-        <v>52</v>
-      </c>
-      <c r="I32" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="J32" s="117"/>
-      <c r="K32" s="152"/>
+      <c r="A32" s="120" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="149"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="141"/>
+      <c r="G32" s="142"/>
+      <c r="H32" s="120" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" s="120"/>
+      <c r="J32" s="120"/>
+      <c r="K32" s="135"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="51">
-        <v>823</v>
-      </c>
-      <c r="B33" s="136"/>
-      <c r="C33" s="137"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="146"/>
-      <c r="F33" s="145"/>
-      <c r="G33" s="146"/>
+        <v>3</v>
+      </c>
+      <c r="B33" s="151"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="143"/>
+      <c r="E33" s="144"/>
+      <c r="F33" s="143"/>
+      <c r="G33" s="144"/>
       <c r="H33" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="I33" s="50" t="s">
-        <v>61</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="I33" s="50"/>
       <c r="J33" s="48"/>
-      <c r="K33" s="153"/>
+      <c r="K33" s="136"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="129" t="s">
         <v>35</v>
-      </c>
-      <c r="B34" s="129" t="s">
-        <v>36</v>
       </c>
       <c r="C34" s="130"/>
       <c r="D34" s="129" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E34" s="130"/>
       <c r="F34" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="130"/>
+      <c r="H34" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="130"/>
-      <c r="H34" s="131" t="s">
+      <c r="I34" s="127"/>
+      <c r="J34" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="131"/>
-      <c r="J34" s="117" t="s">
+      <c r="K34" s="119" t="s">
         <v>40</v>
-      </c>
-      <c r="K34" s="119" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="48">
-        <v>5</v>
-      </c>
-      <c r="B35" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="133"/>
-      <c r="D35" s="141" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="142"/>
-      <c r="F35" s="141" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="142"/>
-      <c r="H35" s="149" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="147"/>
+      <c r="C35" s="148"/>
+      <c r="D35" s="139"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="139"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="145" t="s">
         <v>10</v>
       </c>
-      <c r="I35" s="150"/>
-      <c r="J35" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="K35" s="151"/>
+      <c r="I35" s="146"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="134"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="134"/>
-      <c r="C36" s="135"/>
-      <c r="D36" s="143"/>
-      <c r="E36" s="144"/>
-      <c r="F36" s="143"/>
-      <c r="G36" s="144"/>
+        <v>41</v>
+      </c>
+      <c r="B36" s="149"/>
+      <c r="C36" s="150"/>
+      <c r="D36" s="141"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="141"/>
+      <c r="G36" s="142"/>
       <c r="H36" s="117" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I36" s="117" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J36" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="K36" s="152"/>
+        <v>44</v>
+      </c>
+      <c r="K36" s="135"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="134"/>
-      <c r="C37" s="135"/>
-      <c r="D37" s="143"/>
-      <c r="E37" s="144"/>
-      <c r="F37" s="143"/>
-      <c r="G37" s="144"/>
+        <v>59</v>
+      </c>
+      <c r="B37" s="149"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="141"/>
+      <c r="E37" s="142"/>
+      <c r="F37" s="141"/>
+      <c r="G37" s="142"/>
       <c r="H37" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="J37" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="K37" s="152"/>
+        <v>45</v>
+      </c>
+      <c r="I37" s="50"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="135"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="134"/>
-      <c r="C38" s="135"/>
-      <c r="D38" s="143"/>
-      <c r="E38" s="144"/>
-      <c r="F38" s="143"/>
-      <c r="G38" s="144"/>
+        <v>46</v>
+      </c>
+      <c r="B38" s="149"/>
+      <c r="C38" s="150"/>
+      <c r="D38" s="141"/>
+      <c r="E38" s="142"/>
+      <c r="F38" s="141"/>
+      <c r="G38" s="142"/>
       <c r="H38" s="117" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I38" s="117" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J38" s="117"/>
-      <c r="K38" s="152"/>
+      <c r="K38" s="135"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="51">
-        <v>823</v>
-      </c>
-      <c r="B39" s="136"/>
-      <c r="C39" s="137"/>
-      <c r="D39" s="145"/>
-      <c r="E39" s="146"/>
-      <c r="F39" s="145"/>
-      <c r="G39" s="146"/>
+        <v>4</v>
+      </c>
+      <c r="B39" s="151"/>
+      <c r="C39" s="152"/>
+      <c r="D39" s="143"/>
+      <c r="E39" s="144"/>
+      <c r="F39" s="143"/>
+      <c r="G39" s="144"/>
       <c r="H39" s="50" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I39" s="50" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="J39" s="48"/>
-      <c r="K39" s="153"/>
-    </row>
-    <row r="40" spans="1:11" s="58" customFormat="1">
-      <c r="A40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
-    </row>
-    <row r="41" spans="1:11" s="58" customFormat="1">
-      <c r="A41" s="62"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="62"/>
-      <c r="K41" s="62"/>
-    </row>
-    <row r="42" spans="1:11" s="58" customFormat="1">
-      <c r="A42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-    </row>
-    <row r="43" spans="1:11" s="58" customFormat="1">
-      <c r="A43" s="62"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="62"/>
-      <c r="K43" s="62"/>
-    </row>
-    <row r="44" spans="1:11" s="58" customFormat="1">
-      <c r="A44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62"/>
-      <c r="K44" s="62"/>
-    </row>
-    <row r="45" spans="1:11" s="58" customFormat="1">
-      <c r="A45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="62"/>
-      <c r="K45" s="62"/>
-    </row>
-    <row r="46" spans="1:11" s="58" customFormat="1">
+      <c r="K39" s="136"/>
+    </row>
+    <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A40" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="130"/>
+      <c r="D40" s="129" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="130"/>
+      <c r="F40" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" s="130"/>
+      <c r="H40" s="127" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="127"/>
+      <c r="J40" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="119" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A41" s="48">
+        <v>5</v>
+      </c>
+      <c r="B41" s="147"/>
+      <c r="C41" s="148"/>
+      <c r="D41" s="139"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="139"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="145" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="146"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="134"/>
+    </row>
+    <row r="42" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A42" s="117" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="149"/>
+      <c r="C42" s="150"/>
+      <c r="D42" s="141"/>
+      <c r="E42" s="142"/>
+      <c r="F42" s="141"/>
+      <c r="G42" s="142"/>
+      <c r="H42" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="117" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="135"/>
+    </row>
+    <row r="43" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A43" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="149"/>
+      <c r="C43" s="150"/>
+      <c r="D43" s="141"/>
+      <c r="E43" s="142"/>
+      <c r="F43" s="141"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="50"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="135"/>
+    </row>
+    <row r="44" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A44" s="117" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="149"/>
+      <c r="C44" s="150"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="142"/>
+      <c r="F44" s="141"/>
+      <c r="G44" s="142"/>
+      <c r="H44" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="I44" s="117" t="s">
+        <v>48</v>
+      </c>
+      <c r="J44" s="117"/>
+      <c r="K44" s="135"/>
+    </row>
+    <row r="45" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A45" s="51">
+        <v>5</v>
+      </c>
+      <c r="B45" s="151"/>
+      <c r="C45" s="152"/>
+      <c r="D45" s="143"/>
+      <c r="E45" s="144"/>
+      <c r="F45" s="143"/>
+      <c r="G45" s="144"/>
+      <c r="H45" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="I45" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J45" s="48"/>
+      <c r="K45" s="136"/>
+    </row>
+    <row r="46" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A46" s="62"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
       <c r="H46" s="62"/>
       <c r="I46" s="62"/>
       <c r="J46" s="62"/>
       <c r="K46" s="62"/>
     </row>
-    <row r="47" spans="1:11" s="58" customFormat="1">
+    <row r="47" spans="1:11" ht="10.5" customHeight="1">
       <c r="A47" s="62"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
       <c r="H47" s="62"/>
       <c r="I47" s="62"/>
       <c r="J47" s="62"/>
       <c r="K47" s="62"/>
     </row>
-    <row r="48" spans="1:11" s="58" customFormat="1">
+    <row r="48" spans="1:11" ht="10.5" customHeight="1">
       <c r="A48" s="62"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
       <c r="H48" s="62"/>
       <c r="I48" s="62"/>
       <c r="J48" s="62"/>
       <c r="K48" s="62"/>
     </row>
-    <row r="49" spans="1:11" s="58" customFormat="1">
+    <row r="49" spans="1:11" ht="10.5" customHeight="1">
       <c r="A49" s="62"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
       <c r="H49" s="62"/>
       <c r="I49" s="62"/>
       <c r="J49" s="62"/>
       <c r="K49" s="62"/>
     </row>
-    <row r="50" spans="1:11" s="58" customFormat="1">
+    <row r="50" spans="1:11" ht="10.5" customHeight="1">
       <c r="A50" s="62"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
       <c r="H50" s="62"/>
       <c r="I50" s="62"/>
       <c r="J50" s="62"/>
       <c r="K50" s="62"/>
     </row>
-    <row r="51" spans="1:11" s="58" customFormat="1">
+    <row r="51" spans="1:11" ht="10.5" customHeight="1">
       <c r="A51" s="62"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
       <c r="H51" s="62"/>
       <c r="I51" s="62"/>
       <c r="J51" s="62"/>
@@ -4054,62 +4148,193 @@
       <c r="J96" s="62"/>
       <c r="K96" s="62"/>
     </row>
+    <row r="97" spans="1:11" s="58" customFormat="1">
+      <c r="A97" s="62"/>
+      <c r="H97" s="62"/>
+      <c r="I97" s="62"/>
+      <c r="J97" s="62"/>
+      <c r="K97" s="62"/>
+    </row>
+    <row r="98" spans="1:11" s="58" customFormat="1">
+      <c r="A98" s="62"/>
+      <c r="H98" s="62"/>
+      <c r="I98" s="62"/>
+      <c r="J98" s="62"/>
+      <c r="K98" s="62"/>
+    </row>
+    <row r="99" spans="1:11" s="58" customFormat="1">
+      <c r="A99" s="62"/>
+      <c r="H99" s="62"/>
+      <c r="I99" s="62"/>
+      <c r="J99" s="62"/>
+      <c r="K99" s="62"/>
+    </row>
+    <row r="100" spans="1:11" s="58" customFormat="1">
+      <c r="A100" s="62"/>
+      <c r="H100" s="62"/>
+      <c r="I100" s="62"/>
+      <c r="J100" s="62"/>
+      <c r="K100" s="62"/>
+    </row>
+    <row r="101" spans="1:11" s="58" customFormat="1">
+      <c r="A101" s="62"/>
+      <c r="H101" s="62"/>
+      <c r="I101" s="62"/>
+      <c r="J101" s="62"/>
+      <c r="K101" s="62"/>
+    </row>
+    <row r="102" spans="1:11" s="58" customFormat="1">
+      <c r="A102" s="62"/>
+      <c r="H102" s="62"/>
+      <c r="I102" s="62"/>
+      <c r="J102" s="62"/>
+      <c r="K102" s="62"/>
+    </row>
+    <row r="103" spans="1:11" s="58" customFormat="1">
+      <c r="A103" s="2"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="1:11" s="58" customFormat="1">
+      <c r="A104" s="2"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+    </row>
+    <row r="105" spans="1:11" s="58" customFormat="1">
+      <c r="A105" s="2"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+    </row>
+    <row r="106" spans="1:11" s="58" customFormat="1">
+      <c r="A106" s="2"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+    </row>
+    <row r="107" spans="1:11" s="58" customFormat="1">
+      <c r="A107" s="2"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+    </row>
+    <row r="108" spans="1:11" s="58" customFormat="1">
+      <c r="A108" s="2"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="K23:K27"/>
-    <mergeCell ref="D23:E27"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G27"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
+  <mergeCells count="57">
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="B35:C39"/>
-    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="F9:G13"/>
+    <mergeCell ref="F15:G19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="F21:G25"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B41:C45"/>
     <mergeCell ref="D35:E39"/>
-    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="D41:E45"/>
+    <mergeCell ref="F41:G45"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="D9:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C27"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="D15:E19"/>
     <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="K41:K45"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="B7:K7"/>
     <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B26:K26"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="H35:I35">
+  <conditionalFormatting sqref="H41:I41">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:I34">
+  <conditionalFormatting sqref="H40:I40">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add xemchitiet test case
</commit_message>
<xml_diff>
--- a/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$102</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$95</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -30,183 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Nguyen Duc Tien</author>
-  </authors>
-  <commentList>
-    <comment ref="B27" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Point \ Point 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H28" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Kết quả test:
-OK / Not OK</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J28" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Ánh xạ tới ID tương ứng của Bug được ghi nhận trong BugList</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A29" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Số thứ tự tăng dần testcase, không phần biệt sheet,...
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Người thực hiện test</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Người chịu trách nhiệm về lỗi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Người sửa lỗi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A31" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>SheetNo.Suite.Suite-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>CaseNo</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-CaseNo tăng dần và lặp lại từ 1 giữa các Suite-Point khác nhau</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H32" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Ngày thực hiện test</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I32" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Ngày test lại, trong trường hợp lần test trước có lỗi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>ID tương ứng của TestLink</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -343,9 +168,6 @@
     <t>Repairer</t>
   </si>
   <si>
-    <t>DinhPX</t>
-  </si>
-  <si>
     <t>Online ID</t>
   </si>
   <si>
@@ -355,40 +177,10 @@
     <t>Cpl. Date</t>
   </si>
   <si>
-    <t>20/08/2008</t>
-  </si>
-  <si>
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
-    <t>23/08/2008</t>
-  </si>
-  <si>
     <t>2.</t>
-  </si>
-  <si>
-    <t>Test với tham số chỉ định</t>
-  </si>
-  <si>
-    <t>2.1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test với tham số chỉ định \ Test với tham số -r </t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t>Đăng nhập vào hệ thống</t>
@@ -424,6 +216,74 @@
   <si>
     <t>Hệ thống hiển thị màn hình đăng nhập với thông báo "Tên đăng nhập hoặc mật khẩu không đúng"
 Focus tới trường "Mật khẩu"</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>Xem thông tin chi tiết món ăn</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>XemThongTinChiTietMonAn_01</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem có hiện đầy đủ thông tin chi tiết món ăn không</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị đầy đủ thông tin chi tiết của món ăn đã chọn, gồm:
+- Tên món ăn
+- Nguyên liệu, phần, thời gian thực hiện, độ khó
+- Mục đích
+- Đánh giá của người dùng
+- Mô tả
+- Tác giả
+- Các bài viết liên quan tới món ăn
+- Công thức nấu
+- Hình ảnh, video món ăn (nếu có)
+- Đánh giá của người dùng (nếu có)</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>XemThongTinChiTietMonAn_02</t>
+  </si>
+  <si>
+    <t>Đánh giá (rate) món ăn</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị đánh giá thành công:
+- Tăng số lượng người đánh giá
+- Điểm đánh giá trung bình cho món ăn được tổng hợp lại</t>
+  </si>
+  <si>
+    <t>XemThongTinChiTietMonAn_03</t>
+  </si>
+  <si>
+    <t>Xem thông tin bài viết liên quan</t>
+  </si>
+  <si>
+    <t>Hệ thống được chuyển hướng tới bài viết tương ứng</t>
+  </si>
+  <si>
+    <t>XemThongTinChiTietMonAn_04</t>
+  </si>
+  <si>
+    <t>Đánh giá (bình luận) món ăn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hệ thống cho phép bình luận
+Bình luận được lưu lại và hiển thị ngay sau khi submit
+</t>
   </si>
 </sst>
 </file>
@@ -433,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -459,24 +319,6 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -940,7 +782,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -948,447 +790,494 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="21" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="18" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="18" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1436,7 +1325,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1961,7 +1850,7 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
-      <c r="L10" s="114" t="s">
+      <c r="L10" s="113" t="s">
         <v>5</v>
       </c>
       <c r="O10" s="21"/>
@@ -2224,26 +2113,26 @@
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
-      <c r="O19" s="112">
+      <c r="O19" s="111">
         <f>SUM(O12:O18)</f>
         <v>284</v>
       </c>
-      <c r="P19" s="112"/>
-      <c r="Q19" s="112">
+      <c r="P19" s="111"/>
+      <c r="Q19" s="111">
         <f>SUM(Q12:Q18)</f>
         <v>285</v>
       </c>
-      <c r="R19" s="112"/>
-      <c r="S19" s="112">
+      <c r="R19" s="111"/>
+      <c r="S19" s="111">
         <f>SUM(S12:S18)</f>
         <v>286</v>
       </c>
-      <c r="T19" s="112"/>
-      <c r="U19" s="113">
+      <c r="T19" s="111"/>
+      <c r="U19" s="112">
         <f>SUM(U12:U18)</f>
         <v>855</v>
       </c>
-      <c r="V19" s="113"/>
+      <c r="V19" s="112"/>
       <c r="W19" s="74"/>
       <c r="X19" s="19"/>
     </row>
@@ -2298,19 +2187,19 @@
       <c r="F24" s="44"/>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
-      <c r="L24" s="114" t="s">
+      <c r="L24" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="104"/>
-      <c r="N24" s="104"/>
-      <c r="O24" s="104"/>
-      <c r="P24" s="105"/>
-      <c r="Q24" s="105"/>
-      <c r="R24" s="105"/>
-      <c r="S24" s="105"/>
-      <c r="T24" s="105"/>
-      <c r="U24" s="105"/>
-      <c r="V24" s="105"/>
+      <c r="M24" s="103"/>
+      <c r="N24" s="103"/>
+      <c r="O24" s="103"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="104"/>
+      <c r="V24" s="104"/>
       <c r="W24" s="73"/>
       <c r="X24" s="23"/>
     </row>
@@ -2320,17 +2209,17 @@
       <c r="F25" s="44"/>
       <c r="G25" s="44"/>
       <c r="H25" s="44"/>
-      <c r="L25" s="106"/>
-      <c r="M25" s="107"/>
-      <c r="N25" s="107"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="108"/>
-      <c r="Q25" s="108"/>
-      <c r="R25" s="108"/>
-      <c r="S25" s="108"/>
-      <c r="T25" s="108"/>
-      <c r="U25" s="108"/>
-      <c r="V25" s="108"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="107"/>
+      <c r="S25" s="107"/>
+      <c r="T25" s="107"/>
+      <c r="U25" s="107"/>
+      <c r="V25" s="107"/>
       <c r="W25" s="73"/>
       <c r="X25" s="23"/>
     </row>
@@ -2340,17 +2229,17 @@
       <c r="F26" s="44"/>
       <c r="G26" s="44"/>
       <c r="H26" s="44"/>
-      <c r="L26" s="106"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="108"/>
-      <c r="Q26" s="108"/>
-      <c r="R26" s="108"/>
-      <c r="S26" s="108"/>
-      <c r="T26" s="108"/>
-      <c r="U26" s="108"/>
-      <c r="V26" s="108"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="106"/>
+      <c r="N26" s="106"/>
+      <c r="O26" s="106"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="107"/>
+      <c r="S26" s="107"/>
+      <c r="T26" s="107"/>
+      <c r="U26" s="107"/>
+      <c r="V26" s="107"/>
       <c r="W26" s="73"/>
       <c r="X26" s="23"/>
       <c r="AB26" s="76"/>
@@ -2359,17 +2248,17 @@
       <c r="B27" s="22"/>
       <c r="D27" s="38"/>
       <c r="E27" s="4"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="107"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="107"/>
-      <c r="P27" s="108"/>
-      <c r="Q27" s="108"/>
-      <c r="R27" s="108"/>
-      <c r="S27" s="108"/>
-      <c r="T27" s="108"/>
-      <c r="U27" s="108"/>
-      <c r="V27" s="108"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="106"/>
+      <c r="N27" s="106"/>
+      <c r="O27" s="106"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
+      <c r="S27" s="107"/>
+      <c r="T27" s="107"/>
+      <c r="U27" s="107"/>
+      <c r="V27" s="107"/>
       <c r="W27" s="73"/>
       <c r="X27" s="23"/>
       <c r="AB27" s="76"/>
@@ -2378,17 +2267,17 @@
       <c r="B28" s="22"/>
       <c r="D28" s="38"/>
       <c r="E28" s="4"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="108"/>
-      <c r="Q28" s="108"/>
-      <c r="R28" s="108"/>
-      <c r="S28" s="108"/>
-      <c r="T28" s="108"/>
-      <c r="U28" s="108"/>
-      <c r="V28" s="108"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="106"/>
+      <c r="N28" s="106"/>
+      <c r="O28" s="106"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
+      <c r="T28" s="107"/>
+      <c r="U28" s="107"/>
+      <c r="V28" s="107"/>
       <c r="W28" s="73"/>
       <c r="X28" s="23"/>
       <c r="AB28" s="76"/>
@@ -2401,33 +2290,33 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="K29" s="31"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="108"/>
-      <c r="Q29" s="108"/>
-      <c r="R29" s="108"/>
-      <c r="S29" s="108"/>
-      <c r="T29" s="108"/>
-      <c r="U29" s="108"/>
-      <c r="V29" s="108"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="106"/>
+      <c r="N29" s="106"/>
+      <c r="O29" s="106"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="107"/>
+      <c r="T29" s="107"/>
+      <c r="U29" s="107"/>
+      <c r="V29" s="107"/>
       <c r="W29" s="73"/>
       <c r="X29" s="23"/>
     </row>
     <row r="30" spans="2:35" s="17" customFormat="1">
       <c r="B30" s="22"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="107"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="108"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="108"/>
-      <c r="S30" s="108"/>
-      <c r="T30" s="108"/>
-      <c r="U30" s="108"/>
-      <c r="V30" s="108"/>
+      <c r="L30" s="105"/>
+      <c r="M30" s="106"/>
+      <c r="N30" s="106"/>
+      <c r="O30" s="106"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
+      <c r="T30" s="107"/>
+      <c r="U30" s="107"/>
+      <c r="V30" s="107"/>
       <c r="W30" s="73"/>
       <c r="X30" s="23"/>
     </row>
@@ -2444,17 +2333,17 @@
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
-      <c r="L31" s="109"/>
-      <c r="M31" s="107"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="108"/>
-      <c r="Q31" s="108"/>
-      <c r="R31" s="108"/>
-      <c r="S31" s="108"/>
-      <c r="T31" s="108"/>
-      <c r="U31" s="108"/>
-      <c r="V31" s="108"/>
+      <c r="L31" s="108"/>
+      <c r="M31" s="106"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="106"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
+      <c r="S31" s="107"/>
+      <c r="T31" s="107"/>
+      <c r="U31" s="107"/>
+      <c r="V31" s="107"/>
       <c r="W31" s="73"/>
       <c r="X31" s="23"/>
       <c r="AA31" s="17"/>
@@ -2480,17 +2369,17 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
-      <c r="L32" s="106"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="108"/>
-      <c r="Q32" s="108"/>
-      <c r="R32" s="108"/>
-      <c r="S32" s="108"/>
-      <c r="T32" s="108"/>
-      <c r="U32" s="108"/>
-      <c r="V32" s="108"/>
+      <c r="L32" s="105"/>
+      <c r="M32" s="106"/>
+      <c r="N32" s="106"/>
+      <c r="O32" s="106"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="107"/>
+      <c r="R32" s="107"/>
+      <c r="S32" s="107"/>
+      <c r="T32" s="107"/>
+      <c r="U32" s="107"/>
+      <c r="V32" s="107"/>
       <c r="W32" s="73"/>
       <c r="X32" s="23"/>
       <c r="AA32" s="17"/>
@@ -2514,17 +2403,17 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="106"/>
-      <c r="M33" s="110"/>
-      <c r="N33" s="107"/>
-      <c r="O33" s="107"/>
-      <c r="P33" s="108"/>
-      <c r="Q33" s="108"/>
-      <c r="R33" s="108"/>
-      <c r="S33" s="108"/>
-      <c r="T33" s="108"/>
-      <c r="U33" s="108"/>
-      <c r="V33" s="111"/>
+      <c r="L33" s="105"/>
+      <c r="M33" s="109"/>
+      <c r="N33" s="106"/>
+      <c r="O33" s="106"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="107"/>
+      <c r="S33" s="107"/>
+      <c r="T33" s="107"/>
+      <c r="U33" s="107"/>
+      <c r="V33" s="110"/>
       <c r="W33" s="74"/>
       <c r="X33" s="23"/>
       <c r="AA33" s="17"/>
@@ -2837,14 +2726,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K108"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:K27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2874,9 +2763,9 @@
       <c r="H1" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="101">
-        <f>COUNTIF(H1:H792,"OK")</f>
-        <v>2</v>
+      <c r="I1" s="100">
+        <f>COUNTIF(H1:H785,"OK")</f>
+        <v>3</v>
       </c>
       <c r="J1" s="82" t="s">
         <v>23</v>
@@ -2884,7 +2773,7 @@
       <c r="K1" s="83"/>
     </row>
     <row r="2" spans="1:11" s="58" customFormat="1">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="115" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="85" t="s">
@@ -2892,14 +2781,14 @@
       </c>
       <c r="C2" s="85"/>
       <c r="D2" s="85"/>
-      <c r="E2" s="115"/>
+      <c r="E2" s="114"/>
       <c r="F2" s="86"/>
       <c r="G2" s="87"/>
       <c r="H2" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="102">
-        <f>COUNTIF(H2:H793,"Not OK")</f>
+      <c r="I2" s="101">
+        <f>COUNTIF(H2:H786,"Not OK")</f>
         <v>4</v>
       </c>
       <c r="J2" s="89" t="s">
@@ -2922,8 +2811,8 @@
       <c r="H3" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="103">
-        <f>COUNTIF(H2:H793,"Untested")</f>
+      <c r="I3" s="102">
+        <f>COUNTIF(H2:H786,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="89" t="s">
@@ -2942,9 +2831,9 @@
         <v>32</v>
       </c>
       <c r="H4" s="85"/>
-      <c r="I4" s="102">
-        <f>COUNTIF(H3:H794,"Result")</f>
-        <v>6</v>
+      <c r="I4" s="101">
+        <f>COUNTIF(H3:H787,"Result")</f>
+        <v>7</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="90"/>
@@ -2979,21 +2868,21 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="126" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
+      <c r="B7" s="158" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="158"/>
+      <c r="D7" s="158"/>
+      <c r="E7" s="158"/>
+      <c r="F7" s="158"/>
+      <c r="G7" s="158"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="158"/>
+      <c r="K7" s="158"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="116" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="129" t="s">
@@ -3008,11 +2897,11 @@
         <v>37</v>
       </c>
       <c r="G8" s="130"/>
-      <c r="H8" s="128" t="s">
+      <c r="H8" s="152" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="128"/>
-      <c r="J8" s="118" t="s">
+      <c r="I8" s="152"/>
+      <c r="J8" s="117" t="s">
         <v>39</v>
       </c>
       <c r="K8" s="47" t="s">
@@ -3023,120 +2912,120 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="162" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="163"/>
-      <c r="D9" s="168" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="169"/>
-      <c r="F9" s="156" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="157"/>
-      <c r="H9" s="137" t="s">
+      <c r="B9" s="143" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="144"/>
+      <c r="D9" s="137" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="138"/>
+      <c r="F9" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="132"/>
+      <c r="H9" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="138"/>
+      <c r="I9" s="154"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="134"/>
+      <c r="K9" s="126"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="158"/>
-      <c r="G10" s="159"/>
-      <c r="H10" s="117" t="s">
+      <c r="B10" s="145"/>
+      <c r="C10" s="146"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="117" t="s">
+      <c r="I10" s="116" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="117" t="s">
+      <c r="J10" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="135"/>
+      <c r="K10" s="127"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="164"/>
-      <c r="C11" s="165"/>
-      <c r="D11" s="170"/>
-      <c r="E11" s="171"/>
-      <c r="F11" s="158"/>
-      <c r="G11" s="159"/>
+        <v>61</v>
+      </c>
+      <c r="B11" s="145"/>
+      <c r="C11" s="146"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="134"/>
       <c r="H11" s="50" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="135"/>
+      <c r="K11" s="127"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A12" s="117" t="s">
+      <c r="A12" s="116" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="145"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="134"/>
+      <c r="H12" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="164"/>
-      <c r="C12" s="165"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="171"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="117" t="s">
+      <c r="I12" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="117"/>
-      <c r="K12" s="135"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="127"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>1</v>
       </c>
-      <c r="B13" s="166"/>
-      <c r="C13" s="167"/>
-      <c r="D13" s="172"/>
-      <c r="E13" s="173"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="161"/>
+      <c r="B13" s="147"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="141"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="136"/>
       <c r="H13" s="53">
         <v>43434</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="136"/>
+      <c r="K13" s="128"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="132" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="133"/>
-      <c r="D14" s="132" t="s">
+      <c r="B14" s="150" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="151"/>
+      <c r="D14" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="133"/>
-      <c r="F14" s="132" t="s">
+      <c r="E14" s="151"/>
+      <c r="F14" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="133"/>
-      <c r="H14" s="132" t="s">
+      <c r="G14" s="151"/>
+      <c r="H14" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="133"/>
-      <c r="J14" s="122" t="s">
+      <c r="I14" s="151"/>
+      <c r="J14" s="120" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="56" t="s">
@@ -3147,101 +3036,101 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="162" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="163"/>
-      <c r="D15" s="168" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="169"/>
-      <c r="F15" s="168" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="169"/>
-      <c r="H15" s="137" t="s">
+      <c r="B15" s="143" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="144"/>
+      <c r="D15" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="138"/>
+      <c r="F15" s="137" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="138"/>
+      <c r="H15" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="138"/>
+      <c r="I15" s="154"/>
       <c r="J15" s="52"/>
-      <c r="K15" s="134"/>
+      <c r="K15" s="126"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A16" s="122" t="s">
+      <c r="A16" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="164"/>
-      <c r="C16" s="165"/>
-      <c r="D16" s="170"/>
-      <c r="E16" s="171"/>
-      <c r="F16" s="170"/>
-      <c r="G16" s="171"/>
-      <c r="H16" s="122" t="s">
+      <c r="B16" s="145"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="139"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="122" t="s">
+      <c r="I16" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="122" t="s">
+      <c r="J16" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="135"/>
+      <c r="K16" s="127"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="164"/>
-      <c r="C17" s="165"/>
-      <c r="D17" s="170"/>
-      <c r="E17" s="171"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="171"/>
+        <v>62</v>
+      </c>
+      <c r="B17" s="145"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="140"/>
       <c r="H17" s="50" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48"/>
-      <c r="K17" s="135"/>
+      <c r="K17" s="127"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="145"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="164"/>
-      <c r="C18" s="165"/>
-      <c r="D18" s="170"/>
-      <c r="E18" s="171"/>
-      <c r="F18" s="170"/>
-      <c r="G18" s="171"/>
-      <c r="H18" s="122" t="s">
+      <c r="I18" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="122" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" s="122"/>
-      <c r="K18" s="135"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="127"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>2</v>
       </c>
-      <c r="B19" s="166"/>
-      <c r="C19" s="167"/>
-      <c r="D19" s="172"/>
-      <c r="E19" s="173"/>
-      <c r="F19" s="172"/>
-      <c r="G19" s="173"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="141"/>
+      <c r="G19" s="142"/>
       <c r="H19" s="50">
         <v>43434</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="135"/>
+      <c r="K19" s="127"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A20" s="121" t="s">
+      <c r="A20" s="119" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="129" t="s">
@@ -3256,11 +3145,11 @@
         <v>37</v>
       </c>
       <c r="G20" s="130"/>
-      <c r="H20" s="128" t="s">
+      <c r="H20" s="152" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="128"/>
-      <c r="J20" s="123" t="s">
+      <c r="I20" s="152"/>
+      <c r="J20" s="121" t="s">
         <v>39</v>
       </c>
       <c r="K20" s="47" t="s">
@@ -3271,563 +3160,614 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="162" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="163"/>
-      <c r="D21" s="168" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="169"/>
-      <c r="F21" s="174" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="157"/>
-      <c r="H21" s="137" t="s">
+      <c r="B21" s="143" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="144"/>
+      <c r="D21" s="137" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="138"/>
+      <c r="F21" s="149" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="132"/>
+      <c r="H21" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="138"/>
+      <c r="I21" s="154"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="134"/>
+      <c r="K21" s="126"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="164"/>
-      <c r="C22" s="165"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="121" t="s">
+      <c r="B22" s="145"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="133"/>
+      <c r="G22" s="134"/>
+      <c r="H22" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="121" t="s">
+      <c r="I22" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="121" t="s">
+      <c r="J22" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="135"/>
+      <c r="K22" s="127"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="164"/>
-      <c r="C23" s="165"/>
-      <c r="D23" s="170"/>
-      <c r="E23" s="171"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="159"/>
+        <v>63</v>
+      </c>
+      <c r="B23" s="145"/>
+      <c r="C23" s="146"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="140"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="134"/>
       <c r="H23" s="50" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="135"/>
+      <c r="K23" s="127"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="119" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="145"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="140"/>
+      <c r="F24" s="133"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="164"/>
-      <c r="C24" s="165"/>
-      <c r="D24" s="170"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="121" t="s">
+      <c r="I24" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="I24" s="121" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" s="121"/>
-      <c r="K24" s="135"/>
+      <c r="J24" s="119"/>
+      <c r="K24" s="127"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>3</v>
       </c>
-      <c r="B25" s="166"/>
-      <c r="C25" s="167"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="173"/>
-      <c r="F25" s="160"/>
-      <c r="G25" s="161"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="148"/>
+      <c r="D25" s="141"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="135"/>
+      <c r="G25" s="136"/>
       <c r="H25" s="53">
         <v>43434</v>
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="54"/>
-      <c r="K25" s="136"/>
+      <c r="K25" s="128"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="99" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="131" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="131"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="126"/>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="126"/>
+        <v>49</v>
+      </c>
+      <c r="B26" s="159" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="159"/>
+      <c r="D26" s="158"/>
+      <c r="E26" s="158"/>
+      <c r="F26" s="158"/>
+      <c r="G26" s="158"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="158"/>
+      <c r="K26" s="158"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A27" s="100" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="153" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="153"/>
-      <c r="D27" s="154"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="154"/>
-      <c r="H27" s="154"/>
-      <c r="I27" s="154"/>
-      <c r="J27" s="154"/>
-      <c r="K27" s="154"/>
+      <c r="A27" s="116" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="130"/>
+      <c r="D27" s="129" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="130"/>
+      <c r="F27" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="130"/>
+      <c r="H27" s="155" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="155"/>
+      <c r="J27" s="116" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="118" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A28" s="120" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="132" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="133"/>
-      <c r="D28" s="132" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="133"/>
-      <c r="F28" s="132" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="133"/>
-      <c r="H28" s="155" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="155"/>
-      <c r="J28" s="120" t="s">
-        <v>39</v>
-      </c>
-      <c r="K28" s="120" t="s">
-        <v>40</v>
-      </c>
+      <c r="A28" s="48">
+        <v>4</v>
+      </c>
+      <c r="B28" s="143" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="144"/>
+      <c r="D28" s="137" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="138"/>
+      <c r="F28" s="166" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="167"/>
+      <c r="H28" s="156" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="157"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="126"/>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A29" s="48">
-        <f>A15+1</f>
-        <v>3</v>
-      </c>
-      <c r="B29" s="147"/>
-      <c r="C29" s="148"/>
+      <c r="A29" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="145"/>
+      <c r="C29" s="146"/>
       <c r="D29" s="139"/>
       <c r="E29" s="140"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="140"/>
-      <c r="H29" s="137" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="138"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="134"/>
+      <c r="F29" s="168"/>
+      <c r="G29" s="169"/>
+      <c r="H29" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" s="116" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="127"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A30" s="120" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="149"/>
-      <c r="C30" s="150"/>
-      <c r="D30" s="141"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="141"/>
-      <c r="G30" s="142"/>
-      <c r="H30" s="120" t="s">
-        <v>42</v>
-      </c>
-      <c r="I30" s="120" t="s">
-        <v>43</v>
-      </c>
-      <c r="J30" s="120" t="s">
-        <v>44</v>
-      </c>
-      <c r="K30" s="135"/>
+      <c r="A30" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="145"/>
+      <c r="C30" s="146"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="140"/>
+      <c r="F30" s="168"/>
+      <c r="G30" s="169"/>
+      <c r="H30" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="50"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="127"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A31" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="149"/>
-      <c r="C31" s="150"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="141"/>
-      <c r="G31" s="142"/>
-      <c r="H31" s="50" t="s">
+      <c r="A31" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="50"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="135"/>
+      <c r="B31" s="145"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="139"/>
+      <c r="E31" s="140"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="169"/>
+      <c r="H31" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="116" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="116"/>
+      <c r="K31" s="127"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A32" s="120" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="149"/>
-      <c r="C32" s="150"/>
+      <c r="A32" s="51">
+        <v>4</v>
+      </c>
+      <c r="B32" s="147"/>
+      <c r="C32" s="148"/>
       <c r="D32" s="141"/>
       <c r="E32" s="142"/>
-      <c r="F32" s="141"/>
-      <c r="G32" s="142"/>
-      <c r="H32" s="120" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="120"/>
-      <c r="J32" s="120"/>
-      <c r="K32" s="135"/>
-    </row>
-    <row r="33" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A33" s="51">
-        <v>3</v>
-      </c>
-      <c r="B33" s="151"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="143"/>
-      <c r="E33" s="144"/>
-      <c r="F33" s="143"/>
-      <c r="G33" s="144"/>
-      <c r="H33" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I33" s="50"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="136"/>
-    </row>
-    <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A34" s="117" t="s">
+      <c r="F32" s="170"/>
+      <c r="G32" s="171"/>
+      <c r="H32" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I32" s="50"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="128"/>
+    </row>
+    <row r="33" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A33" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="129" t="s">
+      <c r="B33" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="130"/>
-      <c r="D34" s="129" t="s">
+      <c r="C33" s="130"/>
+      <c r="D33" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="130"/>
-      <c r="F34" s="129" t="s">
+      <c r="E33" s="130"/>
+      <c r="F33" s="129" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="130"/>
-      <c r="H34" s="127" t="s">
+      <c r="G33" s="130"/>
+      <c r="H33" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="127"/>
-      <c r="J34" s="117" t="s">
+      <c r="I33" s="155"/>
+      <c r="J33" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="119" t="s">
+      <c r="K33" s="118" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="34" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A34" s="48">
+        <v>5</v>
+      </c>
+      <c r="B34" s="143" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="144"/>
+      <c r="D34" s="137" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="138"/>
+      <c r="F34" s="166" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="167"/>
+      <c r="H34" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="157"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="126"/>
+    </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A35" s="48">
-        <v>4</v>
-      </c>
-      <c r="B35" s="147"/>
-      <c r="C35" s="148"/>
+      <c r="A35" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="145"/>
+      <c r="C35" s="146"/>
       <c r="D35" s="139"/>
       <c r="E35" s="140"/>
-      <c r="F35" s="139"/>
-      <c r="G35" s="140"/>
-      <c r="H35" s="145" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="146"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="134"/>
+      <c r="F35" s="168"/>
+      <c r="G35" s="169"/>
+      <c r="H35" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35" s="116" t="s">
+        <v>44</v>
+      </c>
+      <c r="K35" s="127"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A36" s="117" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="149"/>
-      <c r="C36" s="150"/>
-      <c r="D36" s="141"/>
-      <c r="E36" s="142"/>
-      <c r="F36" s="141"/>
-      <c r="G36" s="142"/>
-      <c r="H36" s="117" t="s">
-        <v>42</v>
-      </c>
-      <c r="I36" s="117" t="s">
-        <v>43</v>
-      </c>
-      <c r="J36" s="117" t="s">
-        <v>44</v>
-      </c>
-      <c r="K36" s="135"/>
+      <c r="A36" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="145"/>
+      <c r="C36" s="146"/>
+      <c r="D36" s="139"/>
+      <c r="E36" s="140"/>
+      <c r="F36" s="168"/>
+      <c r="G36" s="169"/>
+      <c r="H36" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" s="50"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="127"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A37" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="149"/>
-      <c r="C37" s="150"/>
-      <c r="D37" s="141"/>
-      <c r="E37" s="142"/>
-      <c r="F37" s="141"/>
-      <c r="G37" s="142"/>
-      <c r="H37" s="50" t="s">
+      <c r="A37" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="I37" s="50"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="135"/>
+      <c r="B37" s="145"/>
+      <c r="C37" s="146"/>
+      <c r="D37" s="139"/>
+      <c r="E37" s="140"/>
+      <c r="F37" s="168"/>
+      <c r="G37" s="169"/>
+      <c r="H37" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="116" t="s">
+        <v>47</v>
+      </c>
+      <c r="J37" s="116"/>
+      <c r="K37" s="127"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A38" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="149"/>
-      <c r="C38" s="150"/>
+      <c r="A38" s="51">
+        <v>5</v>
+      </c>
+      <c r="B38" s="147"/>
+      <c r="C38" s="148"/>
       <c r="D38" s="141"/>
       <c r="E38" s="142"/>
-      <c r="F38" s="141"/>
-      <c r="G38" s="142"/>
-      <c r="H38" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="I38" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="J38" s="117"/>
-      <c r="K38" s="135"/>
-    </row>
-    <row r="39" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A39" s="51">
-        <v>4</v>
-      </c>
-      <c r="B39" s="151"/>
-      <c r="C39" s="152"/>
-      <c r="D39" s="143"/>
-      <c r="E39" s="144"/>
-      <c r="F39" s="143"/>
-      <c r="G39" s="144"/>
-      <c r="H39" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I39" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J39" s="48"/>
-      <c r="K39" s="136"/>
-    </row>
-    <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A40" s="117" t="s">
+      <c r="F38" s="170"/>
+      <c r="G38" s="171"/>
+      <c r="H38" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I38" s="50"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="128"/>
+    </row>
+    <row r="39" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A39" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="129" t="s">
+      <c r="B39" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="130"/>
-      <c r="D40" s="129" t="s">
+      <c r="C39" s="130"/>
+      <c r="D39" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="130"/>
-      <c r="F40" s="129" t="s">
+      <c r="E39" s="130"/>
+      <c r="F39" s="129" t="s">
         <v>37</v>
       </c>
-      <c r="G40" s="130"/>
-      <c r="H40" s="127" t="s">
+      <c r="G39" s="130"/>
+      <c r="H39" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="I40" s="127"/>
-      <c r="J40" s="117" t="s">
+      <c r="I39" s="155"/>
+      <c r="J39" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="K40" s="119" t="s">
+      <c r="K39" s="123" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="40" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A40" s="48">
+        <v>5</v>
+      </c>
+      <c r="B40" s="143" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="144"/>
+      <c r="D40" s="137" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="138"/>
+      <c r="F40" s="166" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" s="167"/>
+      <c r="H40" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="157"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="126"/>
+    </row>
     <row r="41" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A41" s="48">
-        <v>5</v>
-      </c>
-      <c r="B41" s="147"/>
-      <c r="C41" s="148"/>
+      <c r="A41" s="122" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="145"/>
+      <c r="C41" s="146"/>
       <c r="D41" s="139"/>
       <c r="E41" s="140"/>
-      <c r="F41" s="139"/>
-      <c r="G41" s="140"/>
-      <c r="H41" s="145" t="s">
-        <v>10</v>
-      </c>
-      <c r="I41" s="146"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="134"/>
+      <c r="F41" s="168"/>
+      <c r="G41" s="169"/>
+      <c r="H41" s="122" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="J41" s="122" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="127"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A42" s="117" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="149"/>
-      <c r="C42" s="150"/>
-      <c r="D42" s="141"/>
-      <c r="E42" s="142"/>
-      <c r="F42" s="141"/>
-      <c r="G42" s="142"/>
-      <c r="H42" s="117" t="s">
-        <v>42</v>
-      </c>
-      <c r="I42" s="117" t="s">
-        <v>43</v>
-      </c>
-      <c r="J42" s="117" t="s">
-        <v>44</v>
-      </c>
-      <c r="K42" s="135"/>
+      <c r="A42" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="145"/>
+      <c r="C42" s="146"/>
+      <c r="D42" s="139"/>
+      <c r="E42" s="140"/>
+      <c r="F42" s="168"/>
+      <c r="G42" s="169"/>
+      <c r="H42" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I42" s="50"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="127"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A43" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="149"/>
-      <c r="C43" s="150"/>
-      <c r="D43" s="141"/>
-      <c r="E43" s="142"/>
-      <c r="F43" s="141"/>
-      <c r="G43" s="142"/>
-      <c r="H43" s="50" t="s">
+      <c r="A43" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="135"/>
+      <c r="B43" s="145"/>
+      <c r="C43" s="146"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="140"/>
+      <c r="F43" s="168"/>
+      <c r="G43" s="169"/>
+      <c r="H43" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" s="122" t="s">
+        <v>47</v>
+      </c>
+      <c r="J43" s="122"/>
+      <c r="K43" s="127"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A44" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="149"/>
-      <c r="C44" s="150"/>
+      <c r="A44" s="51">
+        <v>5</v>
+      </c>
+      <c r="B44" s="147"/>
+      <c r="C44" s="148"/>
       <c r="D44" s="141"/>
       <c r="E44" s="142"/>
-      <c r="F44" s="141"/>
-      <c r="G44" s="142"/>
-      <c r="H44" s="117" t="s">
+      <c r="F44" s="170"/>
+      <c r="G44" s="171"/>
+      <c r="H44" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I44" s="50"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="128"/>
+    </row>
+    <row r="45" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A45" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="130"/>
+      <c r="D45" s="129" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="130"/>
+      <c r="F45" s="129" t="s">
+        <v>37</v>
+      </c>
+      <c r="G45" s="130"/>
+      <c r="H45" s="155" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="155"/>
+      <c r="J45" s="122" t="s">
+        <v>39</v>
+      </c>
+      <c r="K45" s="123" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A46" s="48">
+        <v>5</v>
+      </c>
+      <c r="B46" s="143" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="144"/>
+      <c r="D46" s="137" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="138"/>
+      <c r="F46" s="160" t="s">
+        <v>78</v>
+      </c>
+      <c r="G46" s="161"/>
+      <c r="H46" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="157"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="126"/>
+    </row>
+    <row r="47" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A47" s="122" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="145"/>
+      <c r="C47" s="146"/>
+      <c r="D47" s="139"/>
+      <c r="E47" s="140"/>
+      <c r="F47" s="162"/>
+      <c r="G47" s="163"/>
+      <c r="H47" s="122" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="122" t="s">
+        <v>44</v>
+      </c>
+      <c r="K47" s="127"/>
+    </row>
+    <row r="48" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A48" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="145"/>
+      <c r="C48" s="146"/>
+      <c r="D48" s="139"/>
+      <c r="E48" s="140"/>
+      <c r="F48" s="162"/>
+      <c r="G48" s="163"/>
+      <c r="H48" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I48" s="50"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="127"/>
+    </row>
+    <row r="49" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A49" s="122" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="145"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="139"/>
+      <c r="E49" s="140"/>
+      <c r="F49" s="162"/>
+      <c r="G49" s="163"/>
+      <c r="H49" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="I49" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="I44" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="J44" s="117"/>
-      <c r="K44" s="135"/>
-    </row>
-    <row r="45" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A45" s="51">
+      <c r="J49" s="122"/>
+      <c r="K49" s="127"/>
+    </row>
+    <row r="50" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A50" s="51">
         <v>5</v>
       </c>
-      <c r="B45" s="151"/>
-      <c r="C45" s="152"/>
-      <c r="D45" s="143"/>
-      <c r="E45" s="144"/>
-      <c r="F45" s="143"/>
-      <c r="G45" s="144"/>
-      <c r="H45" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I45" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J45" s="48"/>
-      <c r="K45" s="136"/>
-    </row>
-    <row r="46" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A46" s="62"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="62"/>
-      <c r="I46" s="62"/>
-      <c r="J46" s="62"/>
-      <c r="K46" s="62"/>
-    </row>
-    <row r="47" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A47" s="62"/>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="62"/>
-      <c r="I47" s="62"/>
-      <c r="J47" s="62"/>
-      <c r="K47" s="62"/>
-    </row>
-    <row r="48" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A48" s="62"/>
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="62"/>
-      <c r="I48" s="62"/>
-      <c r="J48" s="62"/>
-      <c r="K48" s="62"/>
-    </row>
-    <row r="49" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A49" s="62"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="62"/>
-      <c r="K49" s="62"/>
-    </row>
-    <row r="50" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A50" s="62"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
-    </row>
-    <row r="51" spans="1:11" ht="10.5" customHeight="1">
+      <c r="B50" s="147"/>
+      <c r="C50" s="148"/>
+      <c r="D50" s="141"/>
+      <c r="E50" s="142"/>
+      <c r="F50" s="164"/>
+      <c r="G50" s="165"/>
+      <c r="H50" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I50" s="50"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="128"/>
+    </row>
+    <row r="51" spans="1:11" s="58" customFormat="1">
       <c r="A51" s="62"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
       <c r="H51" s="62"/>
       <c r="I51" s="62"/>
       <c r="J51" s="62"/>
@@ -4142,53 +4082,95 @@
       <c r="K95" s="62"/>
     </row>
     <row r="96" spans="1:11" s="58" customFormat="1">
-      <c r="A96" s="62"/>
-      <c r="H96" s="62"/>
-      <c r="I96" s="62"/>
-      <c r="J96" s="62"/>
-      <c r="K96" s="62"/>
+      <c r="A96" s="2"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
     </row>
     <row r="97" spans="1:11" s="58" customFormat="1">
-      <c r="A97" s="62"/>
-      <c r="H97" s="62"/>
-      <c r="I97" s="62"/>
-      <c r="J97" s="62"/>
-      <c r="K97" s="62"/>
+      <c r="A97" s="2"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
     </row>
     <row r="98" spans="1:11" s="58" customFormat="1">
-      <c r="A98" s="62"/>
-      <c r="H98" s="62"/>
-      <c r="I98" s="62"/>
-      <c r="J98" s="62"/>
-      <c r="K98" s="62"/>
+      <c r="A98" s="2"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
     </row>
     <row r="99" spans="1:11" s="58" customFormat="1">
-      <c r="A99" s="62"/>
-      <c r="H99" s="62"/>
-      <c r="I99" s="62"/>
-      <c r="J99" s="62"/>
-      <c r="K99" s="62"/>
+      <c r="A99" s="2"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
     </row>
     <row r="100" spans="1:11" s="58" customFormat="1">
-      <c r="A100" s="62"/>
-      <c r="H100" s="62"/>
-      <c r="I100" s="62"/>
-      <c r="J100" s="62"/>
-      <c r="K100" s="62"/>
+      <c r="A100" s="2"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
     </row>
     <row r="101" spans="1:11" s="58" customFormat="1">
-      <c r="A101" s="62"/>
-      <c r="H101" s="62"/>
-      <c r="I101" s="62"/>
-      <c r="J101" s="62"/>
-      <c r="K101" s="62"/>
+      <c r="A101" s="2"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
     </row>
     <row r="102" spans="1:11" s="58" customFormat="1">
-      <c r="A102" s="62"/>
-      <c r="H102" s="62"/>
-      <c r="I102" s="62"/>
-      <c r="J102" s="62"/>
-      <c r="K102" s="62"/>
+      <c r="A102" s="2"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
     </row>
     <row r="103" spans="1:11" s="58" customFormat="1">
       <c r="A103" s="2"/>
@@ -4255,96 +4237,113 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="1:11" s="58" customFormat="1">
-      <c r="A108" s="2"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B35:C39"/>
+  <mergeCells count="65">
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:E50"/>
+    <mergeCell ref="F46:G50"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="K46:K50"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B40:C44"/>
+    <mergeCell ref="D40:E44"/>
+    <mergeCell ref="F40:G44"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="F28:G32"/>
+    <mergeCell ref="K28:K32"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:C38"/>
+    <mergeCell ref="D28:E32"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="F34:G38"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
     <mergeCell ref="F9:G13"/>
     <mergeCell ref="F15:G19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B28:C32"/>
     <mergeCell ref="B21:C25"/>
     <mergeCell ref="D21:E25"/>
     <mergeCell ref="F21:G25"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="D41:E45"/>
-    <mergeCell ref="F41:G45"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="K41:K45"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="H41:I41">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="H34:I34">
+    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:I33">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:I40">
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39:I39">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46:I46">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:I45">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="75" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LTest Case Table&amp;CBig Point: &amp;A</oddHeader>
     <oddFooter>&amp;LAI&amp;&amp;T-ART&amp;CLiveSpark Project&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="63" max="10" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add binhluanmonan test case
</commit_message>
<xml_diff>
--- a/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$95</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$89</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="95">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -284,6 +284,54 @@
     <t xml:space="preserve">Hệ thống cho phép bình luận
 Bình luận được lưu lại và hiển thị ngay sau khi submit
 </t>
+  </si>
+  <si>
+    <t>Bình luận món ăn</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>BinhLuanMonAn_01</t>
+  </si>
+  <si>
+    <t>BinhLuanMonAn_02</t>
+  </si>
+  <si>
+    <t>BinhLuanMonAn_03</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>3-3</t>
+  </si>
+  <si>
+    <t>Kiểm tra load form bình luận món ăn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiển thị đúng form bình luận </t>
+  </si>
+  <si>
+    <t>Kiểm tra khi người dùng bỏ trống form bình luận</t>
+  </si>
+  <si>
+    <t>Hệ thống thông báo lỗi,người dùng chưa nhập bình luận,yêu cầu người dùng nhạp bình luận</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi người dùng nhập đúng định dạng bình luận</t>
+  </si>
+  <si>
+    <t>Hệ thống thông báo bình luận thành công,bình luận được cập nhật lên hệ thống</t>
   </si>
 </sst>
 </file>
@@ -782,7 +830,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1071,6 +1119,12 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1078,6 +1132,66 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1093,6 +1207,48 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1111,117 +1267,57 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1325,7 +1421,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1792,13 +1888,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="124" t="s">
+      <c r="O6" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="124"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
+      <c r="P6" s="126"/>
+      <c r="Q6" s="126"/>
+      <c r="R6" s="126"/>
+      <c r="S6" s="126"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1808,11 +1904,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="124"/>
-      <c r="P7" s="124"/>
-      <c r="Q7" s="124"/>
-      <c r="R7" s="124"/>
-      <c r="S7" s="124"/>
+      <c r="O7" s="126"/>
+      <c r="P7" s="126"/>
+      <c r="Q7" s="126"/>
+      <c r="R7" s="126"/>
+      <c r="S7" s="126"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -1867,12 +1963,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="125">
+      <c r="E11" s="127">
         <f ca="1">TODAY()</f>
         <v>43430</v>
       </c>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="127"/>
       <c r="H11" s="72"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -2730,10 +2826,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K107"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2764,8 +2860,8 @@
         <v>22</v>
       </c>
       <c r="I1" s="100">
-        <f>COUNTIF(H1:H785,"OK")</f>
-        <v>3</v>
+        <f>COUNTIF(H1:H779,"OK")</f>
+        <v>4</v>
       </c>
       <c r="J1" s="82" t="s">
         <v>23</v>
@@ -2788,8 +2884,8 @@
         <v>26</v>
       </c>
       <c r="I2" s="101">
-        <f>COUNTIF(H2:H786,"Not OK")</f>
-        <v>4</v>
+        <f>COUNTIF(H2:H780,"Not OK")</f>
+        <v>6</v>
       </c>
       <c r="J2" s="89" t="s">
         <v>27</v>
@@ -2812,7 +2908,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="102">
-        <f>COUNTIF(H2:H786,"Untested")</f>
+        <f>COUNTIF(H2:H780,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="89" t="s">
@@ -2832,8 +2928,8 @@
       </c>
       <c r="H4" s="85"/>
       <c r="I4" s="101">
-        <f>COUNTIF(H3:H787,"Result")</f>
-        <v>7</v>
+        <f>COUNTIF(H3:H781,"Result")</f>
+        <v>10</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="90"/>
@@ -2868,39 +2964,39 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="158"/>
-      <c r="K7" s="158"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="160"/>
+      <c r="F7" s="160"/>
+      <c r="G7" s="160"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
+      <c r="K7" s="160"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="130"/>
-      <c r="D8" s="129" t="s">
+      <c r="C8" s="152"/>
+      <c r="D8" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="129" t="s">
+      <c r="E8" s="152"/>
+      <c r="F8" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="130"/>
-      <c r="H8" s="152" t="s">
+      <c r="G8" s="152"/>
+      <c r="H8" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="152"/>
+      <c r="I8" s="161"/>
       <c r="J8" s="117" t="s">
         <v>39</v>
       </c>
@@ -2912,35 +3008,35 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="143" t="s">
+      <c r="B9" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="144"/>
-      <c r="D9" s="137" t="s">
+      <c r="C9" s="129"/>
+      <c r="D9" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="138"/>
-      <c r="F9" s="131" t="s">
+      <c r="E9" s="135"/>
+      <c r="F9" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="132"/>
-      <c r="H9" s="153" t="s">
+      <c r="G9" s="168"/>
+      <c r="H9" s="165" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="154"/>
+      <c r="I9" s="166"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="126"/>
+      <c r="K9" s="148"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="145"/>
-      <c r="C10" s="146"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="134"/>
+      <c r="B10" s="130"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="169"/>
+      <c r="G10" s="170"/>
       <c r="H10" s="116" t="s">
         <v>42</v>
       </c>
@@ -2950,35 +3046,35 @@
       <c r="J10" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="127"/>
+      <c r="K10" s="149"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="145"/>
-      <c r="C11" s="146"/>
-      <c r="D11" s="139"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="134"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="169"/>
+      <c r="G11" s="170"/>
       <c r="H11" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="127"/>
+      <c r="K11" s="149"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="146"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="133"/>
-      <c r="G12" s="134"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="169"/>
+      <c r="G12" s="170"/>
       <c r="H12" s="116" t="s">
         <v>46</v>
       </c>
@@ -2986,45 +3082,45 @@
         <v>47</v>
       </c>
       <c r="J12" s="116"/>
-      <c r="K12" s="127"/>
+      <c r="K12" s="149"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>1</v>
       </c>
-      <c r="B13" s="147"/>
-      <c r="C13" s="148"/>
-      <c r="D13" s="141"/>
-      <c r="E13" s="142"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="136"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="171"/>
+      <c r="G13" s="172"/>
       <c r="H13" s="53">
         <v>43434</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="128"/>
+      <c r="K13" s="150"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="163" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="151"/>
-      <c r="D14" s="150" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="151"/>
-      <c r="F14" s="150" t="s">
+      <c r="E14" s="164"/>
+      <c r="F14" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="151"/>
-      <c r="H14" s="150" t="s">
+      <c r="G14" s="164"/>
+      <c r="H14" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="151"/>
+      <c r="I14" s="164"/>
       <c r="J14" s="120" t="s">
         <v>39</v>
       </c>
@@ -3036,35 +3132,35 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="143" t="s">
+      <c r="B15" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="144"/>
-      <c r="D15" s="137" t="s">
+      <c r="C15" s="129"/>
+      <c r="D15" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="138"/>
-      <c r="F15" s="137" t="s">
+      <c r="E15" s="135"/>
+      <c r="F15" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="138"/>
-      <c r="H15" s="153" t="s">
+      <c r="G15" s="135"/>
+      <c r="H15" s="165" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="154"/>
+      <c r="I15" s="166"/>
       <c r="J15" s="52"/>
-      <c r="K15" s="126"/>
+      <c r="K15" s="148"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="146"/>
-      <c r="D16" s="139"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="139"/>
-      <c r="G16" s="140"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="137"/>
       <c r="H16" s="120" t="s">
         <v>42</v>
       </c>
@@ -3074,35 +3170,35 @@
       <c r="J16" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="127"/>
+      <c r="K16" s="149"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="145"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="139"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="139"/>
-      <c r="G17" s="140"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="137"/>
       <c r="H17" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48"/>
-      <c r="K17" s="127"/>
+      <c r="K17" s="149"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="145"/>
-      <c r="C18" s="146"/>
-      <c r="D18" s="139"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="139"/>
-      <c r="G18" s="140"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="131"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="137"/>
       <c r="H18" s="120" t="s">
         <v>46</v>
       </c>
@@ -3110,45 +3206,45 @@
         <v>47</v>
       </c>
       <c r="J18" s="120"/>
-      <c r="K18" s="127"/>
+      <c r="K18" s="149"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>2</v>
       </c>
-      <c r="B19" s="147"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="141"/>
-      <c r="G19" s="142"/>
+      <c r="B19" s="132"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="139"/>
       <c r="H19" s="50">
         <v>43434</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="127"/>
+      <c r="K19" s="149"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="119" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="129" t="s">
+      <c r="B20" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="130"/>
-      <c r="D20" s="129" t="s">
+      <c r="C20" s="152"/>
+      <c r="D20" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="130"/>
-      <c r="F20" s="129" t="s">
+      <c r="E20" s="152"/>
+      <c r="F20" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="130"/>
-      <c r="H20" s="152" t="s">
+      <c r="G20" s="152"/>
+      <c r="H20" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="152"/>
+      <c r="I20" s="161"/>
       <c r="J20" s="121" t="s">
         <v>39</v>
       </c>
@@ -3160,35 +3256,35 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="143" t="s">
+      <c r="B21" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="144"/>
-      <c r="D21" s="137" t="s">
+      <c r="C21" s="129"/>
+      <c r="D21" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="138"/>
-      <c r="F21" s="149" t="s">
+      <c r="E21" s="135"/>
+      <c r="F21" s="173" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="132"/>
-      <c r="H21" s="153" t="s">
+      <c r="G21" s="168"/>
+      <c r="H21" s="165" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="154"/>
+      <c r="I21" s="166"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="126"/>
+      <c r="K21" s="148"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="145"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="139"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="134"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="131"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="170"/>
       <c r="H22" s="119" t="s">
         <v>42</v>
       </c>
@@ -3198,35 +3294,35 @@
       <c r="J22" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="127"/>
+      <c r="K22" s="149"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="145"/>
-      <c r="C23" s="146"/>
-      <c r="D23" s="139"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="133"/>
-      <c r="G23" s="134"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="131"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="170"/>
       <c r="H23" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="127"/>
+      <c r="K23" s="149"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="145"/>
-      <c r="C24" s="146"/>
-      <c r="D24" s="139"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="134"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="169"/>
+      <c r="G24" s="170"/>
       <c r="H24" s="119" t="s">
         <v>46</v>
       </c>
@@ -3234,62 +3330,62 @@
         <v>47</v>
       </c>
       <c r="J24" s="119"/>
-      <c r="K24" s="127"/>
+      <c r="K24" s="149"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>3</v>
       </c>
-      <c r="B25" s="147"/>
-      <c r="C25" s="148"/>
-      <c r="D25" s="141"/>
-      <c r="E25" s="142"/>
-      <c r="F25" s="135"/>
-      <c r="G25" s="136"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="171"/>
+      <c r="G25" s="172"/>
       <c r="H25" s="53">
         <v>43434</v>
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="54"/>
-      <c r="K25" s="128"/>
+      <c r="K25" s="150"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="159" t="s">
+      <c r="B26" s="162" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="159"/>
-      <c r="D26" s="158"/>
-      <c r="E26" s="158"/>
-      <c r="F26" s="158"/>
-      <c r="G26" s="158"/>
-      <c r="H26" s="158"/>
-      <c r="I26" s="158"/>
-      <c r="J26" s="158"/>
-      <c r="K26" s="158"/>
+      <c r="C26" s="162"/>
+      <c r="D26" s="160"/>
+      <c r="E26" s="160"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="160"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="160"/>
+      <c r="J26" s="160"/>
+      <c r="K26" s="160"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="129" t="s">
+      <c r="B27" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="130"/>
-      <c r="D27" s="129" t="s">
+      <c r="C27" s="152"/>
+      <c r="D27" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="130"/>
-      <c r="F27" s="129" t="s">
+      <c r="E27" s="152"/>
+      <c r="F27" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="130"/>
-      <c r="H27" s="155" t="s">
+      <c r="G27" s="152"/>
+      <c r="H27" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="155"/>
+      <c r="I27" s="153"/>
       <c r="J27" s="116" t="s">
         <v>39</v>
       </c>
@@ -3301,35 +3397,35 @@
       <c r="A28" s="48">
         <v>4</v>
       </c>
-      <c r="B28" s="143" t="s">
+      <c r="B28" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="144"/>
-      <c r="D28" s="137" t="s">
+      <c r="C28" s="129"/>
+      <c r="D28" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="138"/>
-      <c r="F28" s="166" t="s">
+      <c r="E28" s="135"/>
+      <c r="F28" s="154" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="167"/>
-      <c r="H28" s="156" t="s">
+      <c r="G28" s="155"/>
+      <c r="H28" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="157"/>
+      <c r="I28" s="147"/>
       <c r="J28" s="52"/>
-      <c r="K28" s="126"/>
+      <c r="K28" s="148"/>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="145"/>
-      <c r="C29" s="146"/>
-      <c r="D29" s="139"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="168"/>
-      <c r="G29" s="169"/>
+      <c r="B29" s="130"/>
+      <c r="C29" s="131"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="137"/>
+      <c r="F29" s="156"/>
+      <c r="G29" s="157"/>
       <c r="H29" s="116" t="s">
         <v>42</v>
       </c>
@@ -3339,35 +3435,35 @@
       <c r="J29" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="127"/>
+      <c r="K29" s="149"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="146"/>
-      <c r="D30" s="139"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="168"/>
-      <c r="G30" s="169"/>
+      <c r="B30" s="130"/>
+      <c r="C30" s="131"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="157"/>
       <c r="H30" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I30" s="50"/>
       <c r="J30" s="48"/>
-      <c r="K30" s="127"/>
+      <c r="K30" s="149"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="145"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="139"/>
-      <c r="E31" s="140"/>
-      <c r="F31" s="168"/>
-      <c r="G31" s="169"/>
+      <c r="B31" s="130"/>
+      <c r="C31" s="131"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="157"/>
       <c r="H31" s="116" t="s">
         <v>46</v>
       </c>
@@ -3375,45 +3471,45 @@
         <v>47</v>
       </c>
       <c r="J31" s="116"/>
-      <c r="K31" s="127"/>
+      <c r="K31" s="149"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="51">
         <v>4</v>
       </c>
-      <c r="B32" s="147"/>
-      <c r="C32" s="148"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="142"/>
-      <c r="F32" s="170"/>
-      <c r="G32" s="171"/>
+      <c r="B32" s="132"/>
+      <c r="C32" s="133"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="158"/>
+      <c r="G32" s="159"/>
       <c r="H32" s="50">
         <v>43434</v>
       </c>
       <c r="I32" s="50"/>
       <c r="J32" s="48"/>
-      <c r="K32" s="128"/>
+      <c r="K32" s="150"/>
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A33" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="129" t="s">
+      <c r="B33" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="130"/>
-      <c r="D33" s="129" t="s">
+      <c r="C33" s="152"/>
+      <c r="D33" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="130"/>
-      <c r="F33" s="129" t="s">
+      <c r="E33" s="152"/>
+      <c r="F33" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="130"/>
-      <c r="H33" s="155" t="s">
+      <c r="G33" s="152"/>
+      <c r="H33" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="155"/>
+      <c r="I33" s="153"/>
       <c r="J33" s="116" t="s">
         <v>39</v>
       </c>
@@ -3425,35 +3521,35 @@
       <c r="A34" s="48">
         <v>5</v>
       </c>
-      <c r="B34" s="143" t="s">
+      <c r="B34" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="144"/>
-      <c r="D34" s="137" t="s">
+      <c r="C34" s="129"/>
+      <c r="D34" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="166" t="s">
+      <c r="E34" s="135"/>
+      <c r="F34" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="167"/>
-      <c r="H34" s="156" t="s">
+      <c r="G34" s="155"/>
+      <c r="H34" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="I34" s="157"/>
+      <c r="I34" s="147"/>
       <c r="J34" s="52"/>
-      <c r="K34" s="126"/>
+      <c r="K34" s="148"/>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="145"/>
-      <c r="C35" s="146"/>
-      <c r="D35" s="139"/>
-      <c r="E35" s="140"/>
-      <c r="F35" s="168"/>
-      <c r="G35" s="169"/>
+      <c r="B35" s="130"/>
+      <c r="C35" s="131"/>
+      <c r="D35" s="136"/>
+      <c r="E35" s="137"/>
+      <c r="F35" s="156"/>
+      <c r="G35" s="157"/>
       <c r="H35" s="116" t="s">
         <v>42</v>
       </c>
@@ -3463,35 +3559,35 @@
       <c r="J35" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="127"/>
+      <c r="K35" s="149"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="145"/>
-      <c r="C36" s="146"/>
-      <c r="D36" s="139"/>
-      <c r="E36" s="140"/>
-      <c r="F36" s="168"/>
-      <c r="G36" s="169"/>
+      <c r="B36" s="130"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="157"/>
       <c r="H36" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I36" s="50"/>
       <c r="J36" s="48"/>
-      <c r="K36" s="127"/>
+      <c r="K36" s="149"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="145"/>
-      <c r="C37" s="146"/>
-      <c r="D37" s="139"/>
-      <c r="E37" s="140"/>
-      <c r="F37" s="168"/>
-      <c r="G37" s="169"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="131"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="137"/>
+      <c r="F37" s="156"/>
+      <c r="G37" s="157"/>
       <c r="H37" s="116" t="s">
         <v>46</v>
       </c>
@@ -3499,45 +3595,45 @@
         <v>47</v>
       </c>
       <c r="J37" s="116"/>
-      <c r="K37" s="127"/>
+      <c r="K37" s="149"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="51">
         <v>5</v>
       </c>
-      <c r="B38" s="147"/>
-      <c r="C38" s="148"/>
-      <c r="D38" s="141"/>
-      <c r="E38" s="142"/>
-      <c r="F38" s="170"/>
-      <c r="G38" s="171"/>
+      <c r="B38" s="132"/>
+      <c r="C38" s="133"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="139"/>
+      <c r="F38" s="158"/>
+      <c r="G38" s="159"/>
       <c r="H38" s="50">
         <v>43434</v>
       </c>
       <c r="I38" s="50"/>
       <c r="J38" s="48"/>
-      <c r="K38" s="128"/>
+      <c r="K38" s="150"/>
     </row>
     <row r="39" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A39" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="129" t="s">
+      <c r="B39" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="130"/>
-      <c r="D39" s="129" t="s">
+      <c r="C39" s="152"/>
+      <c r="D39" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="130"/>
-      <c r="F39" s="129" t="s">
+      <c r="E39" s="152"/>
+      <c r="F39" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="130"/>
-      <c r="H39" s="155" t="s">
+      <c r="G39" s="152"/>
+      <c r="H39" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="155"/>
+      <c r="I39" s="153"/>
       <c r="J39" s="122" t="s">
         <v>39</v>
       </c>
@@ -3547,37 +3643,37 @@
     </row>
     <row r="40" spans="1:11" ht="10.5" customHeight="1">
       <c r="A40" s="48">
-        <v>5</v>
-      </c>
-      <c r="B40" s="143" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="144"/>
-      <c r="D40" s="137" t="s">
+      <c r="C40" s="129"/>
+      <c r="D40" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="138"/>
-      <c r="F40" s="166" t="s">
+      <c r="E40" s="135"/>
+      <c r="F40" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="167"/>
-      <c r="H40" s="156" t="s">
+      <c r="G40" s="155"/>
+      <c r="H40" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="157"/>
+      <c r="I40" s="147"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="126"/>
+      <c r="K40" s="148"/>
     </row>
     <row r="41" spans="1:11" ht="10.5" customHeight="1">
       <c r="A41" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="145"/>
-      <c r="C41" s="146"/>
-      <c r="D41" s="139"/>
-      <c r="E41" s="140"/>
-      <c r="F41" s="168"/>
-      <c r="G41" s="169"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="137"/>
+      <c r="F41" s="156"/>
+      <c r="G41" s="157"/>
       <c r="H41" s="122" t="s">
         <v>42</v>
       </c>
@@ -3587,35 +3683,35 @@
       <c r="J41" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="127"/>
+      <c r="K41" s="149"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="145"/>
-      <c r="C42" s="146"/>
-      <c r="D42" s="139"/>
-      <c r="E42" s="140"/>
-      <c r="F42" s="168"/>
-      <c r="G42" s="169"/>
+        <v>85</v>
+      </c>
+      <c r="B42" s="130"/>
+      <c r="C42" s="131"/>
+      <c r="D42" s="136"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="156"/>
+      <c r="G42" s="157"/>
       <c r="H42" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I42" s="50"/>
       <c r="J42" s="48"/>
-      <c r="K42" s="127"/>
+      <c r="K42" s="149"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="145"/>
-      <c r="C43" s="146"/>
-      <c r="D43" s="139"/>
-      <c r="E43" s="140"/>
-      <c r="F43" s="168"/>
-      <c r="G43" s="169"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="131"/>
+      <c r="D43" s="136"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="156"/>
+      <c r="G43" s="157"/>
       <c r="H43" s="122" t="s">
         <v>46</v>
       </c>
@@ -3623,45 +3719,45 @@
         <v>47</v>
       </c>
       <c r="J43" s="122"/>
-      <c r="K43" s="127"/>
+      <c r="K43" s="149"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="51">
-        <v>5</v>
-      </c>
-      <c r="B44" s="147"/>
-      <c r="C44" s="148"/>
-      <c r="D44" s="141"/>
-      <c r="E44" s="142"/>
-      <c r="F44" s="170"/>
-      <c r="G44" s="171"/>
+        <v>6</v>
+      </c>
+      <c r="B44" s="132"/>
+      <c r="C44" s="133"/>
+      <c r="D44" s="138"/>
+      <c r="E44" s="139"/>
+      <c r="F44" s="158"/>
+      <c r="G44" s="159"/>
       <c r="H44" s="50">
         <v>43434</v>
       </c>
       <c r="I44" s="50"/>
       <c r="J44" s="48"/>
-      <c r="K44" s="128"/>
+      <c r="K44" s="150"/>
     </row>
     <row r="45" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A45" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="129" t="s">
+      <c r="B45" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="130"/>
-      <c r="D45" s="129" t="s">
+      <c r="C45" s="152"/>
+      <c r="D45" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="130"/>
-      <c r="F45" s="129" t="s">
+      <c r="E45" s="152"/>
+      <c r="F45" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="130"/>
-      <c r="H45" s="155" t="s">
+      <c r="G45" s="152"/>
+      <c r="H45" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="155"/>
+      <c r="I45" s="153"/>
       <c r="J45" s="122" t="s">
         <v>39</v>
       </c>
@@ -3671,37 +3767,37 @@
     </row>
     <row r="46" spans="1:11" ht="10.5" customHeight="1">
       <c r="A46" s="48">
-        <v>5</v>
-      </c>
-      <c r="B46" s="143" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="144"/>
-      <c r="D46" s="137" t="s">
+      <c r="C46" s="129"/>
+      <c r="D46" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="138"/>
-      <c r="F46" s="160" t="s">
+      <c r="E46" s="135"/>
+      <c r="F46" s="140" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="161"/>
-      <c r="H46" s="156" t="s">
+      <c r="G46" s="141"/>
+      <c r="H46" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="I46" s="157"/>
+      <c r="I46" s="147"/>
       <c r="J46" s="52"/>
-      <c r="K46" s="126"/>
+      <c r="K46" s="148"/>
     </row>
     <row r="47" spans="1:11" ht="10.5" customHeight="1">
       <c r="A47" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="145"/>
-      <c r="C47" s="146"/>
-      <c r="D47" s="139"/>
-      <c r="E47" s="140"/>
-      <c r="F47" s="162"/>
-      <c r="G47" s="163"/>
+      <c r="B47" s="130"/>
+      <c r="C47" s="131"/>
+      <c r="D47" s="136"/>
+      <c r="E47" s="137"/>
+      <c r="F47" s="142"/>
+      <c r="G47" s="143"/>
       <c r="H47" s="122" t="s">
         <v>42</v>
       </c>
@@ -3711,35 +3807,35 @@
       <c r="J47" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="K47" s="127"/>
+      <c r="K47" s="149"/>
     </row>
     <row r="48" spans="1:11" ht="10.5" customHeight="1">
       <c r="A48" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" s="145"/>
-      <c r="C48" s="146"/>
-      <c r="D48" s="139"/>
-      <c r="E48" s="140"/>
-      <c r="F48" s="162"/>
-      <c r="G48" s="163"/>
+        <v>86</v>
+      </c>
+      <c r="B48" s="130"/>
+      <c r="C48" s="131"/>
+      <c r="D48" s="136"/>
+      <c r="E48" s="137"/>
+      <c r="F48" s="142"/>
+      <c r="G48" s="143"/>
       <c r="H48" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I48" s="50"/>
       <c r="J48" s="48"/>
-      <c r="K48" s="127"/>
+      <c r="K48" s="149"/>
     </row>
     <row r="49" spans="1:11" ht="10.5" customHeight="1">
       <c r="A49" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="145"/>
-      <c r="C49" s="146"/>
-      <c r="D49" s="139"/>
-      <c r="E49" s="140"/>
-      <c r="F49" s="162"/>
-      <c r="G49" s="163"/>
+      <c r="B49" s="130"/>
+      <c r="C49" s="131"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="137"/>
+      <c r="F49" s="142"/>
+      <c r="G49" s="143"/>
       <c r="H49" s="122" t="s">
         <v>46</v>
       </c>
@@ -3747,157 +3843,413 @@
         <v>47</v>
       </c>
       <c r="J49" s="122"/>
-      <c r="K49" s="127"/>
+      <c r="K49" s="149"/>
     </row>
     <row r="50" spans="1:11" ht="10.5" customHeight="1">
       <c r="A50" s="51">
-        <v>5</v>
-      </c>
-      <c r="B50" s="147"/>
-      <c r="C50" s="148"/>
-      <c r="D50" s="141"/>
-      <c r="E50" s="142"/>
-      <c r="F50" s="164"/>
-      <c r="G50" s="165"/>
+        <v>7</v>
+      </c>
+      <c r="B50" s="132"/>
+      <c r="C50" s="133"/>
+      <c r="D50" s="138"/>
+      <c r="E50" s="139"/>
+      <c r="F50" s="144"/>
+      <c r="G50" s="145"/>
       <c r="H50" s="50">
         <v>43434</v>
       </c>
       <c r="I50" s="50"/>
       <c r="J50" s="48"/>
-      <c r="K50" s="128"/>
+      <c r="K50" s="150"/>
     </row>
     <row r="51" spans="1:11" s="58" customFormat="1">
-      <c r="A51" s="62"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="62"/>
-      <c r="K51" s="62"/>
+      <c r="A51" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="162" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="162"/>
+      <c r="D51" s="160"/>
+      <c r="E51" s="160"/>
+      <c r="F51" s="160"/>
+      <c r="G51" s="160"/>
+      <c r="H51" s="160"/>
+      <c r="I51" s="160"/>
+      <c r="J51" s="160"/>
+      <c r="K51" s="160"/>
     </row>
     <row r="52" spans="1:11" s="58" customFormat="1">
-      <c r="A52" s="62"/>
-      <c r="H52" s="62"/>
-      <c r="I52" s="62"/>
-      <c r="J52" s="62"/>
-      <c r="K52" s="62"/>
+      <c r="A52" s="125" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="151" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="152"/>
+      <c r="D52" s="151" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="152"/>
+      <c r="F52" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" s="152"/>
+      <c r="H52" s="153" t="s">
+        <v>38</v>
+      </c>
+      <c r="I52" s="153"/>
+      <c r="J52" s="125" t="s">
+        <v>39</v>
+      </c>
+      <c r="K52" s="124" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="53" spans="1:11" s="58" customFormat="1">
-      <c r="A53" s="62"/>
-      <c r="H53" s="62"/>
-      <c r="I53" s="62"/>
-      <c r="J53" s="62"/>
-      <c r="K53" s="62"/>
+      <c r="A53" s="48">
+        <v>8</v>
+      </c>
+      <c r="B53" s="128" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="129"/>
+      <c r="D53" s="134" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="135"/>
+      <c r="F53" s="154" t="s">
+        <v>90</v>
+      </c>
+      <c r="G53" s="155"/>
+      <c r="H53" s="146" t="s">
+        <v>9</v>
+      </c>
+      <c r="I53" s="147"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="148"/>
     </row>
     <row r="54" spans="1:11" s="58" customFormat="1">
-      <c r="A54" s="62"/>
-      <c r="H54" s="62"/>
-      <c r="I54" s="62"/>
-      <c r="J54" s="62"/>
-      <c r="K54" s="62"/>
+      <c r="A54" s="125" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="130"/>
+      <c r="C54" s="131"/>
+      <c r="D54" s="136"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="156"/>
+      <c r="G54" s="157"/>
+      <c r="H54" s="125" t="s">
+        <v>42</v>
+      </c>
+      <c r="I54" s="125" t="s">
+        <v>43</v>
+      </c>
+      <c r="J54" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="K54" s="149"/>
     </row>
     <row r="55" spans="1:11" s="58" customFormat="1">
-      <c r="A55" s="62"/>
-      <c r="H55" s="62"/>
-      <c r="I55" s="62"/>
-      <c r="J55" s="62"/>
-      <c r="K55" s="62"/>
+      <c r="A55" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="130"/>
+      <c r="C55" s="131"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="156"/>
+      <c r="G55" s="157"/>
+      <c r="H55" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55" s="50"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="149"/>
     </row>
     <row r="56" spans="1:11" s="58" customFormat="1">
-      <c r="A56" s="62"/>
-      <c r="H56" s="62"/>
-      <c r="I56" s="62"/>
-      <c r="J56" s="62"/>
-      <c r="K56" s="62"/>
+      <c r="A56" s="125" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="130"/>
+      <c r="C56" s="131"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="156"/>
+      <c r="G56" s="157"/>
+      <c r="H56" s="125" t="s">
+        <v>46</v>
+      </c>
+      <c r="I56" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="J56" s="125"/>
+      <c r="K56" s="149"/>
     </row>
     <row r="57" spans="1:11" s="58" customFormat="1">
-      <c r="A57" s="62"/>
-      <c r="H57" s="62"/>
-      <c r="I57" s="62"/>
-      <c r="J57" s="62"/>
-      <c r="K57" s="62"/>
+      <c r="A57" s="51">
+        <v>8</v>
+      </c>
+      <c r="B57" s="132"/>
+      <c r="C57" s="133"/>
+      <c r="D57" s="138"/>
+      <c r="E57" s="139"/>
+      <c r="F57" s="158"/>
+      <c r="G57" s="159"/>
+      <c r="H57" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I57" s="50"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="150"/>
     </row>
     <row r="58" spans="1:11" s="58" customFormat="1">
-      <c r="A58" s="62"/>
-      <c r="H58" s="62"/>
-      <c r="I58" s="62"/>
-      <c r="J58" s="62"/>
-      <c r="K58" s="62"/>
+      <c r="A58" s="125" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" s="151" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="152"/>
+      <c r="D58" s="151" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="152"/>
+      <c r="F58" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="G58" s="152"/>
+      <c r="H58" s="153" t="s">
+        <v>38</v>
+      </c>
+      <c r="I58" s="153"/>
+      <c r="J58" s="125" t="s">
+        <v>39</v>
+      </c>
+      <c r="K58" s="124" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="59" spans="1:11" s="58" customFormat="1">
-      <c r="A59" s="62"/>
-      <c r="H59" s="62"/>
-      <c r="I59" s="62"/>
-      <c r="J59" s="62"/>
-      <c r="K59" s="62"/>
+      <c r="A59" s="48">
+        <v>9</v>
+      </c>
+      <c r="B59" s="128" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="129"/>
+      <c r="D59" s="134" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" s="135"/>
+      <c r="F59" s="154" t="s">
+        <v>92</v>
+      </c>
+      <c r="G59" s="155"/>
+      <c r="H59" s="146" t="s">
+        <v>10</v>
+      </c>
+      <c r="I59" s="147"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="148"/>
     </row>
     <row r="60" spans="1:11" s="58" customFormat="1">
-      <c r="A60" s="62"/>
-      <c r="H60" s="62"/>
-      <c r="I60" s="62"/>
-      <c r="J60" s="62"/>
-      <c r="K60" s="62"/>
+      <c r="A60" s="125" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="130"/>
+      <c r="C60" s="131"/>
+      <c r="D60" s="136"/>
+      <c r="E60" s="137"/>
+      <c r="F60" s="156"/>
+      <c r="G60" s="157"/>
+      <c r="H60" s="125" t="s">
+        <v>42</v>
+      </c>
+      <c r="I60" s="125" t="s">
+        <v>43</v>
+      </c>
+      <c r="J60" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="K60" s="149"/>
     </row>
     <row r="61" spans="1:11" s="58" customFormat="1">
-      <c r="A61" s="62"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="62"/>
-      <c r="J61" s="62"/>
-      <c r="K61" s="62"/>
+      <c r="A61" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" s="130"/>
+      <c r="C61" s="131"/>
+      <c r="D61" s="136"/>
+      <c r="E61" s="137"/>
+      <c r="F61" s="156"/>
+      <c r="G61" s="157"/>
+      <c r="H61" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I61" s="50"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="149"/>
     </row>
     <row r="62" spans="1:11" s="58" customFormat="1">
-      <c r="A62" s="62"/>
-      <c r="H62" s="62"/>
-      <c r="I62" s="62"/>
-      <c r="J62" s="62"/>
-      <c r="K62" s="62"/>
+      <c r="A62" s="125" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="130"/>
+      <c r="C62" s="131"/>
+      <c r="D62" s="136"/>
+      <c r="E62" s="137"/>
+      <c r="F62" s="156"/>
+      <c r="G62" s="157"/>
+      <c r="H62" s="125" t="s">
+        <v>46</v>
+      </c>
+      <c r="I62" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="J62" s="125"/>
+      <c r="K62" s="149"/>
     </row>
     <row r="63" spans="1:11" s="58" customFormat="1">
-      <c r="A63" s="62"/>
-      <c r="H63" s="62"/>
-      <c r="I63" s="62"/>
-      <c r="J63" s="62"/>
-      <c r="K63" s="62"/>
+      <c r="A63" s="51">
+        <v>9</v>
+      </c>
+      <c r="B63" s="132"/>
+      <c r="C63" s="133"/>
+      <c r="D63" s="138"/>
+      <c r="E63" s="139"/>
+      <c r="F63" s="158"/>
+      <c r="G63" s="159"/>
+      <c r="H63" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I63" s="50"/>
+      <c r="J63" s="48"/>
+      <c r="K63" s="150"/>
     </row>
     <row r="64" spans="1:11" s="58" customFormat="1">
-      <c r="A64" s="62"/>
-      <c r="H64" s="62"/>
-      <c r="I64" s="62"/>
-      <c r="J64" s="62"/>
-      <c r="K64" s="62"/>
+      <c r="A64" s="125" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="151" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="152"/>
+      <c r="D64" s="151" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="152"/>
+      <c r="F64" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="G64" s="152"/>
+      <c r="H64" s="153" t="s">
+        <v>38</v>
+      </c>
+      <c r="I64" s="153"/>
+      <c r="J64" s="125" t="s">
+        <v>39</v>
+      </c>
+      <c r="K64" s="124" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="65" spans="1:11" s="58" customFormat="1">
-      <c r="A65" s="62"/>
-      <c r="H65" s="62"/>
-      <c r="I65" s="62"/>
-      <c r="J65" s="62"/>
-      <c r="K65" s="62"/>
+      <c r="A65" s="48">
+        <v>10</v>
+      </c>
+      <c r="B65" s="128" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="129"/>
+      <c r="D65" s="134" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="135"/>
+      <c r="F65" s="154" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" s="155"/>
+      <c r="H65" s="146" t="s">
+        <v>10</v>
+      </c>
+      <c r="I65" s="147"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="148"/>
     </row>
     <row r="66" spans="1:11" s="58" customFormat="1">
-      <c r="A66" s="62"/>
-      <c r="H66" s="62"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="62"/>
-      <c r="K66" s="62"/>
+      <c r="A66" s="125" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="130"/>
+      <c r="C66" s="131"/>
+      <c r="D66" s="136"/>
+      <c r="E66" s="137"/>
+      <c r="F66" s="156"/>
+      <c r="G66" s="157"/>
+      <c r="H66" s="125" t="s">
+        <v>42</v>
+      </c>
+      <c r="I66" s="125" t="s">
+        <v>43</v>
+      </c>
+      <c r="J66" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="K66" s="149"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
-      <c r="A67" s="62"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="62"/>
-      <c r="K67" s="62"/>
+      <c r="A67" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="130"/>
+      <c r="C67" s="131"/>
+      <c r="D67" s="136"/>
+      <c r="E67" s="137"/>
+      <c r="F67" s="156"/>
+      <c r="G67" s="157"/>
+      <c r="H67" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I67" s="50"/>
+      <c r="J67" s="48"/>
+      <c r="K67" s="149"/>
     </row>
     <row r="68" spans="1:11" s="58" customFormat="1">
-      <c r="A68" s="62"/>
-      <c r="H68" s="62"/>
-      <c r="I68" s="62"/>
-      <c r="J68" s="62"/>
-      <c r="K68" s="62"/>
+      <c r="A68" s="125" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="130"/>
+      <c r="C68" s="131"/>
+      <c r="D68" s="136"/>
+      <c r="E68" s="137"/>
+      <c r="F68" s="156"/>
+      <c r="G68" s="157"/>
+      <c r="H68" s="125" t="s">
+        <v>46</v>
+      </c>
+      <c r="I68" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="J68" s="125"/>
+      <c r="K68" s="149"/>
     </row>
     <row r="69" spans="1:11" s="58" customFormat="1">
-      <c r="A69" s="62"/>
-      <c r="H69" s="62"/>
-      <c r="I69" s="62"/>
-      <c r="J69" s="62"/>
-      <c r="K69" s="62"/>
+      <c r="A69" s="51">
+        <v>10</v>
+      </c>
+      <c r="B69" s="132"/>
+      <c r="C69" s="133"/>
+      <c r="D69" s="138"/>
+      <c r="E69" s="139"/>
+      <c r="F69" s="158"/>
+      <c r="G69" s="159"/>
+      <c r="H69" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I69" s="50"/>
+      <c r="J69" s="48"/>
+      <c r="K69" s="150"/>
     </row>
     <row r="70" spans="1:11" s="58" customFormat="1">
       <c r="A70" s="62"/>
@@ -4040,46 +4392,82 @@
       <c r="K89" s="62"/>
     </row>
     <row r="90" spans="1:11" s="58" customFormat="1">
-      <c r="A90" s="62"/>
-      <c r="H90" s="62"/>
-      <c r="I90" s="62"/>
-      <c r="J90" s="62"/>
-      <c r="K90" s="62"/>
+      <c r="A90" s="2"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
     </row>
     <row r="91" spans="1:11" s="58" customFormat="1">
-      <c r="A91" s="62"/>
-      <c r="H91" s="62"/>
-      <c r="I91" s="62"/>
-      <c r="J91" s="62"/>
-      <c r="K91" s="62"/>
+      <c r="A91" s="2"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
     </row>
     <row r="92" spans="1:11" s="58" customFormat="1">
-      <c r="A92" s="62"/>
-      <c r="H92" s="62"/>
-      <c r="I92" s="62"/>
-      <c r="J92" s="62"/>
-      <c r="K92" s="62"/>
+      <c r="A92" s="2"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
     </row>
     <row r="93" spans="1:11" s="58" customFormat="1">
-      <c r="A93" s="62"/>
-      <c r="H93" s="62"/>
-      <c r="I93" s="62"/>
-      <c r="J93" s="62"/>
-      <c r="K93" s="62"/>
+      <c r="A93" s="2"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
     </row>
     <row r="94" spans="1:11" s="58" customFormat="1">
-      <c r="A94" s="62"/>
-      <c r="H94" s="62"/>
-      <c r="I94" s="62"/>
-      <c r="J94" s="62"/>
-      <c r="K94" s="62"/>
+      <c r="A94" s="2"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
     </row>
     <row r="95" spans="1:11" s="58" customFormat="1">
-      <c r="A95" s="62"/>
-      <c r="H95" s="62"/>
-      <c r="I95" s="62"/>
-      <c r="J95" s="62"/>
-      <c r="K95" s="62"/>
+      <c r="A95" s="2"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
     </row>
     <row r="96" spans="1:11" s="58" customFormat="1">
       <c r="A96" s="2"/>
@@ -4159,120 +4547,46 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" s="58" customFormat="1">
-      <c r="A102" s="2"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-    </row>
-    <row r="103" spans="1:11" s="58" customFormat="1">
-      <c r="A103" s="2"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-    </row>
-    <row r="104" spans="1:11" s="58" customFormat="1">
-      <c r="A104" s="2"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-    </row>
-    <row r="105" spans="1:11" s="58" customFormat="1">
-      <c r="A105" s="2"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-    </row>
-    <row r="106" spans="1:11" s="58" customFormat="1">
-      <c r="A106" s="2"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-    </row>
-    <row r="107" spans="1:11" s="58" customFormat="1">
-      <c r="A107" s="2"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="B46:C50"/>
-    <mergeCell ref="D46:E50"/>
-    <mergeCell ref="F46:G50"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="K46:K50"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B40:C44"/>
-    <mergeCell ref="D40:E44"/>
-    <mergeCell ref="F40:G44"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="K34:K38"/>
-    <mergeCell ref="F28:G32"/>
-    <mergeCell ref="K28:K32"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H34:I34"/>
+  <mergeCells count="93">
+    <mergeCell ref="B65:C69"/>
+    <mergeCell ref="D65:E69"/>
+    <mergeCell ref="F65:G69"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="K65:K69"/>
+    <mergeCell ref="K59:K63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B59:C63"/>
+    <mergeCell ref="D59:E63"/>
+    <mergeCell ref="F59:G63"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="B53:C57"/>
+    <mergeCell ref="D53:E57"/>
+    <mergeCell ref="F53:G57"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:K57"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="F21:G25"/>
     <mergeCell ref="B34:C38"/>
     <mergeCell ref="D28:E32"/>
     <mergeCell ref="D34:E38"/>
@@ -4285,54 +4599,98 @@
     <mergeCell ref="B15:C19"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C13"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="H20:I20"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="F28:G32"/>
+    <mergeCell ref="K28:K32"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="F9:G13"/>
     <mergeCell ref="F15:G19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="B28:C32"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:E25"/>
-    <mergeCell ref="F21:G25"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B40:C44"/>
+    <mergeCell ref="D40:E44"/>
+    <mergeCell ref="F40:G44"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:E50"/>
+    <mergeCell ref="F46:G50"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="K46:K50"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H34:I34">
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:I33">
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:I40">
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:I39">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46:I46">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:I45">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59:I59">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H58:I58">
+    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65:I65">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64:I64">
+    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Register test case continue
</commit_message>
<xml_diff>
--- a/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="113">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -349,7 +349,43 @@
     <t>Nhập thông tin không đầy đủ</t>
   </si>
   <si>
-    <t>thông báo thông tin điền không đầy đủ ,yêu cầu điền đầy đủ thông tin yêu cầu vào các mục</t>
+    <t>4-2</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>DangKy_02</t>
+  </si>
+  <si>
+    <t>DangKy_03</t>
+  </si>
+  <si>
+    <t>DangKy_04</t>
+  </si>
+  <si>
+    <t>Tài khoản bị trùng</t>
+  </si>
+  <si>
+    <t>Thông báo tài khoản bị trùng, đã được đăng ký, yêu cầu nhập tên tài khoản khác</t>
+  </si>
+  <si>
+    <t>Thông báo thông tin điền không đầy đủ ,yêu cầu điền đầy đủ thông tin yêu cầu vào các mục</t>
+  </si>
+  <si>
+    <t>Mật khẩu không hợp lệ</t>
+  </si>
+  <si>
+    <t>Thông báo mật khẩu không hợp lệ, yêu cầu điền đúng mật khẩu theo yêu cầu (ký tự hoa, có số,….)</t>
+  </si>
+  <si>
+    <t>Hiển thị đúng thứ tự các form</t>
+  </si>
+  <si>
+    <t>Hiển thị đúng thứ tự các trường trong form, có thể chuyển đến các trường gần nhau bằng các nhấn "tab".</t>
   </si>
 </sst>
 </file>
@@ -848,7 +884,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -969,9 +1005,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1149,6 +1182,12 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1225,6 +1264,12 @@
     <xf numFmtId="49" fontId="18" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1234,14 +1279,41 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1258,76 +1330,30 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -1431,7 +1457,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1811,7 +1837,7 @@
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
-      <c r="V2" s="69"/>
+      <c r="V2" s="68"/>
       <c r="W2" s="13"/>
       <c r="X2" s="14"/>
     </row>
@@ -1831,7 +1857,7 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
-      <c r="N3" s="68"/>
+      <c r="N3" s="67"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
@@ -1839,7 +1865,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
-      <c r="V3" s="70"/>
+      <c r="V3" s="69"/>
       <c r="W3" s="18"/>
       <c r="X3" s="19"/>
     </row>
@@ -1898,13 +1924,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="128" t="s">
+      <c r="O6" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="128"/>
-      <c r="Q6" s="128"/>
-      <c r="R6" s="128"/>
-      <c r="S6" s="128"/>
+      <c r="P6" s="129"/>
+      <c r="Q6" s="129"/>
+      <c r="R6" s="129"/>
+      <c r="S6" s="129"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1914,11 +1940,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="128"/>
-      <c r="P7" s="128"/>
-      <c r="Q7" s="128"/>
-      <c r="R7" s="128"/>
-      <c r="S7" s="128"/>
+      <c r="O7" s="129"/>
+      <c r="P7" s="129"/>
+      <c r="Q7" s="129"/>
+      <c r="R7" s="129"/>
+      <c r="S7" s="129"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -1927,7 +1953,7 @@
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="31"/>
-      <c r="X8" s="67"/>
+      <c r="X8" s="66"/>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1">
       <c r="B9" s="30"/>
@@ -1940,7 +1966,7 @@
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="72"/>
+      <c r="H9" s="71"/>
       <c r="X9" s="19"/>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1">
@@ -1952,11 +1978,11 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="72"/>
+      <c r="H10" s="71"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
-      <c r="L10" s="113" t="s">
+      <c r="L10" s="112" t="s">
         <v>5</v>
       </c>
       <c r="O10" s="21"/>
@@ -1973,13 +1999,13 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="129">
+      <c r="E11" s="130">
         <f ca="1">TODAY()</f>
         <v>43430</v>
       </c>
-      <c r="F11" s="129"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="72"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="71"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
       </c>
@@ -2010,23 +2036,23 @@
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="63">
+      <c r="O12" s="62">
         <v>2</v>
       </c>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="64">
+      <c r="P12" s="62"/>
+      <c r="Q12" s="63">
         <v>3</v>
       </c>
-      <c r="R12" s="64"/>
-      <c r="S12" s="65">
+      <c r="R12" s="63"/>
+      <c r="S12" s="64">
         <v>4</v>
       </c>
-      <c r="T12" s="65"/>
-      <c r="U12" s="66">
+      <c r="T12" s="64"/>
+      <c r="U12" s="65">
         <f t="shared" ref="U12:U18" si="0">SUM(O12:T12)</f>
         <v>9</v>
       </c>
-      <c r="V12" s="66"/>
+      <c r="V12" s="65"/>
       <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:24">
@@ -2036,23 +2062,23 @@
       </c>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
-      <c r="O13" s="63">
+      <c r="O13" s="62">
         <v>22</v>
       </c>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="64">
+      <c r="P13" s="62"/>
+      <c r="Q13" s="63">
         <v>22</v>
       </c>
-      <c r="R13" s="64"/>
-      <c r="S13" s="65">
+      <c r="R13" s="63"/>
+      <c r="S13" s="64">
         <v>22</v>
       </c>
-      <c r="T13" s="65"/>
-      <c r="U13" s="66">
+      <c r="T13" s="64"/>
+      <c r="U13" s="65">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="V13" s="66"/>
+      <c r="V13" s="65"/>
       <c r="X13" s="19"/>
     </row>
     <row r="14" spans="1:24">
@@ -2062,23 +2088,23 @@
       </c>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="63">
+      <c r="O14" s="62">
         <v>32</v>
       </c>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="64">
+      <c r="P14" s="62"/>
+      <c r="Q14" s="63">
         <v>32</v>
       </c>
-      <c r="R14" s="64"/>
-      <c r="S14" s="65">
+      <c r="R14" s="63"/>
+      <c r="S14" s="64">
         <v>32</v>
       </c>
-      <c r="T14" s="65"/>
-      <c r="U14" s="66">
+      <c r="T14" s="64"/>
+      <c r="U14" s="65">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="V14" s="66"/>
+      <c r="V14" s="65"/>
       <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24">
@@ -2086,32 +2112,32 @@
       <c r="D15" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
       <c r="L15" s="34">
         <v>4</v>
       </c>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
-      <c r="O15" s="63">
+      <c r="O15" s="62">
         <v>42</v>
       </c>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="64">
+      <c r="P15" s="62"/>
+      <c r="Q15" s="63">
         <v>42</v>
       </c>
-      <c r="R15" s="64"/>
-      <c r="S15" s="65">
+      <c r="R15" s="63"/>
+      <c r="S15" s="64">
         <v>42</v>
       </c>
-      <c r="T15" s="65"/>
-      <c r="U15" s="66">
+      <c r="T15" s="64"/>
+      <c r="U15" s="65">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="V15" s="66"/>
+      <c r="V15" s="65"/>
       <c r="X15" s="19"/>
     </row>
     <row r="16" spans="1:24">
@@ -2126,23 +2152,23 @@
       </c>
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
-      <c r="O16" s="63">
+      <c r="O16" s="62">
         <v>52</v>
       </c>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="64">
+      <c r="P16" s="62"/>
+      <c r="Q16" s="63">
         <v>52</v>
       </c>
-      <c r="R16" s="64"/>
-      <c r="S16" s="65">
+      <c r="R16" s="63"/>
+      <c r="S16" s="64">
         <v>52</v>
       </c>
-      <c r="T16" s="65"/>
-      <c r="U16" s="66">
+      <c r="T16" s="64"/>
+      <c r="U16" s="65">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="V16" s="66"/>
+      <c r="V16" s="65"/>
       <c r="X16" s="19"/>
     </row>
     <row r="17" spans="2:35">
@@ -2157,23 +2183,23 @@
       </c>
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
-      <c r="O17" s="63">
+      <c r="O17" s="62">
         <v>62</v>
       </c>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="64">
+      <c r="P17" s="62"/>
+      <c r="Q17" s="63">
         <v>62</v>
       </c>
-      <c r="R17" s="64"/>
-      <c r="S17" s="65">
+      <c r="R17" s="63"/>
+      <c r="S17" s="64">
         <v>62</v>
       </c>
-      <c r="T17" s="65"/>
-      <c r="U17" s="66">
+      <c r="T17" s="64"/>
+      <c r="U17" s="65">
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="V17" s="66"/>
+      <c r="V17" s="65"/>
       <c r="X17" s="19"/>
     </row>
     <row r="18" spans="2:35">
@@ -2188,23 +2214,23 @@
       </c>
       <c r="M18" s="35"/>
       <c r="N18" s="35"/>
-      <c r="O18" s="63">
+      <c r="O18" s="62">
         <v>72</v>
       </c>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="64">
+      <c r="P18" s="62"/>
+      <c r="Q18" s="63">
         <v>72</v>
       </c>
-      <c r="R18" s="64"/>
-      <c r="S18" s="65">
+      <c r="R18" s="63"/>
+      <c r="S18" s="64">
         <v>72</v>
       </c>
-      <c r="T18" s="65"/>
-      <c r="U18" s="66">
+      <c r="T18" s="64"/>
+      <c r="U18" s="65">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="V18" s="66"/>
+      <c r="V18" s="65"/>
       <c r="X18" s="19"/>
     </row>
     <row r="19" spans="2:35">
@@ -2219,27 +2245,27 @@
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
-      <c r="O19" s="111">
+      <c r="O19" s="110">
         <f>SUM(O12:O18)</f>
         <v>284</v>
       </c>
-      <c r="P19" s="111"/>
-      <c r="Q19" s="111">
+      <c r="P19" s="110"/>
+      <c r="Q19" s="110">
         <f>SUM(Q12:Q18)</f>
         <v>285</v>
       </c>
-      <c r="R19" s="111"/>
-      <c r="S19" s="111">
+      <c r="R19" s="110"/>
+      <c r="S19" s="110">
         <f>SUM(S12:S18)</f>
         <v>286</v>
       </c>
-      <c r="T19" s="111"/>
-      <c r="U19" s="112">
+      <c r="T19" s="110"/>
+      <c r="U19" s="111">
         <f>SUM(U12:U18)</f>
         <v>855</v>
       </c>
-      <c r="V19" s="112"/>
-      <c r="W19" s="74"/>
+      <c r="V19" s="111"/>
+      <c r="W19" s="73"/>
       <c r="X19" s="19"/>
     </row>
     <row r="20" spans="2:35">
@@ -2269,10 +2295,10 @@
       <c r="D22" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
       <c r="W22" s="17"/>
       <c r="X22" s="23"/>
     </row>
@@ -2283,7 +2309,7 @@
       <c r="F23" s="44"/>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
-      <c r="W23" s="75"/>
+      <c r="W23" s="74"/>
       <c r="X23" s="23"/>
     </row>
     <row r="24" spans="2:35" s="17" customFormat="1">
@@ -2293,20 +2319,20 @@
       <c r="F24" s="44"/>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
-      <c r="L24" s="113" t="s">
+      <c r="L24" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="103"/>
-      <c r="N24" s="103"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="104"/>
-      <c r="Q24" s="104"/>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
-      <c r="T24" s="104"/>
-      <c r="U24" s="104"/>
-      <c r="V24" s="104"/>
-      <c r="W24" s="73"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="102"/>
+      <c r="P24" s="103"/>
+      <c r="Q24" s="103"/>
+      <c r="R24" s="103"/>
+      <c r="S24" s="103"/>
+      <c r="T24" s="103"/>
+      <c r="U24" s="103"/>
+      <c r="V24" s="103"/>
+      <c r="W24" s="72"/>
       <c r="X24" s="23"/>
     </row>
     <row r="25" spans="2:35" s="17" customFormat="1">
@@ -2315,18 +2341,18 @@
       <c r="F25" s="44"/>
       <c r="G25" s="44"/>
       <c r="H25" s="44"/>
-      <c r="L25" s="105"/>
-      <c r="M25" s="106"/>
-      <c r="N25" s="106"/>
-      <c r="O25" s="106"/>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
-      <c r="T25" s="107"/>
-      <c r="U25" s="107"/>
-      <c r="V25" s="107"/>
-      <c r="W25" s="73"/>
+      <c r="L25" s="104"/>
+      <c r="M25" s="105"/>
+      <c r="N25" s="105"/>
+      <c r="O25" s="105"/>
+      <c r="P25" s="106"/>
+      <c r="Q25" s="106"/>
+      <c r="R25" s="106"/>
+      <c r="S25" s="106"/>
+      <c r="T25" s="106"/>
+      <c r="U25" s="106"/>
+      <c r="V25" s="106"/>
+      <c r="W25" s="72"/>
       <c r="X25" s="23"/>
     </row>
     <row r="26" spans="2:35" s="17" customFormat="1">
@@ -2335,58 +2361,58 @@
       <c r="F26" s="44"/>
       <c r="G26" s="44"/>
       <c r="H26" s="44"/>
-      <c r="L26" s="105"/>
-      <c r="M26" s="106"/>
-      <c r="N26" s="106"/>
-      <c r="O26" s="106"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
-      <c r="U26" s="107"/>
-      <c r="V26" s="107"/>
-      <c r="W26" s="73"/>
+      <c r="L26" s="104"/>
+      <c r="M26" s="105"/>
+      <c r="N26" s="105"/>
+      <c r="O26" s="105"/>
+      <c r="P26" s="106"/>
+      <c r="Q26" s="106"/>
+      <c r="R26" s="106"/>
+      <c r="S26" s="106"/>
+      <c r="T26" s="106"/>
+      <c r="U26" s="106"/>
+      <c r="V26" s="106"/>
+      <c r="W26" s="72"/>
       <c r="X26" s="23"/>
-      <c r="AB26" s="76"/>
+      <c r="AB26" s="75"/>
     </row>
     <row r="27" spans="2:35" s="17" customFormat="1">
       <c r="B27" s="22"/>
       <c r="D27" s="38"/>
       <c r="E27" s="4"/>
-      <c r="L27" s="105"/>
-      <c r="M27" s="106"/>
-      <c r="N27" s="106"/>
-      <c r="O27" s="106"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="107"/>
-      <c r="U27" s="107"/>
-      <c r="V27" s="107"/>
-      <c r="W27" s="73"/>
+      <c r="L27" s="104"/>
+      <c r="M27" s="105"/>
+      <c r="N27" s="105"/>
+      <c r="O27" s="105"/>
+      <c r="P27" s="106"/>
+      <c r="Q27" s="106"/>
+      <c r="R27" s="106"/>
+      <c r="S27" s="106"/>
+      <c r="T27" s="106"/>
+      <c r="U27" s="106"/>
+      <c r="V27" s="106"/>
+      <c r="W27" s="72"/>
       <c r="X27" s="23"/>
-      <c r="AB27" s="76"/>
+      <c r="AB27" s="75"/>
     </row>
     <row r="28" spans="2:35" s="17" customFormat="1">
       <c r="B28" s="22"/>
       <c r="D28" s="38"/>
       <c r="E28" s="4"/>
-      <c r="L28" s="105"/>
-      <c r="M28" s="106"/>
-      <c r="N28" s="106"/>
-      <c r="O28" s="106"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
-      <c r="T28" s="107"/>
-      <c r="U28" s="107"/>
-      <c r="V28" s="107"/>
-      <c r="W28" s="73"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="105"/>
+      <c r="N28" s="105"/>
+      <c r="O28" s="105"/>
+      <c r="P28" s="106"/>
+      <c r="Q28" s="106"/>
+      <c r="R28" s="106"/>
+      <c r="S28" s="106"/>
+      <c r="T28" s="106"/>
+      <c r="U28" s="106"/>
+      <c r="V28" s="106"/>
+      <c r="W28" s="72"/>
       <c r="X28" s="23"/>
-      <c r="AB28" s="76"/>
+      <c r="AB28" s="75"/>
     </row>
     <row r="29" spans="2:35" s="17" customFormat="1">
       <c r="B29" s="22"/>
@@ -2396,34 +2422,34 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="K29" s="31"/>
-      <c r="L29" s="105"/>
-      <c r="M29" s="106"/>
-      <c r="N29" s="106"/>
-      <c r="O29" s="106"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
-      <c r="T29" s="107"/>
-      <c r="U29" s="107"/>
-      <c r="V29" s="107"/>
-      <c r="W29" s="73"/>
+      <c r="L29" s="104"/>
+      <c r="M29" s="105"/>
+      <c r="N29" s="105"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="106"/>
+      <c r="Q29" s="106"/>
+      <c r="R29" s="106"/>
+      <c r="S29" s="106"/>
+      <c r="T29" s="106"/>
+      <c r="U29" s="106"/>
+      <c r="V29" s="106"/>
+      <c r="W29" s="72"/>
       <c r="X29" s="23"/>
     </row>
     <row r="30" spans="2:35" s="17" customFormat="1">
       <c r="B30" s="22"/>
-      <c r="L30" s="105"/>
-      <c r="M30" s="106"/>
-      <c r="N30" s="106"/>
-      <c r="O30" s="106"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
-      <c r="T30" s="107"/>
-      <c r="U30" s="107"/>
-      <c r="V30" s="107"/>
-      <c r="W30" s="73"/>
+      <c r="L30" s="104"/>
+      <c r="M30" s="105"/>
+      <c r="N30" s="105"/>
+      <c r="O30" s="105"/>
+      <c r="P30" s="106"/>
+      <c r="Q30" s="106"/>
+      <c r="R30" s="106"/>
+      <c r="S30" s="106"/>
+      <c r="T30" s="106"/>
+      <c r="U30" s="106"/>
+      <c r="V30" s="106"/>
+      <c r="W30" s="72"/>
       <c r="X30" s="23"/>
     </row>
     <row r="31" spans="2:35">
@@ -2439,18 +2465,18 @@
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
-      <c r="L31" s="108"/>
-      <c r="M31" s="106"/>
-      <c r="N31" s="106"/>
-      <c r="O31" s="106"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
-      <c r="T31" s="107"/>
-      <c r="U31" s="107"/>
-      <c r="V31" s="107"/>
-      <c r="W31" s="73"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="105"/>
+      <c r="N31" s="105"/>
+      <c r="O31" s="105"/>
+      <c r="P31" s="106"/>
+      <c r="Q31" s="106"/>
+      <c r="R31" s="106"/>
+      <c r="S31" s="106"/>
+      <c r="T31" s="106"/>
+      <c r="U31" s="106"/>
+      <c r="V31" s="106"/>
+      <c r="W31" s="72"/>
       <c r="X31" s="23"/>
       <c r="AA31" s="17"/>
       <c r="AB31" s="17"/>
@@ -2475,18 +2501,18 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
-      <c r="L32" s="105"/>
-      <c r="M32" s="106"/>
-      <c r="N32" s="106"/>
-      <c r="O32" s="106"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="107"/>
-      <c r="T32" s="107"/>
-      <c r="U32" s="107"/>
-      <c r="V32" s="107"/>
-      <c r="W32" s="73"/>
+      <c r="L32" s="104"/>
+      <c r="M32" s="105"/>
+      <c r="N32" s="105"/>
+      <c r="O32" s="105"/>
+      <c r="P32" s="106"/>
+      <c r="Q32" s="106"/>
+      <c r="R32" s="106"/>
+      <c r="S32" s="106"/>
+      <c r="T32" s="106"/>
+      <c r="U32" s="106"/>
+      <c r="V32" s="106"/>
+      <c r="W32" s="72"/>
       <c r="X32" s="23"/>
       <c r="AA32" s="17"/>
       <c r="AB32" s="17"/>
@@ -2509,18 +2535,18 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="105"/>
-      <c r="M33" s="109"/>
-      <c r="N33" s="106"/>
-      <c r="O33" s="106"/>
-      <c r="P33" s="107"/>
-      <c r="Q33" s="107"/>
-      <c r="R33" s="107"/>
-      <c r="S33" s="107"/>
-      <c r="T33" s="107"/>
-      <c r="U33" s="107"/>
-      <c r="V33" s="110"/>
-      <c r="W33" s="74"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="105"/>
+      <c r="O33" s="105"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="106"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="106"/>
+      <c r="T33" s="106"/>
+      <c r="U33" s="106"/>
+      <c r="V33" s="109"/>
+      <c r="W33" s="73"/>
       <c r="X33" s="23"/>
       <c r="AA33" s="17"/>
       <c r="AB33" s="17"/>
@@ -2559,7 +2585,7 @@
       <c r="W34" s="45"/>
       <c r="X34" s="23"/>
       <c r="AA34" s="17"/>
-      <c r="AB34" s="76"/>
+      <c r="AB34" s="75"/>
       <c r="AC34" s="17"/>
       <c r="AD34" s="17"/>
       <c r="AE34" s="17"/>
@@ -2838,8 +2864,8 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A58" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72:G76"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A79" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2852,110 +2878,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="58" customFormat="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="78" t="str">
+      <c r="B1" s="77" t="str">
         <f>Overview!E9</f>
         <v>Hear and Note</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="80" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="100">
+      <c r="I1" s="99">
         <f>COUNTIF(H1:H767,"OK")</f>
-        <v>5</v>
-      </c>
-      <c r="J1" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="83"/>
+      <c r="K1" s="82"/>
     </row>
     <row r="2" spans="1:11" s="58" customFormat="1">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="88" t="s">
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="101">
+      <c r="I2" s="100">
         <f>COUNTIF(H2:H768,"Not OK")</f>
-        <v>6</v>
-      </c>
-      <c r="J2" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="90"/>
+      <c r="K2" s="89"/>
     </row>
     <row r="3" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="88" t="s">
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="102">
+      <c r="I3" s="101">
         <f>COUNTIF(H2:H768,"Untested")</f>
         <v>0</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="90"/>
+      <c r="K3" s="89"/>
     </row>
     <row r="4" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A4" s="91"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="92" t="s">
+      <c r="A4" s="90"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="85"/>
-      <c r="I4" s="101">
+      <c r="H4" s="84"/>
+      <c r="I4" s="100">
         <f>COUNTIF(H3:H769,"Result")</f>
-        <v>11</v>
-      </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="90"/>
+        <v>14</v>
+      </c>
+      <c r="J4" s="88"/>
+      <c r="K4" s="89"/>
     </row>
     <row r="5" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A5" s="93"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="98"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="97"/>
     </row>
     <row r="6" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
       <c r="A6" s="59"/>
@@ -2971,43 +2997,43 @@
       <c r="K6" s="57"/>
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="155" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="157"/>
-      <c r="E7" s="157"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="157"/>
-      <c r="K7" s="157"/>
+      <c r="C7" s="155"/>
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="155"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="155"/>
+      <c r="J7" s="155"/>
+      <c r="K7" s="155"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="153" t="s">
+      <c r="B8" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="154"/>
-      <c r="D8" s="153" t="s">
+      <c r="C8" s="157"/>
+      <c r="D8" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="154"/>
-      <c r="F8" s="153" t="s">
+      <c r="E8" s="157"/>
+      <c r="F8" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="154"/>
-      <c r="H8" s="168" t="s">
+      <c r="G8" s="157"/>
+      <c r="H8" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="168"/>
-      <c r="J8" s="117" t="s">
+      <c r="I8" s="165"/>
+      <c r="J8" s="116" t="s">
         <v>39</v>
       </c>
       <c r="K8" s="47" t="s">
@@ -3018,98 +3044,98 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="130" t="s">
+      <c r="B9" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="131"/>
-      <c r="D9" s="136" t="s">
+      <c r="C9" s="132"/>
+      <c r="D9" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="169" t="s">
+      <c r="E9" s="138"/>
+      <c r="F9" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="159"/>
-      <c r="H9" s="164" t="s">
+      <c r="G9" s="171"/>
+      <c r="H9" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="165"/>
+      <c r="I9" s="169"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="150"/>
+      <c r="K9" s="151"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="132"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="160"/>
-      <c r="G10" s="161"/>
-      <c r="H10" s="116" t="s">
+      <c r="B10" s="133"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="116" t="s">
+      <c r="I10" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="116" t="s">
+      <c r="J10" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="151"/>
+      <c r="K10" s="152"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="132"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="160"/>
-      <c r="G11" s="161"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="172"/>
+      <c r="G11" s="173"/>
       <c r="H11" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="151"/>
+      <c r="K11" s="152"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="132"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="160"/>
-      <c r="G12" s="161"/>
-      <c r="H12" s="116" t="s">
+      <c r="B12" s="133"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="172"/>
+      <c r="G12" s="173"/>
+      <c r="H12" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="116" t="s">
+      <c r="I12" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="116"/>
-      <c r="K12" s="151"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="152"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>1</v>
       </c>
-      <c r="B13" s="134"/>
-      <c r="C13" s="135"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="162"/>
-      <c r="G13" s="163"/>
+      <c r="B13" s="135"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="141"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="174"/>
+      <c r="G13" s="175"/>
       <c r="H13" s="53">
         <v>43434</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="152"/>
+      <c r="K13" s="153"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
@@ -3131,7 +3157,7 @@
         <v>38</v>
       </c>
       <c r="I14" s="167"/>
-      <c r="J14" s="120" t="s">
+      <c r="J14" s="119" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="56" t="s">
@@ -3142,120 +3168,120 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="131"/>
-      <c r="D15" s="136" t="s">
+      <c r="C15" s="132"/>
+      <c r="D15" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="137"/>
-      <c r="F15" s="136" t="s">
+      <c r="E15" s="138"/>
+      <c r="F15" s="143" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="137"/>
-      <c r="H15" s="164" t="s">
+      <c r="G15" s="144"/>
+      <c r="H15" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="165"/>
+      <c r="I15" s="169"/>
       <c r="J15" s="52"/>
-      <c r="K15" s="150"/>
+      <c r="K15" s="151"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A16" s="120" t="s">
+      <c r="A16" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="132"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="139"/>
-      <c r="F16" s="138"/>
-      <c r="G16" s="139"/>
-      <c r="H16" s="120" t="s">
+      <c r="B16" s="133"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="145"/>
+      <c r="G16" s="146"/>
+      <c r="H16" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="120" t="s">
+      <c r="I16" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="120" t="s">
+      <c r="J16" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="151"/>
+      <c r="K16" s="152"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="132"/>
-      <c r="C17" s="133"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="139"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="146"/>
       <c r="H17" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48"/>
-      <c r="K17" s="151"/>
+      <c r="K17" s="152"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="120" t="s">
+      <c r="A18" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="132"/>
-      <c r="C18" s="133"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="139"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="139"/>
-      <c r="H18" s="120" t="s">
+      <c r="B18" s="133"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="120" t="s">
+      <c r="I18" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="J18" s="120"/>
-      <c r="K18" s="151"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="152"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>2</v>
       </c>
-      <c r="B19" s="134"/>
-      <c r="C19" s="135"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="141"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="141"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="50">
         <v>43434</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="151"/>
+      <c r="K19" s="152"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A20" s="119" t="s">
+      <c r="A20" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="153" t="s">
+      <c r="B20" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="154"/>
-      <c r="D20" s="153" t="s">
+      <c r="C20" s="157"/>
+      <c r="D20" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="154"/>
-      <c r="F20" s="153" t="s">
+      <c r="E20" s="157"/>
+      <c r="F20" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="154"/>
-      <c r="H20" s="168" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="168"/>
-      <c r="J20" s="121" t="s">
+      <c r="I20" s="165"/>
+      <c r="J20" s="120" t="s">
         <v>39</v>
       </c>
       <c r="K20" s="47" t="s">
@@ -3266,140 +3292,140 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="130" t="s">
+      <c r="B21" s="131" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="131"/>
-      <c r="D21" s="136" t="s">
+      <c r="C21" s="132"/>
+      <c r="D21" s="137" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="137"/>
-      <c r="F21" s="158" t="s">
+      <c r="E21" s="138"/>
+      <c r="F21" s="176" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="159"/>
-      <c r="H21" s="164" t="s">
+      <c r="G21" s="177"/>
+      <c r="H21" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="165"/>
+      <c r="I21" s="169"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="150"/>
+      <c r="K21" s="151"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="132"/>
-      <c r="C22" s="133"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="160"/>
-      <c r="G22" s="161"/>
-      <c r="H22" s="119" t="s">
+      <c r="B22" s="133"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="178"/>
+      <c r="G22" s="179"/>
+      <c r="H22" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="119" t="s">
+      <c r="I22" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="119" t="s">
+      <c r="J22" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="151"/>
+      <c r="K22" s="152"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="132"/>
-      <c r="C23" s="133"/>
-      <c r="D23" s="138"/>
-      <c r="E23" s="139"/>
-      <c r="F23" s="160"/>
-      <c r="G23" s="161"/>
+      <c r="B23" s="133"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="140"/>
+      <c r="F23" s="178"/>
+      <c r="G23" s="179"/>
       <c r="H23" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="151"/>
+      <c r="K23" s="152"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A24" s="119" t="s">
+      <c r="A24" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="132"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="139"/>
-      <c r="F24" s="160"/>
-      <c r="G24" s="161"/>
-      <c r="H24" s="119" t="s">
+      <c r="B24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="140"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="179"/>
+      <c r="H24" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="119" t="s">
+      <c r="I24" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="J24" s="119"/>
-      <c r="K24" s="151"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="152"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>3</v>
       </c>
-      <c r="B25" s="134"/>
-      <c r="C25" s="135"/>
-      <c r="D25" s="140"/>
-      <c r="E25" s="141"/>
-      <c r="F25" s="162"/>
-      <c r="G25" s="163"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="141"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="180"/>
+      <c r="G25" s="181"/>
       <c r="H25" s="53">
         <v>43434</v>
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="54"/>
-      <c r="K25" s="152"/>
+      <c r="K25" s="153"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A26" s="99" t="s">
+      <c r="A26" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="156" t="s">
+      <c r="B26" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="156"/>
-      <c r="D26" s="157"/>
-      <c r="E26" s="157"/>
-      <c r="F26" s="157"/>
-      <c r="G26" s="157"/>
-      <c r="H26" s="157"/>
-      <c r="I26" s="157"/>
-      <c r="J26" s="157"/>
-      <c r="K26" s="157"/>
+      <c r="C26" s="154"/>
+      <c r="D26" s="155"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="155"/>
+      <c r="H26" s="155"/>
+      <c r="I26" s="155"/>
+      <c r="J26" s="155"/>
+      <c r="K26" s="155"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A27" s="116" t="s">
+      <c r="A27" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="153" t="s">
+      <c r="B27" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="154"/>
-      <c r="D27" s="153" t="s">
+      <c r="C27" s="157"/>
+      <c r="D27" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="154"/>
-      <c r="F27" s="153" t="s">
+      <c r="E27" s="157"/>
+      <c r="F27" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="154"/>
-      <c r="H27" s="155" t="s">
+      <c r="G27" s="157"/>
+      <c r="H27" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="155"/>
-      <c r="J27" s="116" t="s">
+      <c r="I27" s="158"/>
+      <c r="J27" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="K27" s="118" t="s">
+      <c r="K27" s="117" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3407,123 +3433,123 @@
       <c r="A28" s="48">
         <v>4</v>
       </c>
-      <c r="B28" s="130" t="s">
+      <c r="B28" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="131"/>
-      <c r="D28" s="136" t="s">
+      <c r="C28" s="132"/>
+      <c r="D28" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="137"/>
-      <c r="F28" s="142" t="s">
+      <c r="E28" s="138"/>
+      <c r="F28" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="143"/>
-      <c r="H28" s="148" t="s">
+      <c r="G28" s="144"/>
+      <c r="H28" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="149"/>
+      <c r="I28" s="150"/>
       <c r="J28" s="52"/>
-      <c r="K28" s="150"/>
+      <c r="K28" s="151"/>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="132"/>
-      <c r="C29" s="133"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="139"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="116" t="s">
+      <c r="B29" s="133"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="I29" s="116" t="s">
+      <c r="I29" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="J29" s="116" t="s">
+      <c r="J29" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="151"/>
+      <c r="K29" s="152"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="132"/>
-      <c r="C30" s="133"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="139"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="145"/>
+      <c r="B30" s="133"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="140"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="146"/>
       <c r="H30" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I30" s="50"/>
       <c r="J30" s="48"/>
-      <c r="K30" s="151"/>
+      <c r="K30" s="152"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A31" s="116" t="s">
+      <c r="A31" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="132"/>
-      <c r="C31" s="133"/>
-      <c r="D31" s="138"/>
-      <c r="E31" s="139"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="116" t="s">
+      <c r="B31" s="133"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="139"/>
+      <c r="E31" s="140"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="116" t="s">
+      <c r="I31" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="J31" s="116"/>
-      <c r="K31" s="151"/>
+      <c r="J31" s="115"/>
+      <c r="K31" s="152"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="51">
         <v>4</v>
       </c>
-      <c r="B32" s="134"/>
-      <c r="C32" s="135"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="141"/>
-      <c r="F32" s="146"/>
-      <c r="G32" s="147"/>
+      <c r="B32" s="135"/>
+      <c r="C32" s="136"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="148"/>
       <c r="H32" s="50">
         <v>43434</v>
       </c>
       <c r="I32" s="50"/>
       <c r="J32" s="48"/>
-      <c r="K32" s="152"/>
+      <c r="K32" s="153"/>
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="153" t="s">
+      <c r="B33" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="154"/>
-      <c r="D33" s="153" t="s">
+      <c r="C33" s="157"/>
+      <c r="D33" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="154"/>
-      <c r="F33" s="153" t="s">
+      <c r="E33" s="157"/>
+      <c r="F33" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="154"/>
-      <c r="H33" s="155" t="s">
+      <c r="G33" s="157"/>
+      <c r="H33" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="155"/>
-      <c r="J33" s="116" t="s">
+      <c r="I33" s="158"/>
+      <c r="J33" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="K33" s="118" t="s">
+      <c r="K33" s="117" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3531,123 +3557,123 @@
       <c r="A34" s="48">
         <v>5</v>
       </c>
-      <c r="B34" s="130" t="s">
+      <c r="B34" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="131"/>
-      <c r="D34" s="136" t="s">
+      <c r="C34" s="132"/>
+      <c r="D34" s="137" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="137"/>
-      <c r="F34" s="142" t="s">
+      <c r="E34" s="138"/>
+      <c r="F34" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="143"/>
-      <c r="H34" s="148" t="s">
+      <c r="G34" s="144"/>
+      <c r="H34" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="I34" s="149"/>
+      <c r="I34" s="150"/>
       <c r="J34" s="52"/>
-      <c r="K34" s="150"/>
+      <c r="K34" s="151"/>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A35" s="116" t="s">
+      <c r="A35" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="132"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="138"/>
-      <c r="E35" s="139"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="145"/>
-      <c r="H35" s="116" t="s">
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
+      <c r="D35" s="139"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="146"/>
+      <c r="H35" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="I35" s="116" t="s">
+      <c r="I35" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="J35" s="116" t="s">
+      <c r="J35" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="151"/>
+      <c r="K35" s="152"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="132"/>
-      <c r="C36" s="133"/>
-      <c r="D36" s="138"/>
-      <c r="E36" s="139"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="145"/>
+      <c r="B36" s="133"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="139"/>
+      <c r="E36" s="140"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="146"/>
       <c r="H36" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I36" s="50"/>
       <c r="J36" s="48"/>
-      <c r="K36" s="151"/>
+      <c r="K36" s="152"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A37" s="116" t="s">
+      <c r="A37" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="132"/>
-      <c r="C37" s="133"/>
-      <c r="D37" s="138"/>
-      <c r="E37" s="139"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="116" t="s">
+      <c r="B37" s="133"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="139"/>
+      <c r="E37" s="140"/>
+      <c r="F37" s="145"/>
+      <c r="G37" s="146"/>
+      <c r="H37" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="116" t="s">
+      <c r="I37" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="J37" s="116"/>
-      <c r="K37" s="151"/>
+      <c r="J37" s="115"/>
+      <c r="K37" s="152"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="51">
         <v>5</v>
       </c>
-      <c r="B38" s="134"/>
-      <c r="C38" s="135"/>
-      <c r="D38" s="140"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="146"/>
-      <c r="G38" s="147"/>
+      <c r="B38" s="135"/>
+      <c r="C38" s="136"/>
+      <c r="D38" s="141"/>
+      <c r="E38" s="142"/>
+      <c r="F38" s="147"/>
+      <c r="G38" s="148"/>
       <c r="H38" s="50">
         <v>43434</v>
       </c>
       <c r="I38" s="50"/>
       <c r="J38" s="48"/>
-      <c r="K38" s="152"/>
+      <c r="K38" s="153"/>
     </row>
     <row r="39" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A39" s="122" t="s">
+      <c r="A39" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="153" t="s">
+      <c r="B39" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="154"/>
-      <c r="D39" s="153" t="s">
+      <c r="C39" s="157"/>
+      <c r="D39" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="154"/>
-      <c r="F39" s="153" t="s">
+      <c r="E39" s="157"/>
+      <c r="F39" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="154"/>
-      <c r="H39" s="155" t="s">
+      <c r="G39" s="157"/>
+      <c r="H39" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="155"/>
-      <c r="J39" s="122" t="s">
+      <c r="I39" s="158"/>
+      <c r="J39" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="K39" s="123" t="s">
+      <c r="K39" s="122" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3655,123 +3681,123 @@
       <c r="A40" s="48">
         <v>6</v>
       </c>
-      <c r="B40" s="130" t="s">
+      <c r="B40" s="131" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="131"/>
-      <c r="D40" s="136" t="s">
+      <c r="C40" s="132"/>
+      <c r="D40" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="137"/>
-      <c r="F40" s="142" t="s">
+      <c r="E40" s="138"/>
+      <c r="F40" s="143" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="143"/>
-      <c r="H40" s="148" t="s">
+      <c r="G40" s="144"/>
+      <c r="H40" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="149"/>
+      <c r="I40" s="150"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="150"/>
+      <c r="K40" s="151"/>
     </row>
     <row r="41" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A41" s="122" t="s">
+      <c r="A41" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="132"/>
-      <c r="C41" s="133"/>
-      <c r="D41" s="138"/>
-      <c r="E41" s="139"/>
-      <c r="F41" s="144"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="122" t="s">
+      <c r="B41" s="133"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="139"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="146"/>
+      <c r="H41" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="122" t="s">
+      <c r="I41" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="122" t="s">
+      <c r="J41" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="151"/>
+      <c r="K41" s="152"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="132"/>
-      <c r="C42" s="133"/>
-      <c r="D42" s="138"/>
-      <c r="E42" s="139"/>
-      <c r="F42" s="144"/>
-      <c r="G42" s="145"/>
+      <c r="B42" s="133"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="139"/>
+      <c r="E42" s="140"/>
+      <c r="F42" s="145"/>
+      <c r="G42" s="146"/>
       <c r="H42" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I42" s="50"/>
       <c r="J42" s="48"/>
-      <c r="K42" s="151"/>
+      <c r="K42" s="152"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A43" s="122" t="s">
+      <c r="A43" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="132"/>
-      <c r="C43" s="133"/>
-      <c r="D43" s="138"/>
-      <c r="E43" s="139"/>
-      <c r="F43" s="144"/>
-      <c r="G43" s="145"/>
-      <c r="H43" s="122" t="s">
+      <c r="B43" s="133"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="140"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="146"/>
+      <c r="H43" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="I43" s="122" t="s">
+      <c r="I43" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="J43" s="122"/>
-      <c r="K43" s="151"/>
+      <c r="J43" s="121"/>
+      <c r="K43" s="152"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="51">
         <v>6</v>
       </c>
-      <c r="B44" s="134"/>
-      <c r="C44" s="135"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="141"/>
-      <c r="F44" s="146"/>
-      <c r="G44" s="147"/>
+      <c r="B44" s="135"/>
+      <c r="C44" s="136"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="142"/>
+      <c r="F44" s="147"/>
+      <c r="G44" s="148"/>
       <c r="H44" s="50">
         <v>43434</v>
       </c>
       <c r="I44" s="50"/>
       <c r="J44" s="48"/>
-      <c r="K44" s="152"/>
+      <c r="K44" s="153"/>
     </row>
     <row r="45" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A45" s="122" t="s">
+      <c r="A45" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="153" t="s">
+      <c r="B45" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="154"/>
-      <c r="D45" s="153" t="s">
+      <c r="C45" s="157"/>
+      <c r="D45" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="154"/>
-      <c r="F45" s="153" t="s">
+      <c r="E45" s="157"/>
+      <c r="F45" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="154"/>
-      <c r="H45" s="155" t="s">
+      <c r="G45" s="157"/>
+      <c r="H45" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="155"/>
-      <c r="J45" s="122" t="s">
+      <c r="I45" s="158"/>
+      <c r="J45" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="K45" s="123" t="s">
+      <c r="K45" s="122" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3779,140 +3805,140 @@
       <c r="A46" s="48">
         <v>7</v>
       </c>
-      <c r="B46" s="130" t="s">
+      <c r="B46" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="131"/>
-      <c r="D46" s="136" t="s">
+      <c r="C46" s="132"/>
+      <c r="D46" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="137"/>
-      <c r="F46" s="170" t="s">
+      <c r="E46" s="138"/>
+      <c r="F46" s="159" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="171"/>
-      <c r="H46" s="148" t="s">
+      <c r="G46" s="160"/>
+      <c r="H46" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="I46" s="149"/>
+      <c r="I46" s="150"/>
       <c r="J46" s="52"/>
-      <c r="K46" s="150"/>
+      <c r="K46" s="151"/>
     </row>
     <row r="47" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A47" s="122" t="s">
+      <c r="A47" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="132"/>
-      <c r="C47" s="133"/>
-      <c r="D47" s="138"/>
-      <c r="E47" s="139"/>
-      <c r="F47" s="172"/>
-      <c r="G47" s="173"/>
-      <c r="H47" s="122" t="s">
+      <c r="B47" s="133"/>
+      <c r="C47" s="134"/>
+      <c r="D47" s="139"/>
+      <c r="E47" s="140"/>
+      <c r="F47" s="161"/>
+      <c r="G47" s="162"/>
+      <c r="H47" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="I47" s="122" t="s">
+      <c r="I47" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="J47" s="122" t="s">
+      <c r="J47" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="K47" s="151"/>
+      <c r="K47" s="152"/>
     </row>
     <row r="48" spans="1:11" ht="10.5" customHeight="1">
       <c r="A48" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="132"/>
-      <c r="C48" s="133"/>
-      <c r="D48" s="138"/>
-      <c r="E48" s="139"/>
-      <c r="F48" s="172"/>
-      <c r="G48" s="173"/>
+      <c r="B48" s="133"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="139"/>
+      <c r="E48" s="140"/>
+      <c r="F48" s="161"/>
+      <c r="G48" s="162"/>
       <c r="H48" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I48" s="50"/>
       <c r="J48" s="48"/>
-      <c r="K48" s="151"/>
+      <c r="K48" s="152"/>
     </row>
     <row r="49" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A49" s="122" t="s">
+      <c r="A49" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="132"/>
-      <c r="C49" s="133"/>
-      <c r="D49" s="138"/>
-      <c r="E49" s="139"/>
-      <c r="F49" s="172"/>
-      <c r="G49" s="173"/>
-      <c r="H49" s="122" t="s">
+      <c r="B49" s="133"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="139"/>
+      <c r="E49" s="140"/>
+      <c r="F49" s="161"/>
+      <c r="G49" s="162"/>
+      <c r="H49" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="I49" s="122" t="s">
+      <c r="I49" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="J49" s="122"/>
-      <c r="K49" s="151"/>
+      <c r="J49" s="121"/>
+      <c r="K49" s="152"/>
     </row>
     <row r="50" spans="1:11" ht="10.5" customHeight="1">
       <c r="A50" s="51">
         <v>7</v>
       </c>
-      <c r="B50" s="134"/>
-      <c r="C50" s="135"/>
-      <c r="D50" s="140"/>
-      <c r="E50" s="141"/>
-      <c r="F50" s="174"/>
-      <c r="G50" s="175"/>
+      <c r="B50" s="135"/>
+      <c r="C50" s="136"/>
+      <c r="D50" s="141"/>
+      <c r="E50" s="142"/>
+      <c r="F50" s="163"/>
+      <c r="G50" s="164"/>
       <c r="H50" s="50">
         <v>43434</v>
       </c>
       <c r="I50" s="50"/>
       <c r="J50" s="48"/>
-      <c r="K50" s="152"/>
+      <c r="K50" s="153"/>
     </row>
     <row r="51" spans="1:11" s="58" customFormat="1">
-      <c r="A51" s="99" t="s">
+      <c r="A51" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="156" t="s">
+      <c r="B51" s="154" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="156"/>
-      <c r="D51" s="157"/>
-      <c r="E51" s="157"/>
-      <c r="F51" s="157"/>
-      <c r="G51" s="157"/>
-      <c r="H51" s="157"/>
-      <c r="I51" s="157"/>
-      <c r="J51" s="157"/>
-      <c r="K51" s="157"/>
+      <c r="C51" s="154"/>
+      <c r="D51" s="155"/>
+      <c r="E51" s="155"/>
+      <c r="F51" s="155"/>
+      <c r="G51" s="155"/>
+      <c r="H51" s="155"/>
+      <c r="I51" s="155"/>
+      <c r="J51" s="155"/>
+      <c r="K51" s="155"/>
     </row>
     <row r="52" spans="1:11" s="58" customFormat="1">
-      <c r="A52" s="125" t="s">
+      <c r="A52" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="153" t="s">
+      <c r="B52" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="154"/>
-      <c r="D52" s="153" t="s">
+      <c r="C52" s="157"/>
+      <c r="D52" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="154"/>
-      <c r="F52" s="153" t="s">
+      <c r="E52" s="157"/>
+      <c r="F52" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G52" s="154"/>
-      <c r="H52" s="155" t="s">
+      <c r="G52" s="157"/>
+      <c r="H52" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I52" s="155"/>
-      <c r="J52" s="125" t="s">
+      <c r="I52" s="158"/>
+      <c r="J52" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="K52" s="124" t="s">
+      <c r="K52" s="123" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3920,123 +3946,123 @@
       <c r="A53" s="48">
         <v>8</v>
       </c>
-      <c r="B53" s="130" t="s">
+      <c r="B53" s="131" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="131"/>
-      <c r="D53" s="136" t="s">
+      <c r="C53" s="132"/>
+      <c r="D53" s="137" t="s">
         <v>89</v>
       </c>
-      <c r="E53" s="137"/>
-      <c r="F53" s="142" t="s">
+      <c r="E53" s="138"/>
+      <c r="F53" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="G53" s="143"/>
-      <c r="H53" s="148" t="s">
+      <c r="G53" s="144"/>
+      <c r="H53" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="I53" s="149"/>
+      <c r="I53" s="150"/>
       <c r="J53" s="52"/>
-      <c r="K53" s="150"/>
+      <c r="K53" s="151"/>
     </row>
     <row r="54" spans="1:11" s="58" customFormat="1">
-      <c r="A54" s="125" t="s">
+      <c r="A54" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="132"/>
-      <c r="C54" s="133"/>
-      <c r="D54" s="138"/>
-      <c r="E54" s="139"/>
-      <c r="F54" s="144"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="125" t="s">
+      <c r="B54" s="133"/>
+      <c r="C54" s="134"/>
+      <c r="D54" s="139"/>
+      <c r="E54" s="140"/>
+      <c r="F54" s="145"/>
+      <c r="G54" s="146"/>
+      <c r="H54" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="I54" s="125" t="s">
+      <c r="I54" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="J54" s="125" t="s">
+      <c r="J54" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K54" s="151"/>
+      <c r="K54" s="152"/>
     </row>
     <row r="55" spans="1:11" s="58" customFormat="1">
       <c r="A55" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="132"/>
-      <c r="C55" s="133"/>
-      <c r="D55" s="138"/>
-      <c r="E55" s="139"/>
-      <c r="F55" s="144"/>
-      <c r="G55" s="145"/>
+      <c r="B55" s="133"/>
+      <c r="C55" s="134"/>
+      <c r="D55" s="139"/>
+      <c r="E55" s="140"/>
+      <c r="F55" s="145"/>
+      <c r="G55" s="146"/>
       <c r="H55" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I55" s="50"/>
       <c r="J55" s="48"/>
-      <c r="K55" s="151"/>
+      <c r="K55" s="152"/>
     </row>
     <row r="56" spans="1:11" s="58" customFormat="1">
-      <c r="A56" s="125" t="s">
+      <c r="A56" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="132"/>
-      <c r="C56" s="133"/>
-      <c r="D56" s="138"/>
-      <c r="E56" s="139"/>
-      <c r="F56" s="144"/>
-      <c r="G56" s="145"/>
-      <c r="H56" s="125" t="s">
+      <c r="B56" s="133"/>
+      <c r="C56" s="134"/>
+      <c r="D56" s="139"/>
+      <c r="E56" s="140"/>
+      <c r="F56" s="145"/>
+      <c r="G56" s="146"/>
+      <c r="H56" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="I56" s="125" t="s">
+      <c r="I56" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="J56" s="125"/>
-      <c r="K56" s="151"/>
+      <c r="J56" s="124"/>
+      <c r="K56" s="152"/>
     </row>
     <row r="57" spans="1:11" s="58" customFormat="1">
       <c r="A57" s="51">
         <v>8</v>
       </c>
-      <c r="B57" s="134"/>
-      <c r="C57" s="135"/>
-      <c r="D57" s="140"/>
-      <c r="E57" s="141"/>
-      <c r="F57" s="146"/>
-      <c r="G57" s="147"/>
+      <c r="B57" s="135"/>
+      <c r="C57" s="136"/>
+      <c r="D57" s="141"/>
+      <c r="E57" s="142"/>
+      <c r="F57" s="147"/>
+      <c r="G57" s="148"/>
       <c r="H57" s="50">
         <v>43434</v>
       </c>
       <c r="I57" s="50"/>
       <c r="J57" s="48"/>
-      <c r="K57" s="152"/>
+      <c r="K57" s="153"/>
     </row>
     <row r="58" spans="1:11" s="58" customFormat="1">
-      <c r="A58" s="125" t="s">
+      <c r="A58" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="153" t="s">
+      <c r="B58" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="154"/>
-      <c r="D58" s="153" t="s">
+      <c r="C58" s="157"/>
+      <c r="D58" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="154"/>
-      <c r="F58" s="153" t="s">
+      <c r="E58" s="157"/>
+      <c r="F58" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G58" s="154"/>
-      <c r="H58" s="155" t="s">
+      <c r="G58" s="157"/>
+      <c r="H58" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I58" s="155"/>
-      <c r="J58" s="125" t="s">
+      <c r="I58" s="158"/>
+      <c r="J58" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="K58" s="124" t="s">
+      <c r="K58" s="123" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4044,123 +4070,123 @@
       <c r="A59" s="48">
         <v>9</v>
       </c>
-      <c r="B59" s="130" t="s">
+      <c r="B59" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="131"/>
-      <c r="D59" s="136" t="s">
+      <c r="C59" s="132"/>
+      <c r="D59" s="137" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="137"/>
-      <c r="F59" s="142" t="s">
+      <c r="E59" s="138"/>
+      <c r="F59" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="G59" s="143"/>
-      <c r="H59" s="148" t="s">
+      <c r="G59" s="144"/>
+      <c r="H59" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="I59" s="149"/>
+      <c r="I59" s="150"/>
       <c r="J59" s="52"/>
-      <c r="K59" s="150"/>
+      <c r="K59" s="151"/>
     </row>
     <row r="60" spans="1:11" s="58" customFormat="1">
-      <c r="A60" s="125" t="s">
+      <c r="A60" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="132"/>
-      <c r="C60" s="133"/>
-      <c r="D60" s="138"/>
-      <c r="E60" s="139"/>
-      <c r="F60" s="144"/>
-      <c r="G60" s="145"/>
-      <c r="H60" s="125" t="s">
+      <c r="B60" s="133"/>
+      <c r="C60" s="134"/>
+      <c r="D60" s="139"/>
+      <c r="E60" s="140"/>
+      <c r="F60" s="145"/>
+      <c r="G60" s="146"/>
+      <c r="H60" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="I60" s="125" t="s">
+      <c r="I60" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="J60" s="125" t="s">
+      <c r="J60" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K60" s="151"/>
+      <c r="K60" s="152"/>
     </row>
     <row r="61" spans="1:11" s="58" customFormat="1">
       <c r="A61" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B61" s="132"/>
-      <c r="C61" s="133"/>
-      <c r="D61" s="138"/>
-      <c r="E61" s="139"/>
-      <c r="F61" s="144"/>
-      <c r="G61" s="145"/>
+      <c r="B61" s="133"/>
+      <c r="C61" s="134"/>
+      <c r="D61" s="139"/>
+      <c r="E61" s="140"/>
+      <c r="F61" s="145"/>
+      <c r="G61" s="146"/>
       <c r="H61" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I61" s="50"/>
       <c r="J61" s="48"/>
-      <c r="K61" s="151"/>
+      <c r="K61" s="152"/>
     </row>
     <row r="62" spans="1:11" s="58" customFormat="1">
-      <c r="A62" s="125" t="s">
+      <c r="A62" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="132"/>
-      <c r="C62" s="133"/>
-      <c r="D62" s="138"/>
-      <c r="E62" s="139"/>
-      <c r="F62" s="144"/>
-      <c r="G62" s="145"/>
-      <c r="H62" s="125" t="s">
+      <c r="B62" s="133"/>
+      <c r="C62" s="134"/>
+      <c r="D62" s="139"/>
+      <c r="E62" s="140"/>
+      <c r="F62" s="145"/>
+      <c r="G62" s="146"/>
+      <c r="H62" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="I62" s="125" t="s">
+      <c r="I62" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="J62" s="125"/>
-      <c r="K62" s="151"/>
+      <c r="J62" s="124"/>
+      <c r="K62" s="152"/>
     </row>
     <row r="63" spans="1:11" s="58" customFormat="1">
       <c r="A63" s="51">
         <v>9</v>
       </c>
-      <c r="B63" s="134"/>
-      <c r="C63" s="135"/>
-      <c r="D63" s="140"/>
-      <c r="E63" s="141"/>
-      <c r="F63" s="146"/>
-      <c r="G63" s="147"/>
+      <c r="B63" s="135"/>
+      <c r="C63" s="136"/>
+      <c r="D63" s="141"/>
+      <c r="E63" s="142"/>
+      <c r="F63" s="147"/>
+      <c r="G63" s="148"/>
       <c r="H63" s="50">
         <v>43434</v>
       </c>
       <c r="I63" s="50"/>
       <c r="J63" s="48"/>
-      <c r="K63" s="152"/>
+      <c r="K63" s="153"/>
     </row>
     <row r="64" spans="1:11" s="58" customFormat="1">
-      <c r="A64" s="125" t="s">
+      <c r="A64" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="153" t="s">
+      <c r="B64" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="154"/>
-      <c r="D64" s="153" t="s">
+      <c r="C64" s="157"/>
+      <c r="D64" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E64" s="154"/>
-      <c r="F64" s="153" t="s">
+      <c r="E64" s="157"/>
+      <c r="F64" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G64" s="154"/>
-      <c r="H64" s="155" t="s">
+      <c r="G64" s="157"/>
+      <c r="H64" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I64" s="155"/>
-      <c r="J64" s="125" t="s">
+      <c r="I64" s="158"/>
+      <c r="J64" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="K64" s="124" t="s">
+      <c r="K64" s="123" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4168,140 +4194,140 @@
       <c r="A65" s="48">
         <v>10</v>
       </c>
-      <c r="B65" s="130" t="s">
+      <c r="B65" s="131" t="s">
         <v>83</v>
       </c>
-      <c r="C65" s="131"/>
-      <c r="D65" s="136" t="s">
+      <c r="C65" s="132"/>
+      <c r="D65" s="137" t="s">
         <v>93</v>
       </c>
-      <c r="E65" s="137"/>
-      <c r="F65" s="142" t="s">
+      <c r="E65" s="138"/>
+      <c r="F65" s="143" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="143"/>
-      <c r="H65" s="148" t="s">
+      <c r="G65" s="144"/>
+      <c r="H65" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="I65" s="149"/>
+      <c r="I65" s="150"/>
       <c r="J65" s="52"/>
-      <c r="K65" s="150"/>
+      <c r="K65" s="151"/>
     </row>
     <row r="66" spans="1:11" s="58" customFormat="1">
-      <c r="A66" s="125" t="s">
+      <c r="A66" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="132"/>
-      <c r="C66" s="133"/>
-      <c r="D66" s="138"/>
-      <c r="E66" s="139"/>
-      <c r="F66" s="144"/>
-      <c r="G66" s="145"/>
-      <c r="H66" s="125" t="s">
+      <c r="B66" s="133"/>
+      <c r="C66" s="134"/>
+      <c r="D66" s="139"/>
+      <c r="E66" s="140"/>
+      <c r="F66" s="145"/>
+      <c r="G66" s="146"/>
+      <c r="H66" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="I66" s="125" t="s">
+      <c r="I66" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="J66" s="125" t="s">
+      <c r="J66" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K66" s="151"/>
+      <c r="K66" s="152"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B67" s="132"/>
-      <c r="C67" s="133"/>
-      <c r="D67" s="138"/>
-      <c r="E67" s="139"/>
-      <c r="F67" s="144"/>
-      <c r="G67" s="145"/>
+      <c r="B67" s="133"/>
+      <c r="C67" s="134"/>
+      <c r="D67" s="139"/>
+      <c r="E67" s="140"/>
+      <c r="F67" s="145"/>
+      <c r="G67" s="146"/>
       <c r="H67" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I67" s="50"/>
       <c r="J67" s="48"/>
-      <c r="K67" s="151"/>
+      <c r="K67" s="152"/>
     </row>
     <row r="68" spans="1:11" s="58" customFormat="1">
-      <c r="A68" s="125" t="s">
+      <c r="A68" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="132"/>
-      <c r="C68" s="133"/>
-      <c r="D68" s="138"/>
-      <c r="E68" s="139"/>
-      <c r="F68" s="144"/>
-      <c r="G68" s="145"/>
-      <c r="H68" s="125" t="s">
+      <c r="B68" s="133"/>
+      <c r="C68" s="134"/>
+      <c r="D68" s="139"/>
+      <c r="E68" s="140"/>
+      <c r="F68" s="145"/>
+      <c r="G68" s="146"/>
+      <c r="H68" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="I68" s="125" t="s">
+      <c r="I68" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="J68" s="125"/>
-      <c r="K68" s="151"/>
+      <c r="J68" s="124"/>
+      <c r="K68" s="152"/>
     </row>
     <row r="69" spans="1:11" s="58" customFormat="1">
       <c r="A69" s="51">
         <v>10</v>
       </c>
-      <c r="B69" s="134"/>
-      <c r="C69" s="135"/>
-      <c r="D69" s="140"/>
-      <c r="E69" s="141"/>
-      <c r="F69" s="146"/>
-      <c r="G69" s="147"/>
+      <c r="B69" s="135"/>
+      <c r="C69" s="136"/>
+      <c r="D69" s="141"/>
+      <c r="E69" s="142"/>
+      <c r="F69" s="147"/>
+      <c r="G69" s="148"/>
       <c r="H69" s="50">
         <v>43434</v>
       </c>
       <c r="I69" s="50"/>
       <c r="J69" s="48"/>
-      <c r="K69" s="152"/>
+      <c r="K69" s="153"/>
     </row>
     <row r="70" spans="1:11" s="58" customFormat="1">
-      <c r="A70" s="99" t="s">
+      <c r="A70" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="B70" s="156" t="s">
+      <c r="B70" s="154" t="s">
         <v>96</v>
       </c>
-      <c r="C70" s="156"/>
-      <c r="D70" s="157"/>
-      <c r="E70" s="157"/>
-      <c r="F70" s="157"/>
-      <c r="G70" s="157"/>
-      <c r="H70" s="157"/>
-      <c r="I70" s="157"/>
-      <c r="J70" s="157"/>
-      <c r="K70" s="157"/>
+      <c r="C70" s="154"/>
+      <c r="D70" s="155"/>
+      <c r="E70" s="155"/>
+      <c r="F70" s="155"/>
+      <c r="G70" s="155"/>
+      <c r="H70" s="155"/>
+      <c r="I70" s="155"/>
+      <c r="J70" s="155"/>
+      <c r="K70" s="155"/>
     </row>
     <row r="71" spans="1:11" s="58" customFormat="1">
-      <c r="A71" s="127" t="s">
+      <c r="A71" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B71" s="153" t="s">
+      <c r="B71" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C71" s="154"/>
-      <c r="D71" s="153" t="s">
+      <c r="C71" s="157"/>
+      <c r="D71" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="E71" s="154"/>
-      <c r="F71" s="153" t="s">
+      <c r="E71" s="157"/>
+      <c r="F71" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="G71" s="154"/>
-      <c r="H71" s="155" t="s">
+      <c r="G71" s="157"/>
+      <c r="H71" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="I71" s="155"/>
-      <c r="J71" s="127" t="s">
+      <c r="I71" s="158"/>
+      <c r="J71" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="K71" s="126" t="s">
+      <c r="K71" s="125" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4309,326 +4335,470 @@
       <c r="A72" s="48">
         <v>11</v>
       </c>
-      <c r="B72" s="130" t="s">
+      <c r="B72" s="131" t="s">
         <v>98</v>
       </c>
-      <c r="C72" s="131"/>
-      <c r="D72" s="136" t="s">
-        <v>99</v>
-      </c>
-      <c r="E72" s="137"/>
-      <c r="F72" s="142" t="s">
-        <v>100</v>
-      </c>
-      <c r="G72" s="143"/>
-      <c r="H72" s="148" t="s">
+      <c r="C72" s="132"/>
+      <c r="D72" s="137" t="s">
+        <v>106</v>
+      </c>
+      <c r="E72" s="138"/>
+      <c r="F72" s="143" t="s">
+        <v>107</v>
+      </c>
+      <c r="G72" s="144"/>
+      <c r="H72" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="I72" s="149"/>
+      <c r="I72" s="150"/>
       <c r="J72" s="52"/>
-      <c r="K72" s="150"/>
+      <c r="K72" s="151"/>
     </row>
     <row r="73" spans="1:11" s="58" customFormat="1">
-      <c r="A73" s="127" t="s">
+      <c r="A73" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="132"/>
-      <c r="C73" s="133"/>
-      <c r="D73" s="138"/>
-      <c r="E73" s="139"/>
-      <c r="F73" s="144"/>
-      <c r="G73" s="145"/>
-      <c r="H73" s="127" t="s">
+      <c r="B73" s="133"/>
+      <c r="C73" s="134"/>
+      <c r="D73" s="139"/>
+      <c r="E73" s="140"/>
+      <c r="F73" s="145"/>
+      <c r="G73" s="146"/>
+      <c r="H73" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="I73" s="127" t="s">
+      <c r="I73" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="J73" s="127" t="s">
+      <c r="J73" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K73" s="151"/>
+      <c r="K73" s="152"/>
     </row>
     <row r="74" spans="1:11" s="58" customFormat="1">
       <c r="A74" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="132"/>
-      <c r="C74" s="133"/>
-      <c r="D74" s="138"/>
-      <c r="E74" s="139"/>
-      <c r="F74" s="144"/>
-      <c r="G74" s="145"/>
+      <c r="B74" s="133"/>
+      <c r="C74" s="134"/>
+      <c r="D74" s="139"/>
+      <c r="E74" s="140"/>
+      <c r="F74" s="145"/>
+      <c r="G74" s="146"/>
       <c r="H74" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I74" s="50"/>
       <c r="J74" s="48"/>
-      <c r="K74" s="151"/>
+      <c r="K74" s="152"/>
     </row>
     <row r="75" spans="1:11" s="58" customFormat="1">
-      <c r="A75" s="127" t="s">
+      <c r="A75" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="B75" s="132"/>
-      <c r="C75" s="133"/>
-      <c r="D75" s="138"/>
-      <c r="E75" s="139"/>
-      <c r="F75" s="144"/>
-      <c r="G75" s="145"/>
-      <c r="H75" s="127" t="s">
+      <c r="B75" s="133"/>
+      <c r="C75" s="134"/>
+      <c r="D75" s="139"/>
+      <c r="E75" s="140"/>
+      <c r="F75" s="145"/>
+      <c r="G75" s="146"/>
+      <c r="H75" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="I75" s="127" t="s">
+      <c r="I75" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="J75" s="127"/>
-      <c r="K75" s="151"/>
+      <c r="J75" s="126"/>
+      <c r="K75" s="152"/>
     </row>
     <row r="76" spans="1:11" s="58" customFormat="1">
       <c r="A76" s="51">
         <v>11</v>
       </c>
-      <c r="B76" s="134"/>
-      <c r="C76" s="135"/>
-      <c r="D76" s="140"/>
-      <c r="E76" s="141"/>
-      <c r="F76" s="146"/>
-      <c r="G76" s="147"/>
+      <c r="B76" s="135"/>
+      <c r="C76" s="136"/>
+      <c r="D76" s="141"/>
+      <c r="E76" s="142"/>
+      <c r="F76" s="147"/>
+      <c r="G76" s="148"/>
       <c r="H76" s="50">
         <v>43434</v>
       </c>
       <c r="I76" s="50"/>
       <c r="J76" s="48"/>
-      <c r="K76" s="152"/>
+      <c r="K76" s="153"/>
     </row>
     <row r="77" spans="1:11" s="58" customFormat="1">
-      <c r="A77" s="62"/>
-      <c r="H77" s="62"/>
-      <c r="I77" s="62"/>
-      <c r="J77" s="62"/>
-      <c r="K77" s="62"/>
+      <c r="A77" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="166" t="s">
+        <v>48</v>
+      </c>
+      <c r="C77" s="167"/>
+      <c r="D77" s="166" t="s">
+        <v>36</v>
+      </c>
+      <c r="E77" s="167"/>
+      <c r="F77" s="166" t="s">
+        <v>37</v>
+      </c>
+      <c r="G77" s="167"/>
+      <c r="H77" s="166" t="s">
+        <v>38</v>
+      </c>
+      <c r="I77" s="167"/>
+      <c r="J77" s="119" t="s">
+        <v>39</v>
+      </c>
+      <c r="K77" s="56" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="78" spans="1:11" s="58" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A78" s="2"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
+      <c r="A78" s="48">
+        <v>12</v>
+      </c>
+      <c r="B78" s="131" t="s">
+        <v>103</v>
+      </c>
+      <c r="C78" s="132"/>
+      <c r="D78" s="137" t="s">
+        <v>99</v>
+      </c>
+      <c r="E78" s="138"/>
+      <c r="F78" s="143" t="s">
+        <v>108</v>
+      </c>
+      <c r="G78" s="144"/>
+      <c r="H78" s="168" t="s">
+        <v>10</v>
+      </c>
+      <c r="I78" s="169"/>
+      <c r="J78" s="52"/>
+      <c r="K78" s="151"/>
     </row>
     <row r="79" spans="1:11" s="58" customFormat="1">
-      <c r="A79" s="2"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
+      <c r="A79" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="133"/>
+      <c r="C79" s="134"/>
+      <c r="D79" s="139"/>
+      <c r="E79" s="140"/>
+      <c r="F79" s="145"/>
+      <c r="G79" s="146"/>
+      <c r="H79" s="119" t="s">
+        <v>42</v>
+      </c>
+      <c r="I79" s="119" t="s">
+        <v>43</v>
+      </c>
+      <c r="J79" s="119" t="s">
+        <v>44</v>
+      </c>
+      <c r="K79" s="152"/>
     </row>
     <row r="80" spans="1:11" s="58" customFormat="1">
-      <c r="A80" s="2"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
+      <c r="A80" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="133"/>
+      <c r="C80" s="134"/>
+      <c r="D80" s="139"/>
+      <c r="E80" s="140"/>
+      <c r="F80" s="145"/>
+      <c r="G80" s="146"/>
+      <c r="H80" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I80" s="50"/>
+      <c r="J80" s="48"/>
+      <c r="K80" s="152"/>
     </row>
     <row r="81" spans="1:11" s="58" customFormat="1">
-      <c r="A81" s="2"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
+      <c r="A81" s="119" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81" s="133"/>
+      <c r="C81" s="134"/>
+      <c r="D81" s="139"/>
+      <c r="E81" s="140"/>
+      <c r="F81" s="145"/>
+      <c r="G81" s="146"/>
+      <c r="H81" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="I81" s="119" t="s">
+        <v>47</v>
+      </c>
+      <c r="J81" s="119"/>
+      <c r="K81" s="152"/>
     </row>
     <row r="82" spans="1:11" s="58" customFormat="1">
-      <c r="A82" s="2"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
+      <c r="A82" s="51">
+        <v>12</v>
+      </c>
+      <c r="B82" s="135"/>
+      <c r="C82" s="136"/>
+      <c r="D82" s="141"/>
+      <c r="E82" s="142"/>
+      <c r="F82" s="147"/>
+      <c r="G82" s="148"/>
+      <c r="H82" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I82" s="50"/>
+      <c r="J82" s="48"/>
+      <c r="K82" s="152"/>
     </row>
     <row r="83" spans="1:11" s="58" customFormat="1">
-      <c r="A83" s="2"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
+      <c r="A83" s="128" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" s="156" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="157"/>
+      <c r="D83" s="156" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83" s="157"/>
+      <c r="F83" s="156" t="s">
+        <v>37</v>
+      </c>
+      <c r="G83" s="157"/>
+      <c r="H83" s="158" t="s">
+        <v>38</v>
+      </c>
+      <c r="I83" s="158"/>
+      <c r="J83" s="128" t="s">
+        <v>39</v>
+      </c>
+      <c r="K83" s="127" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="84" spans="1:11" s="58" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A84" s="2"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
+      <c r="A84" s="48">
+        <v>13</v>
+      </c>
+      <c r="B84" s="131" t="s">
+        <v>104</v>
+      </c>
+      <c r="C84" s="132"/>
+      <c r="D84" s="137" t="s">
+        <v>109</v>
+      </c>
+      <c r="E84" s="138"/>
+      <c r="F84" s="143" t="s">
+        <v>110</v>
+      </c>
+      <c r="G84" s="144"/>
+      <c r="H84" s="149" t="s">
+        <v>9</v>
+      </c>
+      <c r="I84" s="150"/>
+      <c r="J84" s="52"/>
+      <c r="K84" s="151"/>
     </row>
     <row r="85" spans="1:11" s="58" customFormat="1">
-      <c r="A85" s="2"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
+      <c r="A85" s="128" t="s">
+        <v>41</v>
+      </c>
+      <c r="B85" s="133"/>
+      <c r="C85" s="134"/>
+      <c r="D85" s="139"/>
+      <c r="E85" s="140"/>
+      <c r="F85" s="145"/>
+      <c r="G85" s="146"/>
+      <c r="H85" s="128" t="s">
+        <v>42</v>
+      </c>
+      <c r="I85" s="128" t="s">
+        <v>43</v>
+      </c>
+      <c r="J85" s="128" t="s">
+        <v>44</v>
+      </c>
+      <c r="K85" s="152"/>
     </row>
     <row r="86" spans="1:11" s="58" customFormat="1">
-      <c r="A86" s="2"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
+      <c r="A86" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="133"/>
+      <c r="C86" s="134"/>
+      <c r="D86" s="139"/>
+      <c r="E86" s="140"/>
+      <c r="F86" s="145"/>
+      <c r="G86" s="146"/>
+      <c r="H86" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I86" s="50"/>
+      <c r="J86" s="48"/>
+      <c r="K86" s="152"/>
     </row>
     <row r="87" spans="1:11" s="58" customFormat="1">
-      <c r="A87" s="2"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
+      <c r="A87" s="128" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87" s="133"/>
+      <c r="C87" s="134"/>
+      <c r="D87" s="139"/>
+      <c r="E87" s="140"/>
+      <c r="F87" s="145"/>
+      <c r="G87" s="146"/>
+      <c r="H87" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="I87" s="128" t="s">
+        <v>47</v>
+      </c>
+      <c r="J87" s="128"/>
+      <c r="K87" s="152"/>
     </row>
     <row r="88" spans="1:11" s="58" customFormat="1">
-      <c r="A88" s="2"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
+      <c r="A88" s="51">
+        <v>13</v>
+      </c>
+      <c r="B88" s="135"/>
+      <c r="C88" s="136"/>
+      <c r="D88" s="141"/>
+      <c r="E88" s="142"/>
+      <c r="F88" s="147"/>
+      <c r="G88" s="148"/>
+      <c r="H88" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I88" s="50"/>
+      <c r="J88" s="48"/>
+      <c r="K88" s="153"/>
     </row>
     <row r="89" spans="1:11" s="58" customFormat="1">
-      <c r="A89" s="2"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
+      <c r="A89" s="128" t="s">
+        <v>34</v>
+      </c>
+      <c r="B89" s="156" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" s="157"/>
+      <c r="D89" s="156" t="s">
+        <v>36</v>
+      </c>
+      <c r="E89" s="157"/>
+      <c r="F89" s="156" t="s">
+        <v>37</v>
+      </c>
+      <c r="G89" s="157"/>
+      <c r="H89" s="158" t="s">
+        <v>38</v>
+      </c>
+      <c r="I89" s="158"/>
+      <c r="J89" s="128" t="s">
+        <v>39</v>
+      </c>
+      <c r="K89" s="127" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="90" spans="1:11" s="58" customFormat="1">
-      <c r="A90" s="2"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
+      <c r="A90" s="48">
+        <v>14</v>
+      </c>
+      <c r="B90" s="131" t="s">
+        <v>105</v>
+      </c>
+      <c r="C90" s="132"/>
+      <c r="D90" s="137" t="s">
+        <v>111</v>
+      </c>
+      <c r="E90" s="138"/>
+      <c r="F90" s="143" t="s">
+        <v>112</v>
+      </c>
+      <c r="G90" s="144"/>
+      <c r="H90" s="149" t="s">
+        <v>9</v>
+      </c>
+      <c r="I90" s="150"/>
+      <c r="J90" s="52"/>
+      <c r="K90" s="151"/>
     </row>
     <row r="91" spans="1:11" s="58" customFormat="1">
-      <c r="A91" s="2"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
+      <c r="A91" s="128" t="s">
+        <v>41</v>
+      </c>
+      <c r="B91" s="133"/>
+      <c r="C91" s="134"/>
+      <c r="D91" s="139"/>
+      <c r="E91" s="140"/>
+      <c r="F91" s="145"/>
+      <c r="G91" s="146"/>
+      <c r="H91" s="128" t="s">
+        <v>42</v>
+      </c>
+      <c r="I91" s="128" t="s">
+        <v>43</v>
+      </c>
+      <c r="J91" s="128" t="s">
+        <v>44</v>
+      </c>
+      <c r="K91" s="152"/>
     </row>
     <row r="92" spans="1:11" s="58" customFormat="1">
-      <c r="A92" s="2"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
+      <c r="A92" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B92" s="133"/>
+      <c r="C92" s="134"/>
+      <c r="D92" s="139"/>
+      <c r="E92" s="140"/>
+      <c r="F92" s="145"/>
+      <c r="G92" s="146"/>
+      <c r="H92" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I92" s="50"/>
+      <c r="J92" s="48"/>
+      <c r="K92" s="152"/>
     </row>
     <row r="93" spans="1:11" s="58" customFormat="1">
-      <c r="A93" s="2"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
+      <c r="A93" s="128" t="s">
+        <v>45</v>
+      </c>
+      <c r="B93" s="133"/>
+      <c r="C93" s="134"/>
+      <c r="D93" s="139"/>
+      <c r="E93" s="140"/>
+      <c r="F93" s="145"/>
+      <c r="G93" s="146"/>
+      <c r="H93" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="I93" s="128" t="s">
+        <v>47</v>
+      </c>
+      <c r="J93" s="128"/>
+      <c r="K93" s="152"/>
     </row>
     <row r="94" spans="1:11" s="58" customFormat="1">
-      <c r="A94" s="2"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
+      <c r="A94" s="51">
+        <v>14</v>
+      </c>
+      <c r="B94" s="135"/>
+      <c r="C94" s="136"/>
+      <c r="D94" s="141"/>
+      <c r="E94" s="142"/>
+      <c r="F94" s="147"/>
+      <c r="G94" s="148"/>
+      <c r="H94" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I94" s="50"/>
+      <c r="J94" s="48"/>
+      <c r="K94" s="153"/>
     </row>
     <row r="95" spans="1:11" s="58" customFormat="1">
       <c r="A95" s="2"/>
@@ -4722,27 +4892,93 @@
       <c r="K101" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="103">
-    <mergeCell ref="B72:C76"/>
-    <mergeCell ref="D72:E76"/>
-    <mergeCell ref="F72:G76"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="K72:K76"/>
-    <mergeCell ref="B70:K70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="B46:C50"/>
-    <mergeCell ref="D46:E50"/>
-    <mergeCell ref="F46:G50"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="K46:K50"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
+  <mergeCells count="130">
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="B90:C94"/>
+    <mergeCell ref="D90:E94"/>
+    <mergeCell ref="F90:G94"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="K90:K94"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="B84:C88"/>
+    <mergeCell ref="D84:E88"/>
+    <mergeCell ref="F84:G88"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="K84:K88"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="B78:C82"/>
+    <mergeCell ref="D78:E82"/>
+    <mergeCell ref="F78:G82"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="B65:C69"/>
+    <mergeCell ref="D65:E69"/>
+    <mergeCell ref="F65:G69"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="K65:K69"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B59:C63"/>
+    <mergeCell ref="D59:E63"/>
+    <mergeCell ref="F59:G63"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="K59:K63"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B53:C57"/>
+    <mergeCell ref="D53:E57"/>
+    <mergeCell ref="F53:G57"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:K57"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="F21:G25"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="F28:G32"/>
+    <mergeCell ref="K28:K32"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:C38"/>
+    <mergeCell ref="D28:E32"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="F34:G38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:G39"/>
@@ -4767,65 +5003,26 @@
     <mergeCell ref="F9:G13"/>
     <mergeCell ref="F15:G19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="K34:K38"/>
-    <mergeCell ref="F28:G32"/>
-    <mergeCell ref="K28:K32"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B34:C38"/>
-    <mergeCell ref="D28:E32"/>
-    <mergeCell ref="D34:E38"/>
-    <mergeCell ref="F34:G38"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="B28:C32"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:E25"/>
-    <mergeCell ref="F21:G25"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="B53:C57"/>
-    <mergeCell ref="D53:E57"/>
-    <mergeCell ref="F53:G57"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="K53:K57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="B59:C63"/>
-    <mergeCell ref="D59:E63"/>
-    <mergeCell ref="F59:G63"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="K59:K63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="B65:C69"/>
-    <mergeCell ref="D65:E69"/>
-    <mergeCell ref="F65:G69"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="K65:K69"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:E50"/>
+    <mergeCell ref="F46:G50"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="K46:K50"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B72:C76"/>
+    <mergeCell ref="D72:E76"/>
+    <mergeCell ref="F72:G76"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="K72:K76"/>
+    <mergeCell ref="B70:K70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H34:I34">

</xml_diff>

<commit_message>
Add DangBai test case
</commit_message>
<xml_diff>
--- a/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$157</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$151</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="141">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -440,6 +440,36 @@
   </si>
   <si>
     <t>Hệ thống hiển thị thông báo thành công và quay lại trang xem chi tiết nhà hàng</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>Đăng bài viết</t>
+  </si>
+  <si>
+    <t>6-1</t>
+  </si>
+  <si>
+    <t>6-2</t>
+  </si>
+  <si>
+    <t>DangBai_01</t>
+  </si>
+  <si>
+    <t>Kiểm tra người dùng có nhập đầy đủ các trường yêu cầu không</t>
+  </si>
+  <si>
+    <t>Nếu chưa nhập đủ hệ thống thông báo cho người dùng: chưa nhập dữ liệu hoặc vị trí còn thiếu ,yêu cầu người dùng nhập lại</t>
+  </si>
+  <si>
+    <t>DangBai_02</t>
+  </si>
+  <si>
+    <t>Kiểm tra khi người dùng nhập sai định dạng dữ liệu</t>
+  </si>
+  <si>
+    <t>Hệ thống thông báo lỗi cho người dùng,trường sai định dạng và nhập lại</t>
   </si>
 </sst>
 </file>
@@ -938,7 +968,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1248,6 +1278,12 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1345,6 +1381,51 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1362,51 +1443,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1517,7 +1553,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1984,13 +2020,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="131" t="s">
+      <c r="O6" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="131"/>
-      <c r="Q6" s="131"/>
-      <c r="R6" s="131"/>
-      <c r="S6" s="131"/>
+      <c r="P6" s="133"/>
+      <c r="Q6" s="133"/>
+      <c r="R6" s="133"/>
+      <c r="S6" s="133"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -2000,11 +2036,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="131"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="131"/>
-      <c r="R7" s="131"/>
-      <c r="S7" s="131"/>
+      <c r="O7" s="133"/>
+      <c r="P7" s="133"/>
+      <c r="Q7" s="133"/>
+      <c r="R7" s="133"/>
+      <c r="S7" s="133"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -2059,12 +2095,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="132">
+      <c r="E11" s="134">
         <f ca="1">TODAY()</f>
-        <v>43430</v>
-      </c>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
+        <v>43431</v>
+      </c>
+      <c r="F11" s="134"/>
+      <c r="G11" s="134"/>
       <c r="H11" s="71"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -2922,10 +2958,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K119"/>
+  <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A82" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A115" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2956,8 +2992,8 @@
         <v>22</v>
       </c>
       <c r="I1" s="99">
-        <f>COUNTIF(H1:H767,"OK")</f>
-        <v>10</v>
+        <f>COUNTIF(H1:H761,"OK")</f>
+        <v>12</v>
       </c>
       <c r="J1" s="81" t="s">
         <v>23</v>
@@ -2980,7 +3016,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="100">
-        <f>COUNTIF(H2:H768,"Not OK")</f>
+        <f>COUNTIF(H2:H762,"Not OK")</f>
         <v>8</v>
       </c>
       <c r="J2" s="88" t="s">
@@ -3004,7 +3040,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="101">
-        <f>COUNTIF(H2:H768,"Untested")</f>
+        <f>COUNTIF(H2:H762,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="88" t="s">
@@ -3024,8 +3060,8 @@
       </c>
       <c r="H4" s="84"/>
       <c r="I4" s="100">
-        <f>COUNTIF(H3:H769,"Result")</f>
-        <v>18</v>
+        <f>COUNTIF(H3:H763,"Result")</f>
+        <v>20</v>
       </c>
       <c r="J4" s="88"/>
       <c r="K4" s="89"/>
@@ -3060,39 +3096,39 @@
       <c r="A7" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="170" t="s">
+      <c r="B7" s="166" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="170"/>
-      <c r="H7" s="170"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="170"/>
-      <c r="K7" s="170"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
+      <c r="G7" s="166"/>
+      <c r="H7" s="166"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="133" t="s">
+      <c r="B8" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="134"/>
-      <c r="D8" s="133" t="s">
+      <c r="C8" s="136"/>
+      <c r="D8" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="134"/>
-      <c r="F8" s="133" t="s">
+      <c r="E8" s="136"/>
+      <c r="F8" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="134"/>
-      <c r="H8" s="171" t="s">
+      <c r="G8" s="136"/>
+      <c r="H8" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="171"/>
+      <c r="I8" s="173"/>
       <c r="J8" s="116" t="s">
         <v>39</v>
       </c>
@@ -3104,35 +3140,35 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="142" t="s">
+      <c r="C9" s="139"/>
+      <c r="D9" s="144" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="172" t="s">
+      <c r="E9" s="145"/>
+      <c r="F9" s="174" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="173"/>
-      <c r="H9" s="161" t="s">
+      <c r="G9" s="175"/>
+      <c r="H9" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="162"/>
+      <c r="I9" s="164"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="156"/>
+      <c r="K9" s="158"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="138"/>
-      <c r="C10" s="139"/>
-      <c r="D10" s="144"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="174"/>
-      <c r="G10" s="175"/>
+      <c r="B10" s="140"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="146"/>
+      <c r="E10" s="147"/>
+      <c r="F10" s="176"/>
+      <c r="G10" s="177"/>
       <c r="H10" s="115" t="s">
         <v>42</v>
       </c>
@@ -3142,35 +3178,35 @@
       <c r="J10" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="157"/>
+      <c r="K10" s="159"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="139"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="174"/>
-      <c r="G11" s="175"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="146"/>
+      <c r="E11" s="147"/>
+      <c r="F11" s="176"/>
+      <c r="G11" s="177"/>
       <c r="H11" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="157"/>
+      <c r="K11" s="159"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="174"/>
-      <c r="G12" s="175"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="176"/>
+      <c r="G12" s="177"/>
       <c r="H12" s="115" t="s">
         <v>46</v>
       </c>
@@ -3178,45 +3214,45 @@
         <v>47</v>
       </c>
       <c r="J12" s="115"/>
-      <c r="K12" s="157"/>
+      <c r="K12" s="159"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>1</v>
       </c>
-      <c r="B13" s="140"/>
-      <c r="C13" s="141"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="147"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="177"/>
+      <c r="B13" s="142"/>
+      <c r="C13" s="143"/>
+      <c r="D13" s="148"/>
+      <c r="E13" s="149"/>
+      <c r="F13" s="178"/>
+      <c r="G13" s="179"/>
       <c r="H13" s="53">
         <v>43434</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="158"/>
+      <c r="K13" s="160"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="159" t="s">
+      <c r="B14" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="160"/>
-      <c r="D14" s="159" t="s">
+      <c r="C14" s="162"/>
+      <c r="D14" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="159" t="s">
+      <c r="E14" s="162"/>
+      <c r="F14" s="161" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="160"/>
-      <c r="H14" s="159" t="s">
+      <c r="G14" s="162"/>
+      <c r="H14" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="160"/>
+      <c r="I14" s="162"/>
       <c r="J14" s="119" t="s">
         <v>39</v>
       </c>
@@ -3228,35 +3264,35 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="136" t="s">
+      <c r="B15" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="137"/>
-      <c r="D15" s="142" t="s">
+      <c r="C15" s="139"/>
+      <c r="D15" s="144" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="143"/>
-      <c r="F15" s="148" t="s">
+      <c r="E15" s="145"/>
+      <c r="F15" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="149"/>
-      <c r="H15" s="161" t="s">
+      <c r="G15" s="151"/>
+      <c r="H15" s="163" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="162"/>
+      <c r="I15" s="164"/>
       <c r="J15" s="52"/>
-      <c r="K15" s="156"/>
+      <c r="K15" s="158"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="138"/>
-      <c r="C16" s="139"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="145"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="151"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="146"/>
+      <c r="E16" s="147"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="153"/>
       <c r="H16" s="119" t="s">
         <v>42</v>
       </c>
@@ -3266,35 +3302,35 @@
       <c r="J16" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="157"/>
+      <c r="K16" s="159"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="138"/>
-      <c r="C17" s="139"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="150"/>
-      <c r="G17" s="151"/>
+      <c r="B17" s="140"/>
+      <c r="C17" s="141"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="147"/>
+      <c r="F17" s="152"/>
+      <c r="G17" s="153"/>
       <c r="H17" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48"/>
-      <c r="K17" s="157"/>
+      <c r="K17" s="159"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="138"/>
-      <c r="C18" s="139"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="150"/>
-      <c r="G18" s="151"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="152"/>
+      <c r="G18" s="153"/>
       <c r="H18" s="119" t="s">
         <v>46</v>
       </c>
@@ -3302,45 +3338,45 @@
         <v>47</v>
       </c>
       <c r="J18" s="119"/>
-      <c r="K18" s="157"/>
+      <c r="K18" s="159"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>2</v>
       </c>
-      <c r="B19" s="140"/>
-      <c r="C19" s="141"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="147"/>
-      <c r="F19" s="152"/>
-      <c r="G19" s="153"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="143"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="149"/>
+      <c r="F19" s="154"/>
+      <c r="G19" s="155"/>
       <c r="H19" s="50">
         <v>43434</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="157"/>
+      <c r="K19" s="159"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="133" t="s">
+      <c r="B20" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="133" t="s">
+      <c r="C20" s="136"/>
+      <c r="D20" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="134"/>
-      <c r="F20" s="133" t="s">
+      <c r="E20" s="136"/>
+      <c r="F20" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="134"/>
-      <c r="H20" s="171" t="s">
+      <c r="G20" s="136"/>
+      <c r="H20" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="171"/>
+      <c r="I20" s="173"/>
       <c r="J20" s="120" t="s">
         <v>39</v>
       </c>
@@ -3352,35 +3388,35 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="138" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="137"/>
-      <c r="D21" s="142" t="s">
+      <c r="C21" s="139"/>
+      <c r="D21" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="143"/>
-      <c r="F21" s="163" t="s">
+      <c r="E21" s="145"/>
+      <c r="F21" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="164"/>
-      <c r="H21" s="161" t="s">
+      <c r="G21" s="181"/>
+      <c r="H21" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="162"/>
+      <c r="I21" s="164"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="156"/>
+      <c r="K21" s="158"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="138"/>
-      <c r="C22" s="139"/>
-      <c r="D22" s="144"/>
-      <c r="E22" s="145"/>
-      <c r="F22" s="165"/>
-      <c r="G22" s="166"/>
+      <c r="B22" s="140"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="182"/>
+      <c r="G22" s="183"/>
       <c r="H22" s="118" t="s">
         <v>42</v>
       </c>
@@ -3390,35 +3426,35 @@
       <c r="J22" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="157"/>
+      <c r="K22" s="159"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="138"/>
-      <c r="C23" s="139"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="145"/>
-      <c r="F23" s="165"/>
-      <c r="G23" s="166"/>
+      <c r="B23" s="140"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="147"/>
+      <c r="F23" s="182"/>
+      <c r="G23" s="183"/>
       <c r="H23" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="157"/>
+      <c r="K23" s="159"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="138"/>
-      <c r="C24" s="139"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="165"/>
-      <c r="G24" s="166"/>
+      <c r="B24" s="140"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="146"/>
+      <c r="E24" s="147"/>
+      <c r="F24" s="182"/>
+      <c r="G24" s="183"/>
       <c r="H24" s="118" t="s">
         <v>46</v>
       </c>
@@ -3426,62 +3462,62 @@
         <v>47</v>
       </c>
       <c r="J24" s="118"/>
-      <c r="K24" s="157"/>
+      <c r="K24" s="159"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>3</v>
       </c>
-      <c r="B25" s="140"/>
-      <c r="C25" s="141"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="147"/>
-      <c r="F25" s="167"/>
-      <c r="G25" s="168"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="148"/>
+      <c r="E25" s="149"/>
+      <c r="F25" s="184"/>
+      <c r="G25" s="185"/>
       <c r="H25" s="53">
         <v>43434</v>
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="54"/>
-      <c r="K25" s="158"/>
+      <c r="K25" s="160"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="169" t="s">
+      <c r="B26" s="165" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="169"/>
-      <c r="D26" s="170"/>
-      <c r="E26" s="170"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="170"/>
+      <c r="C26" s="165"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
+      <c r="H26" s="166"/>
+      <c r="I26" s="166"/>
+      <c r="J26" s="166"/>
+      <c r="K26" s="166"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="133" t="s">
+      <c r="B27" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="134"/>
-      <c r="D27" s="133" t="s">
+      <c r="C27" s="136"/>
+      <c r="D27" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="134"/>
-      <c r="F27" s="133" t="s">
+      <c r="E27" s="136"/>
+      <c r="F27" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135" t="s">
+      <c r="G27" s="136"/>
+      <c r="H27" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="135"/>
+      <c r="I27" s="137"/>
       <c r="J27" s="115" t="s">
         <v>39</v>
       </c>
@@ -3493,35 +3529,35 @@
       <c r="A28" s="48">
         <v>4</v>
       </c>
-      <c r="B28" s="136" t="s">
+      <c r="B28" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="137"/>
-      <c r="D28" s="142" t="s">
+      <c r="C28" s="139"/>
+      <c r="D28" s="144" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="143"/>
-      <c r="F28" s="148" t="s">
+      <c r="E28" s="145"/>
+      <c r="F28" s="150" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="149"/>
-      <c r="H28" s="154" t="s">
+      <c r="G28" s="151"/>
+      <c r="H28" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="155"/>
+      <c r="I28" s="157"/>
       <c r="J28" s="52"/>
-      <c r="K28" s="156"/>
+      <c r="K28" s="158"/>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="138"/>
-      <c r="C29" s="139"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="145"/>
-      <c r="F29" s="150"/>
-      <c r="G29" s="151"/>
+      <c r="B29" s="140"/>
+      <c r="C29" s="141"/>
+      <c r="D29" s="146"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="153"/>
       <c r="H29" s="115" t="s">
         <v>42</v>
       </c>
@@ -3531,35 +3567,35 @@
       <c r="J29" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="157"/>
+      <c r="K29" s="159"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="138"/>
-      <c r="C30" s="139"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="151"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="146"/>
+      <c r="E30" s="147"/>
+      <c r="F30" s="152"/>
+      <c r="G30" s="153"/>
       <c r="H30" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I30" s="50"/>
       <c r="J30" s="48"/>
-      <c r="K30" s="157"/>
+      <c r="K30" s="159"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="138"/>
-      <c r="C31" s="139"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="150"/>
-      <c r="G31" s="151"/>
+      <c r="B31" s="140"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="147"/>
+      <c r="F31" s="152"/>
+      <c r="G31" s="153"/>
       <c r="H31" s="115" t="s">
         <v>46</v>
       </c>
@@ -3567,45 +3603,45 @@
         <v>47</v>
       </c>
       <c r="J31" s="115"/>
-      <c r="K31" s="157"/>
+      <c r="K31" s="159"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="51">
         <v>4</v>
       </c>
-      <c r="B32" s="140"/>
-      <c r="C32" s="141"/>
-      <c r="D32" s="146"/>
-      <c r="E32" s="147"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="153"/>
+      <c r="B32" s="142"/>
+      <c r="C32" s="143"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="149"/>
+      <c r="F32" s="154"/>
+      <c r="G32" s="155"/>
       <c r="H32" s="50">
         <v>43434</v>
       </c>
       <c r="I32" s="50"/>
       <c r="J32" s="48"/>
-      <c r="K32" s="158"/>
+      <c r="K32" s="160"/>
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A33" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="133" t="s">
+      <c r="B33" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="134"/>
-      <c r="D33" s="133" t="s">
+      <c r="C33" s="136"/>
+      <c r="D33" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="134"/>
-      <c r="F33" s="133" t="s">
+      <c r="E33" s="136"/>
+      <c r="F33" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="134"/>
-      <c r="H33" s="135" t="s">
+      <c r="G33" s="136"/>
+      <c r="H33" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="135"/>
+      <c r="I33" s="137"/>
       <c r="J33" s="115" t="s">
         <v>39</v>
       </c>
@@ -3617,35 +3653,35 @@
       <c r="A34" s="48">
         <v>5</v>
       </c>
-      <c r="B34" s="136" t="s">
+      <c r="B34" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="137"/>
-      <c r="D34" s="142" t="s">
+      <c r="C34" s="139"/>
+      <c r="D34" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="143"/>
-      <c r="F34" s="148" t="s">
+      <c r="E34" s="145"/>
+      <c r="F34" s="150" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="149"/>
-      <c r="H34" s="154" t="s">
+      <c r="G34" s="151"/>
+      <c r="H34" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="I34" s="155"/>
+      <c r="I34" s="157"/>
       <c r="J34" s="52"/>
-      <c r="K34" s="156"/>
+      <c r="K34" s="158"/>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="138"/>
-      <c r="C35" s="139"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="145"/>
-      <c r="F35" s="150"/>
-      <c r="G35" s="151"/>
+      <c r="B35" s="140"/>
+      <c r="C35" s="141"/>
+      <c r="D35" s="146"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
       <c r="H35" s="115" t="s">
         <v>42</v>
       </c>
@@ -3655,35 +3691,35 @@
       <c r="J35" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="157"/>
+      <c r="K35" s="159"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="138"/>
-      <c r="C36" s="139"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="150"/>
-      <c r="G36" s="151"/>
+      <c r="B36" s="140"/>
+      <c r="C36" s="141"/>
+      <c r="D36" s="146"/>
+      <c r="E36" s="147"/>
+      <c r="F36" s="152"/>
+      <c r="G36" s="153"/>
       <c r="H36" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I36" s="50"/>
       <c r="J36" s="48"/>
-      <c r="K36" s="157"/>
+      <c r="K36" s="159"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="138"/>
-      <c r="C37" s="139"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="150"/>
-      <c r="G37" s="151"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="146"/>
+      <c r="E37" s="147"/>
+      <c r="F37" s="152"/>
+      <c r="G37" s="153"/>
       <c r="H37" s="115" t="s">
         <v>46</v>
       </c>
@@ -3691,45 +3727,45 @@
         <v>47</v>
       </c>
       <c r="J37" s="115"/>
-      <c r="K37" s="157"/>
+      <c r="K37" s="159"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="51">
         <v>5</v>
       </c>
-      <c r="B38" s="140"/>
-      <c r="C38" s="141"/>
-      <c r="D38" s="146"/>
-      <c r="E38" s="147"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
+      <c r="B38" s="142"/>
+      <c r="C38" s="143"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="149"/>
+      <c r="F38" s="154"/>
+      <c r="G38" s="155"/>
       <c r="H38" s="50">
         <v>43434</v>
       </c>
       <c r="I38" s="50"/>
       <c r="J38" s="48"/>
-      <c r="K38" s="158"/>
+      <c r="K38" s="160"/>
     </row>
     <row r="39" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A39" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="133" t="s">
+      <c r="B39" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="134"/>
-      <c r="D39" s="133" t="s">
+      <c r="C39" s="136"/>
+      <c r="D39" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="134"/>
-      <c r="F39" s="133" t="s">
+      <c r="E39" s="136"/>
+      <c r="F39" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="134"/>
-      <c r="H39" s="135" t="s">
+      <c r="G39" s="136"/>
+      <c r="H39" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="135"/>
+      <c r="I39" s="137"/>
       <c r="J39" s="121" t="s">
         <v>39</v>
       </c>
@@ -3741,35 +3777,35 @@
       <c r="A40" s="48">
         <v>6</v>
       </c>
-      <c r="B40" s="136" t="s">
+      <c r="B40" s="138" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="137"/>
-      <c r="D40" s="142" t="s">
+      <c r="C40" s="139"/>
+      <c r="D40" s="144" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="143"/>
-      <c r="F40" s="148" t="s">
+      <c r="E40" s="145"/>
+      <c r="F40" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="149"/>
-      <c r="H40" s="154" t="s">
+      <c r="G40" s="151"/>
+      <c r="H40" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="155"/>
+      <c r="I40" s="157"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="156"/>
+      <c r="K40" s="158"/>
     </row>
     <row r="41" spans="1:11" ht="10.5" customHeight="1">
       <c r="A41" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="138"/>
-      <c r="C41" s="139"/>
-      <c r="D41" s="144"/>
-      <c r="E41" s="145"/>
-      <c r="F41" s="150"/>
-      <c r="G41" s="151"/>
+      <c r="B41" s="140"/>
+      <c r="C41" s="141"/>
+      <c r="D41" s="146"/>
+      <c r="E41" s="147"/>
+      <c r="F41" s="152"/>
+      <c r="G41" s="153"/>
       <c r="H41" s="121" t="s">
         <v>42</v>
       </c>
@@ -3779,35 +3815,35 @@
       <c r="J41" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="157"/>
+      <c r="K41" s="159"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="138"/>
-      <c r="C42" s="139"/>
-      <c r="D42" s="144"/>
-      <c r="E42" s="145"/>
-      <c r="F42" s="150"/>
-      <c r="G42" s="151"/>
+      <c r="B42" s="140"/>
+      <c r="C42" s="141"/>
+      <c r="D42" s="146"/>
+      <c r="E42" s="147"/>
+      <c r="F42" s="152"/>
+      <c r="G42" s="153"/>
       <c r="H42" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I42" s="50"/>
       <c r="J42" s="48"/>
-      <c r="K42" s="157"/>
+      <c r="K42" s="159"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="138"/>
-      <c r="C43" s="139"/>
-      <c r="D43" s="144"/>
-      <c r="E43" s="145"/>
-      <c r="F43" s="150"/>
-      <c r="G43" s="151"/>
+      <c r="B43" s="140"/>
+      <c r="C43" s="141"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="147"/>
+      <c r="F43" s="152"/>
+      <c r="G43" s="153"/>
       <c r="H43" s="121" t="s">
         <v>46</v>
       </c>
@@ -3815,45 +3851,45 @@
         <v>47</v>
       </c>
       <c r="J43" s="121"/>
-      <c r="K43" s="157"/>
+      <c r="K43" s="159"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="51">
         <v>6</v>
       </c>
-      <c r="B44" s="140"/>
-      <c r="C44" s="141"/>
-      <c r="D44" s="146"/>
-      <c r="E44" s="147"/>
-      <c r="F44" s="152"/>
-      <c r="G44" s="153"/>
+      <c r="B44" s="142"/>
+      <c r="C44" s="143"/>
+      <c r="D44" s="148"/>
+      <c r="E44" s="149"/>
+      <c r="F44" s="154"/>
+      <c r="G44" s="155"/>
       <c r="H44" s="50">
         <v>43434</v>
       </c>
       <c r="I44" s="50"/>
       <c r="J44" s="48"/>
-      <c r="K44" s="158"/>
+      <c r="K44" s="160"/>
     </row>
     <row r="45" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A45" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="133" t="s">
+      <c r="B45" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="134"/>
-      <c r="D45" s="133" t="s">
+      <c r="C45" s="136"/>
+      <c r="D45" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="134"/>
-      <c r="F45" s="133" t="s">
+      <c r="E45" s="136"/>
+      <c r="F45" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="134"/>
-      <c r="H45" s="135" t="s">
+      <c r="G45" s="136"/>
+      <c r="H45" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="135"/>
+      <c r="I45" s="137"/>
       <c r="J45" s="121" t="s">
         <v>39</v>
       </c>
@@ -3865,35 +3901,35 @@
       <c r="A46" s="48">
         <v>7</v>
       </c>
-      <c r="B46" s="136" t="s">
+      <c r="B46" s="138" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="137"/>
-      <c r="D46" s="142" t="s">
+      <c r="C46" s="139"/>
+      <c r="D46" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="143"/>
-      <c r="F46" s="178" t="s">
+      <c r="E46" s="145"/>
+      <c r="F46" s="167" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="179"/>
-      <c r="H46" s="154" t="s">
+      <c r="G46" s="168"/>
+      <c r="H46" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="I46" s="155"/>
+      <c r="I46" s="157"/>
       <c r="J46" s="52"/>
-      <c r="K46" s="156"/>
+      <c r="K46" s="158"/>
     </row>
     <row r="47" spans="1:11" ht="10.5" customHeight="1">
       <c r="A47" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="138"/>
-      <c r="C47" s="139"/>
-      <c r="D47" s="144"/>
-      <c r="E47" s="145"/>
-      <c r="F47" s="180"/>
-      <c r="G47" s="181"/>
+      <c r="B47" s="140"/>
+      <c r="C47" s="141"/>
+      <c r="D47" s="146"/>
+      <c r="E47" s="147"/>
+      <c r="F47" s="169"/>
+      <c r="G47" s="170"/>
       <c r="H47" s="121" t="s">
         <v>42</v>
       </c>
@@ -3903,35 +3939,35 @@
       <c r="J47" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="K47" s="157"/>
+      <c r="K47" s="159"/>
     </row>
     <row r="48" spans="1:11" ht="10.5" customHeight="1">
       <c r="A48" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="138"/>
-      <c r="C48" s="139"/>
-      <c r="D48" s="144"/>
-      <c r="E48" s="145"/>
-      <c r="F48" s="180"/>
-      <c r="G48" s="181"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="141"/>
+      <c r="D48" s="146"/>
+      <c r="E48" s="147"/>
+      <c r="F48" s="169"/>
+      <c r="G48" s="170"/>
       <c r="H48" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I48" s="50"/>
       <c r="J48" s="48"/>
-      <c r="K48" s="157"/>
+      <c r="K48" s="159"/>
     </row>
     <row r="49" spans="1:11" ht="10.5" customHeight="1">
       <c r="A49" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="138"/>
-      <c r="C49" s="139"/>
-      <c r="D49" s="144"/>
-      <c r="E49" s="145"/>
-      <c r="F49" s="180"/>
-      <c r="G49" s="181"/>
+      <c r="B49" s="140"/>
+      <c r="C49" s="141"/>
+      <c r="D49" s="146"/>
+      <c r="E49" s="147"/>
+      <c r="F49" s="169"/>
+      <c r="G49" s="170"/>
       <c r="H49" s="121" t="s">
         <v>46</v>
       </c>
@@ -3939,62 +3975,62 @@
         <v>47</v>
       </c>
       <c r="J49" s="121"/>
-      <c r="K49" s="157"/>
+      <c r="K49" s="159"/>
     </row>
     <row r="50" spans="1:11" ht="10.5" customHeight="1">
       <c r="A50" s="51">
         <v>7</v>
       </c>
-      <c r="B50" s="140"/>
-      <c r="C50" s="141"/>
-      <c r="D50" s="146"/>
-      <c r="E50" s="147"/>
-      <c r="F50" s="182"/>
-      <c r="G50" s="183"/>
+      <c r="B50" s="142"/>
+      <c r="C50" s="143"/>
+      <c r="D50" s="148"/>
+      <c r="E50" s="149"/>
+      <c r="F50" s="171"/>
+      <c r="G50" s="172"/>
       <c r="H50" s="50">
         <v>43434</v>
       </c>
       <c r="I50" s="50"/>
       <c r="J50" s="48"/>
-      <c r="K50" s="158"/>
+      <c r="K50" s="160"/>
     </row>
     <row r="51" spans="1:11" s="58" customFormat="1">
       <c r="A51" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="169" t="s">
+      <c r="B51" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="169"/>
-      <c r="D51" s="170"/>
-      <c r="E51" s="170"/>
-      <c r="F51" s="170"/>
-      <c r="G51" s="170"/>
-      <c r="H51" s="170"/>
-      <c r="I51" s="170"/>
-      <c r="J51" s="170"/>
-      <c r="K51" s="170"/>
+      <c r="C51" s="165"/>
+      <c r="D51" s="166"/>
+      <c r="E51" s="166"/>
+      <c r="F51" s="166"/>
+      <c r="G51" s="166"/>
+      <c r="H51" s="166"/>
+      <c r="I51" s="166"/>
+      <c r="J51" s="166"/>
+      <c r="K51" s="166"/>
     </row>
     <row r="52" spans="1:11" s="58" customFormat="1">
       <c r="A52" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="133" t="s">
+      <c r="B52" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="134"/>
-      <c r="D52" s="133" t="s">
+      <c r="C52" s="136"/>
+      <c r="D52" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="134"/>
-      <c r="F52" s="133" t="s">
+      <c r="E52" s="136"/>
+      <c r="F52" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G52" s="134"/>
-      <c r="H52" s="135" t="s">
+      <c r="G52" s="136"/>
+      <c r="H52" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I52" s="135"/>
+      <c r="I52" s="137"/>
       <c r="J52" s="124" t="s">
         <v>39</v>
       </c>
@@ -4006,35 +4042,35 @@
       <c r="A53" s="48">
         <v>8</v>
       </c>
-      <c r="B53" s="136" t="s">
+      <c r="B53" s="138" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="137"/>
-      <c r="D53" s="142" t="s">
+      <c r="C53" s="139"/>
+      <c r="D53" s="144" t="s">
         <v>89</v>
       </c>
-      <c r="E53" s="143"/>
-      <c r="F53" s="148" t="s">
+      <c r="E53" s="145"/>
+      <c r="F53" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="G53" s="149"/>
-      <c r="H53" s="154" t="s">
+      <c r="G53" s="151"/>
+      <c r="H53" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I53" s="155"/>
+      <c r="I53" s="157"/>
       <c r="J53" s="52"/>
-      <c r="K53" s="156"/>
+      <c r="K53" s="158"/>
     </row>
     <row r="54" spans="1:11" s="58" customFormat="1">
       <c r="A54" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="138"/>
-      <c r="C54" s="139"/>
-      <c r="D54" s="144"/>
-      <c r="E54" s="145"/>
-      <c r="F54" s="150"/>
-      <c r="G54" s="151"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="141"/>
+      <c r="D54" s="146"/>
+      <c r="E54" s="147"/>
+      <c r="F54" s="152"/>
+      <c r="G54" s="153"/>
       <c r="H54" s="124" t="s">
         <v>42</v>
       </c>
@@ -4044,35 +4080,35 @@
       <c r="J54" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K54" s="157"/>
+      <c r="K54" s="159"/>
     </row>
     <row r="55" spans="1:11" s="58" customFormat="1">
       <c r="A55" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="138"/>
-      <c r="C55" s="139"/>
-      <c r="D55" s="144"/>
-      <c r="E55" s="145"/>
-      <c r="F55" s="150"/>
-      <c r="G55" s="151"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="141"/>
+      <c r="D55" s="146"/>
+      <c r="E55" s="147"/>
+      <c r="F55" s="152"/>
+      <c r="G55" s="153"/>
       <c r="H55" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I55" s="50"/>
       <c r="J55" s="48"/>
-      <c r="K55" s="157"/>
+      <c r="K55" s="159"/>
     </row>
     <row r="56" spans="1:11" s="58" customFormat="1">
       <c r="A56" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="138"/>
-      <c r="C56" s="139"/>
-      <c r="D56" s="144"/>
-      <c r="E56" s="145"/>
-      <c r="F56" s="150"/>
-      <c r="G56" s="151"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="141"/>
+      <c r="D56" s="146"/>
+      <c r="E56" s="147"/>
+      <c r="F56" s="152"/>
+      <c r="G56" s="153"/>
       <c r="H56" s="124" t="s">
         <v>46</v>
       </c>
@@ -4080,45 +4116,45 @@
         <v>47</v>
       </c>
       <c r="J56" s="124"/>
-      <c r="K56" s="157"/>
+      <c r="K56" s="159"/>
     </row>
     <row r="57" spans="1:11" s="58" customFormat="1">
       <c r="A57" s="51">
         <v>8</v>
       </c>
-      <c r="B57" s="140"/>
-      <c r="C57" s="141"/>
-      <c r="D57" s="146"/>
-      <c r="E57" s="147"/>
-      <c r="F57" s="152"/>
-      <c r="G57" s="153"/>
+      <c r="B57" s="142"/>
+      <c r="C57" s="143"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="149"/>
+      <c r="F57" s="154"/>
+      <c r="G57" s="155"/>
       <c r="H57" s="50">
         <v>43434</v>
       </c>
       <c r="I57" s="50"/>
       <c r="J57" s="48"/>
-      <c r="K57" s="158"/>
+      <c r="K57" s="160"/>
     </row>
     <row r="58" spans="1:11" s="58" customFormat="1">
       <c r="A58" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="133" t="s">
+      <c r="B58" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="134"/>
-      <c r="D58" s="133" t="s">
+      <c r="C58" s="136"/>
+      <c r="D58" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="134"/>
-      <c r="F58" s="133" t="s">
+      <c r="E58" s="136"/>
+      <c r="F58" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G58" s="134"/>
-      <c r="H58" s="135" t="s">
+      <c r="G58" s="136"/>
+      <c r="H58" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I58" s="135"/>
+      <c r="I58" s="137"/>
       <c r="J58" s="124" t="s">
         <v>39</v>
       </c>
@@ -4130,35 +4166,35 @@
       <c r="A59" s="48">
         <v>9</v>
       </c>
-      <c r="B59" s="136" t="s">
+      <c r="B59" s="138" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="137"/>
-      <c r="D59" s="142" t="s">
+      <c r="C59" s="139"/>
+      <c r="D59" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="143"/>
-      <c r="F59" s="148" t="s">
+      <c r="E59" s="145"/>
+      <c r="F59" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="G59" s="149"/>
-      <c r="H59" s="154" t="s">
+      <c r="G59" s="151"/>
+      <c r="H59" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="I59" s="155"/>
+      <c r="I59" s="157"/>
       <c r="J59" s="52"/>
-      <c r="K59" s="156"/>
+      <c r="K59" s="158"/>
     </row>
     <row r="60" spans="1:11" s="58" customFormat="1">
       <c r="A60" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="138"/>
-      <c r="C60" s="139"/>
-      <c r="D60" s="144"/>
-      <c r="E60" s="145"/>
-      <c r="F60" s="150"/>
-      <c r="G60" s="151"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="141"/>
+      <c r="D60" s="146"/>
+      <c r="E60" s="147"/>
+      <c r="F60" s="152"/>
+      <c r="G60" s="153"/>
       <c r="H60" s="124" t="s">
         <v>42</v>
       </c>
@@ -4168,35 +4204,35 @@
       <c r="J60" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K60" s="157"/>
+      <c r="K60" s="159"/>
     </row>
     <row r="61" spans="1:11" s="58" customFormat="1">
       <c r="A61" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B61" s="138"/>
-      <c r="C61" s="139"/>
-      <c r="D61" s="144"/>
-      <c r="E61" s="145"/>
-      <c r="F61" s="150"/>
-      <c r="G61" s="151"/>
+      <c r="B61" s="140"/>
+      <c r="C61" s="141"/>
+      <c r="D61" s="146"/>
+      <c r="E61" s="147"/>
+      <c r="F61" s="152"/>
+      <c r="G61" s="153"/>
       <c r="H61" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I61" s="50"/>
       <c r="J61" s="48"/>
-      <c r="K61" s="157"/>
+      <c r="K61" s="159"/>
     </row>
     <row r="62" spans="1:11" s="58" customFormat="1">
       <c r="A62" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="138"/>
-      <c r="C62" s="139"/>
-      <c r="D62" s="144"/>
-      <c r="E62" s="145"/>
-      <c r="F62" s="150"/>
-      <c r="G62" s="151"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="141"/>
+      <c r="D62" s="146"/>
+      <c r="E62" s="147"/>
+      <c r="F62" s="152"/>
+      <c r="G62" s="153"/>
       <c r="H62" s="124" t="s">
         <v>46</v>
       </c>
@@ -4204,45 +4240,45 @@
         <v>47</v>
       </c>
       <c r="J62" s="124"/>
-      <c r="K62" s="157"/>
+      <c r="K62" s="159"/>
     </row>
     <row r="63" spans="1:11" s="58" customFormat="1">
       <c r="A63" s="51">
         <v>9</v>
       </c>
-      <c r="B63" s="140"/>
-      <c r="C63" s="141"/>
-      <c r="D63" s="146"/>
-      <c r="E63" s="147"/>
-      <c r="F63" s="152"/>
-      <c r="G63" s="153"/>
+      <c r="B63" s="142"/>
+      <c r="C63" s="143"/>
+      <c r="D63" s="148"/>
+      <c r="E63" s="149"/>
+      <c r="F63" s="154"/>
+      <c r="G63" s="155"/>
       <c r="H63" s="50">
         <v>43434</v>
       </c>
       <c r="I63" s="50"/>
       <c r="J63" s="48"/>
-      <c r="K63" s="158"/>
+      <c r="K63" s="160"/>
     </row>
     <row r="64" spans="1:11" s="58" customFormat="1">
       <c r="A64" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="133" t="s">
+      <c r="B64" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="134"/>
-      <c r="D64" s="133" t="s">
+      <c r="C64" s="136"/>
+      <c r="D64" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E64" s="134"/>
-      <c r="F64" s="133" t="s">
+      <c r="E64" s="136"/>
+      <c r="F64" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G64" s="134"/>
-      <c r="H64" s="135" t="s">
+      <c r="G64" s="136"/>
+      <c r="H64" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I64" s="135"/>
+      <c r="I64" s="137"/>
       <c r="J64" s="124" t="s">
         <v>39</v>
       </c>
@@ -4254,35 +4290,35 @@
       <c r="A65" s="48">
         <v>10</v>
       </c>
-      <c r="B65" s="136" t="s">
+      <c r="B65" s="138" t="s">
         <v>83</v>
       </c>
-      <c r="C65" s="137"/>
-      <c r="D65" s="142" t="s">
+      <c r="C65" s="139"/>
+      <c r="D65" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="E65" s="143"/>
-      <c r="F65" s="148" t="s">
+      <c r="E65" s="145"/>
+      <c r="F65" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="149"/>
-      <c r="H65" s="154" t="s">
+      <c r="G65" s="151"/>
+      <c r="H65" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="I65" s="155"/>
+      <c r="I65" s="157"/>
       <c r="J65" s="52"/>
-      <c r="K65" s="156"/>
+      <c r="K65" s="158"/>
     </row>
     <row r="66" spans="1:11" s="58" customFormat="1">
       <c r="A66" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="138"/>
-      <c r="C66" s="139"/>
-      <c r="D66" s="144"/>
-      <c r="E66" s="145"/>
-      <c r="F66" s="150"/>
-      <c r="G66" s="151"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="141"/>
+      <c r="D66" s="146"/>
+      <c r="E66" s="147"/>
+      <c r="F66" s="152"/>
+      <c r="G66" s="153"/>
       <c r="H66" s="124" t="s">
         <v>42</v>
       </c>
@@ -4292,35 +4328,35 @@
       <c r="J66" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K66" s="157"/>
+      <c r="K66" s="159"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B67" s="138"/>
-      <c r="C67" s="139"/>
-      <c r="D67" s="144"/>
-      <c r="E67" s="145"/>
-      <c r="F67" s="150"/>
-      <c r="G67" s="151"/>
+      <c r="B67" s="140"/>
+      <c r="C67" s="141"/>
+      <c r="D67" s="146"/>
+      <c r="E67" s="147"/>
+      <c r="F67" s="152"/>
+      <c r="G67" s="153"/>
       <c r="H67" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I67" s="50"/>
       <c r="J67" s="48"/>
-      <c r="K67" s="157"/>
+      <c r="K67" s="159"/>
     </row>
     <row r="68" spans="1:11" s="58" customFormat="1">
       <c r="A68" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="138"/>
-      <c r="C68" s="139"/>
-      <c r="D68" s="144"/>
-      <c r="E68" s="145"/>
-      <c r="F68" s="150"/>
-      <c r="G68" s="151"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="141"/>
+      <c r="D68" s="146"/>
+      <c r="E68" s="147"/>
+      <c r="F68" s="152"/>
+      <c r="G68" s="153"/>
       <c r="H68" s="124" t="s">
         <v>46</v>
       </c>
@@ -4328,62 +4364,62 @@
         <v>47</v>
       </c>
       <c r="J68" s="124"/>
-      <c r="K68" s="157"/>
+      <c r="K68" s="159"/>
     </row>
     <row r="69" spans="1:11" s="58" customFormat="1">
       <c r="A69" s="51">
         <v>10</v>
       </c>
-      <c r="B69" s="140"/>
-      <c r="C69" s="141"/>
-      <c r="D69" s="146"/>
-      <c r="E69" s="147"/>
-      <c r="F69" s="152"/>
-      <c r="G69" s="153"/>
+      <c r="B69" s="142"/>
+      <c r="C69" s="143"/>
+      <c r="D69" s="148"/>
+      <c r="E69" s="149"/>
+      <c r="F69" s="154"/>
+      <c r="G69" s="155"/>
       <c r="H69" s="50">
         <v>43434</v>
       </c>
       <c r="I69" s="50"/>
       <c r="J69" s="48"/>
-      <c r="K69" s="158"/>
+      <c r="K69" s="160"/>
     </row>
     <row r="70" spans="1:11" s="58" customFormat="1">
       <c r="A70" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="B70" s="169" t="s">
+      <c r="B70" s="165" t="s">
         <v>96</v>
       </c>
-      <c r="C70" s="169"/>
-      <c r="D70" s="170"/>
-      <c r="E70" s="170"/>
-      <c r="F70" s="170"/>
-      <c r="G70" s="170"/>
-      <c r="H70" s="170"/>
-      <c r="I70" s="170"/>
-      <c r="J70" s="170"/>
-      <c r="K70" s="170"/>
+      <c r="C70" s="165"/>
+      <c r="D70" s="166"/>
+      <c r="E70" s="166"/>
+      <c r="F70" s="166"/>
+      <c r="G70" s="166"/>
+      <c r="H70" s="166"/>
+      <c r="I70" s="166"/>
+      <c r="J70" s="166"/>
+      <c r="K70" s="166"/>
     </row>
     <row r="71" spans="1:11" s="58" customFormat="1">
       <c r="A71" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B71" s="133" t="s">
+      <c r="B71" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C71" s="134"/>
-      <c r="D71" s="133" t="s">
+      <c r="C71" s="136"/>
+      <c r="D71" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E71" s="134"/>
-      <c r="F71" s="133" t="s">
+      <c r="E71" s="136"/>
+      <c r="F71" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G71" s="134"/>
-      <c r="H71" s="135" t="s">
+      <c r="G71" s="136"/>
+      <c r="H71" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I71" s="135"/>
+      <c r="I71" s="137"/>
       <c r="J71" s="126" t="s">
         <v>39</v>
       </c>
@@ -4395,35 +4431,35 @@
       <c r="A72" s="48">
         <v>11</v>
       </c>
-      <c r="B72" s="136" t="s">
+      <c r="B72" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="C72" s="137"/>
-      <c r="D72" s="142" t="s">
+      <c r="C72" s="139"/>
+      <c r="D72" s="144" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="143"/>
-      <c r="F72" s="148" t="s">
+      <c r="E72" s="145"/>
+      <c r="F72" s="150" t="s">
         <v>107</v>
       </c>
-      <c r="G72" s="149"/>
-      <c r="H72" s="154" t="s">
+      <c r="G72" s="151"/>
+      <c r="H72" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I72" s="155"/>
+      <c r="I72" s="157"/>
       <c r="J72" s="52"/>
-      <c r="K72" s="156"/>
+      <c r="K72" s="158"/>
     </row>
     <row r="73" spans="1:11" s="58" customFormat="1">
       <c r="A73" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="138"/>
-      <c r="C73" s="139"/>
-      <c r="D73" s="144"/>
-      <c r="E73" s="145"/>
-      <c r="F73" s="150"/>
-      <c r="G73" s="151"/>
+      <c r="B73" s="140"/>
+      <c r="C73" s="141"/>
+      <c r="D73" s="146"/>
+      <c r="E73" s="147"/>
+      <c r="F73" s="152"/>
+      <c r="G73" s="153"/>
       <c r="H73" s="126" t="s">
         <v>42</v>
       </c>
@@ -4433,35 +4469,35 @@
       <c r="J73" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K73" s="157"/>
+      <c r="K73" s="159"/>
     </row>
     <row r="74" spans="1:11" s="58" customFormat="1">
       <c r="A74" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="138"/>
-      <c r="C74" s="139"/>
-      <c r="D74" s="144"/>
-      <c r="E74" s="145"/>
-      <c r="F74" s="150"/>
-      <c r="G74" s="151"/>
+      <c r="B74" s="140"/>
+      <c r="C74" s="141"/>
+      <c r="D74" s="146"/>
+      <c r="E74" s="147"/>
+      <c r="F74" s="152"/>
+      <c r="G74" s="153"/>
       <c r="H74" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I74" s="50"/>
       <c r="J74" s="48"/>
-      <c r="K74" s="157"/>
+      <c r="K74" s="159"/>
     </row>
     <row r="75" spans="1:11" s="58" customFormat="1">
       <c r="A75" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="B75" s="138"/>
-      <c r="C75" s="139"/>
-      <c r="D75" s="144"/>
-      <c r="E75" s="145"/>
-      <c r="F75" s="150"/>
-      <c r="G75" s="151"/>
+      <c r="B75" s="140"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="146"/>
+      <c r="E75" s="147"/>
+      <c r="F75" s="152"/>
+      <c r="G75" s="153"/>
       <c r="H75" s="126" t="s">
         <v>46</v>
       </c>
@@ -4469,45 +4505,45 @@
         <v>47</v>
       </c>
       <c r="J75" s="126"/>
-      <c r="K75" s="157"/>
+      <c r="K75" s="159"/>
     </row>
     <row r="76" spans="1:11" s="58" customFormat="1">
       <c r="A76" s="51">
         <v>11</v>
       </c>
-      <c r="B76" s="140"/>
-      <c r="C76" s="141"/>
-      <c r="D76" s="146"/>
-      <c r="E76" s="147"/>
-      <c r="F76" s="152"/>
-      <c r="G76" s="153"/>
+      <c r="B76" s="142"/>
+      <c r="C76" s="143"/>
+      <c r="D76" s="148"/>
+      <c r="E76" s="149"/>
+      <c r="F76" s="154"/>
+      <c r="G76" s="155"/>
       <c r="H76" s="50">
         <v>43434</v>
       </c>
       <c r="I76" s="50"/>
       <c r="J76" s="48"/>
-      <c r="K76" s="158"/>
+      <c r="K76" s="160"/>
     </row>
     <row r="77" spans="1:11" s="58" customFormat="1">
       <c r="A77" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B77" s="159" t="s">
+      <c r="B77" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="C77" s="160"/>
-      <c r="D77" s="159" t="s">
+      <c r="C77" s="162"/>
+      <c r="D77" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="E77" s="160"/>
-      <c r="F77" s="159" t="s">
+      <c r="E77" s="162"/>
+      <c r="F77" s="161" t="s">
         <v>37</v>
       </c>
-      <c r="G77" s="160"/>
-      <c r="H77" s="159" t="s">
+      <c r="G77" s="162"/>
+      <c r="H77" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I77" s="160"/>
+      <c r="I77" s="162"/>
       <c r="J77" s="119" t="s">
         <v>39</v>
       </c>
@@ -4519,35 +4555,35 @@
       <c r="A78" s="48">
         <v>12</v>
       </c>
-      <c r="B78" s="136" t="s">
+      <c r="B78" s="138" t="s">
         <v>103</v>
       </c>
-      <c r="C78" s="137"/>
-      <c r="D78" s="142" t="s">
+      <c r="C78" s="139"/>
+      <c r="D78" s="144" t="s">
         <v>99</v>
       </c>
-      <c r="E78" s="143"/>
-      <c r="F78" s="148" t="s">
+      <c r="E78" s="145"/>
+      <c r="F78" s="150" t="s">
         <v>108</v>
       </c>
-      <c r="G78" s="149"/>
-      <c r="H78" s="161" t="s">
+      <c r="G78" s="151"/>
+      <c r="H78" s="163" t="s">
         <v>10</v>
       </c>
-      <c r="I78" s="162"/>
+      <c r="I78" s="164"/>
       <c r="J78" s="52"/>
-      <c r="K78" s="156"/>
+      <c r="K78" s="158"/>
     </row>
     <row r="79" spans="1:11" s="58" customFormat="1">
       <c r="A79" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="138"/>
-      <c r="C79" s="139"/>
-      <c r="D79" s="144"/>
-      <c r="E79" s="145"/>
-      <c r="F79" s="150"/>
-      <c r="G79" s="151"/>
+      <c r="B79" s="140"/>
+      <c r="C79" s="141"/>
+      <c r="D79" s="146"/>
+      <c r="E79" s="147"/>
+      <c r="F79" s="152"/>
+      <c r="G79" s="153"/>
       <c r="H79" s="119" t="s">
         <v>42</v>
       </c>
@@ -4557,35 +4593,35 @@
       <c r="J79" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K79" s="157"/>
+      <c r="K79" s="159"/>
     </row>
     <row r="80" spans="1:11" s="58" customFormat="1">
       <c r="A80" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="138"/>
-      <c r="C80" s="139"/>
-      <c r="D80" s="144"/>
-      <c r="E80" s="145"/>
-      <c r="F80" s="150"/>
-      <c r="G80" s="151"/>
+      <c r="B80" s="140"/>
+      <c r="C80" s="141"/>
+      <c r="D80" s="146"/>
+      <c r="E80" s="147"/>
+      <c r="F80" s="152"/>
+      <c r="G80" s="153"/>
       <c r="H80" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I80" s="50"/>
       <c r="J80" s="48"/>
-      <c r="K80" s="157"/>
+      <c r="K80" s="159"/>
     </row>
     <row r="81" spans="1:11" s="58" customFormat="1">
       <c r="A81" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B81" s="138"/>
-      <c r="C81" s="139"/>
-      <c r="D81" s="144"/>
-      <c r="E81" s="145"/>
-      <c r="F81" s="150"/>
-      <c r="G81" s="151"/>
+      <c r="B81" s="140"/>
+      <c r="C81" s="141"/>
+      <c r="D81" s="146"/>
+      <c r="E81" s="147"/>
+      <c r="F81" s="152"/>
+      <c r="G81" s="153"/>
       <c r="H81" s="119" t="s">
         <v>46</v>
       </c>
@@ -4593,45 +4629,45 @@
         <v>47</v>
       </c>
       <c r="J81" s="119"/>
-      <c r="K81" s="157"/>
+      <c r="K81" s="159"/>
     </row>
     <row r="82" spans="1:11" s="58" customFormat="1">
       <c r="A82" s="51">
         <v>12</v>
       </c>
-      <c r="B82" s="140"/>
-      <c r="C82" s="141"/>
-      <c r="D82" s="146"/>
-      <c r="E82" s="147"/>
-      <c r="F82" s="152"/>
-      <c r="G82" s="153"/>
+      <c r="B82" s="142"/>
+      <c r="C82" s="143"/>
+      <c r="D82" s="148"/>
+      <c r="E82" s="149"/>
+      <c r="F82" s="154"/>
+      <c r="G82" s="155"/>
       <c r="H82" s="50">
         <v>43434</v>
       </c>
       <c r="I82" s="50"/>
       <c r="J82" s="48"/>
-      <c r="K82" s="157"/>
+      <c r="K82" s="159"/>
     </row>
     <row r="83" spans="1:11" s="58" customFormat="1">
       <c r="A83" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="B83" s="133" t="s">
+      <c r="B83" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="134"/>
-      <c r="D83" s="133" t="s">
+      <c r="C83" s="136"/>
+      <c r="D83" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E83" s="134"/>
-      <c r="F83" s="133" t="s">
+      <c r="E83" s="136"/>
+      <c r="F83" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G83" s="134"/>
-      <c r="H83" s="135" t="s">
+      <c r="G83" s="136"/>
+      <c r="H83" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I83" s="135"/>
+      <c r="I83" s="137"/>
       <c r="J83" s="128" t="s">
         <v>39</v>
       </c>
@@ -4643,35 +4679,35 @@
       <c r="A84" s="48">
         <v>13</v>
       </c>
-      <c r="B84" s="136" t="s">
+      <c r="B84" s="138" t="s">
         <v>104</v>
       </c>
-      <c r="C84" s="137"/>
-      <c r="D84" s="142" t="s">
+      <c r="C84" s="139"/>
+      <c r="D84" s="144" t="s">
         <v>109</v>
       </c>
-      <c r="E84" s="143"/>
-      <c r="F84" s="148" t="s">
+      <c r="E84" s="145"/>
+      <c r="F84" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="G84" s="149"/>
-      <c r="H84" s="154" t="s">
+      <c r="G84" s="151"/>
+      <c r="H84" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I84" s="155"/>
+      <c r="I84" s="157"/>
       <c r="J84" s="52"/>
-      <c r="K84" s="156"/>
+      <c r="K84" s="158"/>
     </row>
     <row r="85" spans="1:11" s="58" customFormat="1">
       <c r="A85" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="138"/>
-      <c r="C85" s="139"/>
-      <c r="D85" s="144"/>
-      <c r="E85" s="145"/>
-      <c r="F85" s="150"/>
-      <c r="G85" s="151"/>
+      <c r="B85" s="140"/>
+      <c r="C85" s="141"/>
+      <c r="D85" s="146"/>
+      <c r="E85" s="147"/>
+      <c r="F85" s="152"/>
+      <c r="G85" s="153"/>
       <c r="H85" s="128" t="s">
         <v>42</v>
       </c>
@@ -4681,35 +4717,35 @@
       <c r="J85" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="K85" s="157"/>
+      <c r="K85" s="159"/>
     </row>
     <row r="86" spans="1:11" s="58" customFormat="1">
       <c r="A86" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="B86" s="138"/>
-      <c r="C86" s="139"/>
-      <c r="D86" s="144"/>
-      <c r="E86" s="145"/>
-      <c r="F86" s="150"/>
-      <c r="G86" s="151"/>
+      <c r="B86" s="140"/>
+      <c r="C86" s="141"/>
+      <c r="D86" s="146"/>
+      <c r="E86" s="147"/>
+      <c r="F86" s="152"/>
+      <c r="G86" s="153"/>
       <c r="H86" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I86" s="50"/>
       <c r="J86" s="48"/>
-      <c r="K86" s="157"/>
+      <c r="K86" s="159"/>
     </row>
     <row r="87" spans="1:11" s="58" customFormat="1">
       <c r="A87" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="B87" s="138"/>
-      <c r="C87" s="139"/>
-      <c r="D87" s="144"/>
-      <c r="E87" s="145"/>
-      <c r="F87" s="150"/>
-      <c r="G87" s="151"/>
+      <c r="B87" s="140"/>
+      <c r="C87" s="141"/>
+      <c r="D87" s="146"/>
+      <c r="E87" s="147"/>
+      <c r="F87" s="152"/>
+      <c r="G87" s="153"/>
       <c r="H87" s="128" t="s">
         <v>46</v>
       </c>
@@ -4717,45 +4753,45 @@
         <v>47</v>
       </c>
       <c r="J87" s="128"/>
-      <c r="K87" s="157"/>
+      <c r="K87" s="159"/>
     </row>
     <row r="88" spans="1:11" s="58" customFormat="1">
       <c r="A88" s="51">
         <v>13</v>
       </c>
-      <c r="B88" s="140"/>
-      <c r="C88" s="141"/>
-      <c r="D88" s="146"/>
-      <c r="E88" s="147"/>
-      <c r="F88" s="152"/>
-      <c r="G88" s="153"/>
+      <c r="B88" s="142"/>
+      <c r="C88" s="143"/>
+      <c r="D88" s="148"/>
+      <c r="E88" s="149"/>
+      <c r="F88" s="154"/>
+      <c r="G88" s="155"/>
       <c r="H88" s="50">
         <v>43434</v>
       </c>
       <c r="I88" s="50"/>
       <c r="J88" s="48"/>
-      <c r="K88" s="158"/>
+      <c r="K88" s="160"/>
     </row>
     <row r="89" spans="1:11" s="58" customFormat="1">
       <c r="A89" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="B89" s="133" t="s">
+      <c r="B89" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="134"/>
-      <c r="D89" s="133" t="s">
+      <c r="C89" s="136"/>
+      <c r="D89" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E89" s="134"/>
-      <c r="F89" s="133" t="s">
+      <c r="E89" s="136"/>
+      <c r="F89" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G89" s="134"/>
-      <c r="H89" s="135" t="s">
+      <c r="G89" s="136"/>
+      <c r="H89" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I89" s="135"/>
+      <c r="I89" s="137"/>
       <c r="J89" s="128" t="s">
         <v>39</v>
       </c>
@@ -4767,35 +4803,35 @@
       <c r="A90" s="48">
         <v>14</v>
       </c>
-      <c r="B90" s="136" t="s">
+      <c r="B90" s="138" t="s">
         <v>105</v>
       </c>
-      <c r="C90" s="137"/>
-      <c r="D90" s="142" t="s">
+      <c r="C90" s="139"/>
+      <c r="D90" s="144" t="s">
         <v>111</v>
       </c>
-      <c r="E90" s="143"/>
-      <c r="F90" s="148" t="s">
+      <c r="E90" s="145"/>
+      <c r="F90" s="150" t="s">
         <v>112</v>
       </c>
-      <c r="G90" s="149"/>
-      <c r="H90" s="154" t="s">
+      <c r="G90" s="151"/>
+      <c r="H90" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I90" s="155"/>
+      <c r="I90" s="157"/>
       <c r="J90" s="52"/>
-      <c r="K90" s="156"/>
+      <c r="K90" s="158"/>
     </row>
     <row r="91" spans="1:11" s="58" customFormat="1">
       <c r="A91" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B91" s="138"/>
-      <c r="C91" s="139"/>
-      <c r="D91" s="144"/>
-      <c r="E91" s="145"/>
-      <c r="F91" s="150"/>
-      <c r="G91" s="151"/>
+      <c r="B91" s="140"/>
+      <c r="C91" s="141"/>
+      <c r="D91" s="146"/>
+      <c r="E91" s="147"/>
+      <c r="F91" s="152"/>
+      <c r="G91" s="153"/>
       <c r="H91" s="128" t="s">
         <v>42</v>
       </c>
@@ -4805,35 +4841,35 @@
       <c r="J91" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="K91" s="157"/>
+      <c r="K91" s="159"/>
     </row>
     <row r="92" spans="1:11" s="58" customFormat="1">
       <c r="A92" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B92" s="138"/>
-      <c r="C92" s="139"/>
-      <c r="D92" s="144"/>
-      <c r="E92" s="145"/>
-      <c r="F92" s="150"/>
-      <c r="G92" s="151"/>
+      <c r="B92" s="140"/>
+      <c r="C92" s="141"/>
+      <c r="D92" s="146"/>
+      <c r="E92" s="147"/>
+      <c r="F92" s="152"/>
+      <c r="G92" s="153"/>
       <c r="H92" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I92" s="50"/>
       <c r="J92" s="48"/>
-      <c r="K92" s="157"/>
+      <c r="K92" s="159"/>
     </row>
     <row r="93" spans="1:11" s="58" customFormat="1">
       <c r="A93" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="B93" s="138"/>
-      <c r="C93" s="139"/>
-      <c r="D93" s="144"/>
-      <c r="E93" s="145"/>
-      <c r="F93" s="150"/>
-      <c r="G93" s="151"/>
+      <c r="B93" s="140"/>
+      <c r="C93" s="141"/>
+      <c r="D93" s="146"/>
+      <c r="E93" s="147"/>
+      <c r="F93" s="152"/>
+      <c r="G93" s="153"/>
       <c r="H93" s="128" t="s">
         <v>46</v>
       </c>
@@ -4841,62 +4877,62 @@
         <v>47</v>
       </c>
       <c r="J93" s="128"/>
-      <c r="K93" s="157"/>
+      <c r="K93" s="159"/>
     </row>
     <row r="94" spans="1:11" s="58" customFormat="1">
       <c r="A94" s="51">
         <v>14</v>
       </c>
-      <c r="B94" s="140"/>
-      <c r="C94" s="141"/>
-      <c r="D94" s="146"/>
-      <c r="E94" s="147"/>
-      <c r="F94" s="152"/>
-      <c r="G94" s="153"/>
+      <c r="B94" s="142"/>
+      <c r="C94" s="143"/>
+      <c r="D94" s="148"/>
+      <c r="E94" s="149"/>
+      <c r="F94" s="154"/>
+      <c r="G94" s="155"/>
       <c r="H94" s="50">
         <v>43434</v>
       </c>
       <c r="I94" s="50"/>
       <c r="J94" s="48"/>
-      <c r="K94" s="158"/>
+      <c r="K94" s="160"/>
     </row>
     <row r="95" spans="1:11" s="58" customFormat="1">
       <c r="A95" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="B95" s="169" t="s">
+      <c r="B95" s="165" t="s">
         <v>114</v>
       </c>
-      <c r="C95" s="169"/>
-      <c r="D95" s="170"/>
-      <c r="E95" s="170"/>
-      <c r="F95" s="170"/>
-      <c r="G95" s="170"/>
-      <c r="H95" s="170"/>
-      <c r="I95" s="170"/>
-      <c r="J95" s="170"/>
-      <c r="K95" s="170"/>
+      <c r="C95" s="165"/>
+      <c r="D95" s="166"/>
+      <c r="E95" s="166"/>
+      <c r="F95" s="166"/>
+      <c r="G95" s="166"/>
+      <c r="H95" s="166"/>
+      <c r="I95" s="166"/>
+      <c r="J95" s="166"/>
+      <c r="K95" s="166"/>
     </row>
     <row r="96" spans="1:11" s="58" customFormat="1">
       <c r="A96" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B96" s="133" t="s">
+      <c r="B96" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C96" s="134"/>
-      <c r="D96" s="133" t="s">
+      <c r="C96" s="136"/>
+      <c r="D96" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E96" s="134"/>
-      <c r="F96" s="133" t="s">
+      <c r="E96" s="136"/>
+      <c r="F96" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G96" s="134"/>
-      <c r="H96" s="135" t="s">
+      <c r="G96" s="136"/>
+      <c r="H96" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I96" s="135"/>
+      <c r="I96" s="137"/>
       <c r="J96" s="130" t="s">
         <v>39</v>
       </c>
@@ -4908,35 +4944,35 @@
       <c r="A97" s="48">
         <v>15</v>
       </c>
-      <c r="B97" s="136" t="s">
+      <c r="B97" s="138" t="s">
         <v>119</v>
       </c>
-      <c r="C97" s="137"/>
-      <c r="D97" s="142" t="s">
+      <c r="C97" s="139"/>
+      <c r="D97" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="E97" s="143"/>
-      <c r="F97" s="148" t="s">
+      <c r="E97" s="145"/>
+      <c r="F97" s="150" t="s">
         <v>121</v>
       </c>
-      <c r="G97" s="149"/>
-      <c r="H97" s="154" t="s">
+      <c r="G97" s="151"/>
+      <c r="H97" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I97" s="155"/>
+      <c r="I97" s="157"/>
       <c r="J97" s="52"/>
-      <c r="K97" s="156"/>
+      <c r="K97" s="158"/>
     </row>
     <row r="98" spans="1:11" s="58" customFormat="1">
       <c r="A98" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B98" s="138"/>
-      <c r="C98" s="139"/>
-      <c r="D98" s="144"/>
-      <c r="E98" s="145"/>
-      <c r="F98" s="150"/>
-      <c r="G98" s="151"/>
+      <c r="B98" s="140"/>
+      <c r="C98" s="141"/>
+      <c r="D98" s="146"/>
+      <c r="E98" s="147"/>
+      <c r="F98" s="152"/>
+      <c r="G98" s="153"/>
       <c r="H98" s="130" t="s">
         <v>42</v>
       </c>
@@ -4946,35 +4982,35 @@
       <c r="J98" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="K98" s="157"/>
+      <c r="K98" s="159"/>
     </row>
     <row r="99" spans="1:11" s="58" customFormat="1">
       <c r="A99" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="B99" s="138"/>
-      <c r="C99" s="139"/>
-      <c r="D99" s="144"/>
-      <c r="E99" s="145"/>
-      <c r="F99" s="150"/>
-      <c r="G99" s="151"/>
+      <c r="B99" s="140"/>
+      <c r="C99" s="141"/>
+      <c r="D99" s="146"/>
+      <c r="E99" s="147"/>
+      <c r="F99" s="152"/>
+      <c r="G99" s="153"/>
       <c r="H99" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I99" s="50"/>
       <c r="J99" s="48"/>
-      <c r="K99" s="157"/>
+      <c r="K99" s="159"/>
     </row>
     <row r="100" spans="1:11" s="58" customFormat="1">
       <c r="A100" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B100" s="138"/>
-      <c r="C100" s="139"/>
-      <c r="D100" s="144"/>
-      <c r="E100" s="145"/>
-      <c r="F100" s="150"/>
-      <c r="G100" s="151"/>
+      <c r="B100" s="140"/>
+      <c r="C100" s="141"/>
+      <c r="D100" s="146"/>
+      <c r="E100" s="147"/>
+      <c r="F100" s="152"/>
+      <c r="G100" s="153"/>
       <c r="H100" s="130" t="s">
         <v>46</v>
       </c>
@@ -4982,45 +5018,45 @@
         <v>47</v>
       </c>
       <c r="J100" s="130"/>
-      <c r="K100" s="157"/>
+      <c r="K100" s="159"/>
     </row>
     <row r="101" spans="1:11" s="58" customFormat="1">
       <c r="A101" s="51">
         <v>15</v>
       </c>
-      <c r="B101" s="140"/>
-      <c r="C101" s="141"/>
-      <c r="D101" s="146"/>
-      <c r="E101" s="147"/>
-      <c r="F101" s="152"/>
-      <c r="G101" s="153"/>
+      <c r="B101" s="142"/>
+      <c r="C101" s="143"/>
+      <c r="D101" s="148"/>
+      <c r="E101" s="149"/>
+      <c r="F101" s="154"/>
+      <c r="G101" s="155"/>
       <c r="H101" s="50">
         <v>43434</v>
       </c>
       <c r="I101" s="50"/>
       <c r="J101" s="48"/>
-      <c r="K101" s="158"/>
+      <c r="K101" s="160"/>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B102" s="159" t="s">
+      <c r="B102" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="C102" s="160"/>
-      <c r="D102" s="159" t="s">
+      <c r="C102" s="162"/>
+      <c r="D102" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="E102" s="160"/>
-      <c r="F102" s="159" t="s">
+      <c r="E102" s="162"/>
+      <c r="F102" s="161" t="s">
         <v>37</v>
       </c>
-      <c r="G102" s="160"/>
-      <c r="H102" s="159" t="s">
+      <c r="G102" s="162"/>
+      <c r="H102" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I102" s="160"/>
+      <c r="I102" s="162"/>
       <c r="J102" s="119" t="s">
         <v>39</v>
       </c>
@@ -5032,35 +5068,35 @@
       <c r="A103" s="48">
         <v>16</v>
       </c>
-      <c r="B103" s="136" t="s">
+      <c r="B103" s="138" t="s">
         <v>122</v>
       </c>
-      <c r="C103" s="137"/>
-      <c r="D103" s="142" t="s">
+      <c r="C103" s="139"/>
+      <c r="D103" s="144" t="s">
         <v>125</v>
       </c>
-      <c r="E103" s="143"/>
-      <c r="F103" s="148" t="s">
+      <c r="E103" s="145"/>
+      <c r="F103" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="G103" s="149"/>
-      <c r="H103" s="161" t="s">
+      <c r="G103" s="151"/>
+      <c r="H103" s="163" t="s">
         <v>10</v>
       </c>
-      <c r="I103" s="162"/>
+      <c r="I103" s="164"/>
       <c r="J103" s="52"/>
-      <c r="K103" s="156"/>
+      <c r="K103" s="158"/>
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B104" s="138"/>
-      <c r="C104" s="139"/>
-      <c r="D104" s="144"/>
-      <c r="E104" s="145"/>
-      <c r="F104" s="150"/>
-      <c r="G104" s="151"/>
+      <c r="B104" s="140"/>
+      <c r="C104" s="141"/>
+      <c r="D104" s="146"/>
+      <c r="E104" s="147"/>
+      <c r="F104" s="152"/>
+      <c r="G104" s="153"/>
       <c r="H104" s="119" t="s">
         <v>42</v>
       </c>
@@ -5070,35 +5106,35 @@
       <c r="J104" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K104" s="157"/>
+      <c r="K104" s="159"/>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="B105" s="138"/>
-      <c r="C105" s="139"/>
-      <c r="D105" s="144"/>
-      <c r="E105" s="145"/>
-      <c r="F105" s="150"/>
-      <c r="G105" s="151"/>
+      <c r="B105" s="140"/>
+      <c r="C105" s="141"/>
+      <c r="D105" s="146"/>
+      <c r="E105" s="147"/>
+      <c r="F105" s="152"/>
+      <c r="G105" s="153"/>
       <c r="H105" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I105" s="50"/>
       <c r="J105" s="48"/>
-      <c r="K105" s="157"/>
+      <c r="K105" s="159"/>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B106" s="138"/>
-      <c r="C106" s="139"/>
-      <c r="D106" s="144"/>
-      <c r="E106" s="145"/>
-      <c r="F106" s="150"/>
-      <c r="G106" s="151"/>
+      <c r="B106" s="140"/>
+      <c r="C106" s="141"/>
+      <c r="D106" s="146"/>
+      <c r="E106" s="147"/>
+      <c r="F106" s="152"/>
+      <c r="G106" s="153"/>
       <c r="H106" s="119" t="s">
         <v>46</v>
       </c>
@@ -5106,45 +5142,45 @@
         <v>47</v>
       </c>
       <c r="J106" s="119"/>
-      <c r="K106" s="157"/>
+      <c r="K106" s="159"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="51">
         <v>16</v>
       </c>
-      <c r="B107" s="140"/>
-      <c r="C107" s="141"/>
-      <c r="D107" s="146"/>
-      <c r="E107" s="147"/>
-      <c r="F107" s="152"/>
-      <c r="G107" s="153"/>
+      <c r="B107" s="142"/>
+      <c r="C107" s="143"/>
+      <c r="D107" s="148"/>
+      <c r="E107" s="149"/>
+      <c r="F107" s="154"/>
+      <c r="G107" s="155"/>
       <c r="H107" s="50">
         <v>43434</v>
       </c>
       <c r="I107" s="50"/>
       <c r="J107" s="48"/>
-      <c r="K107" s="157"/>
+      <c r="K107" s="159"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B108" s="133" t="s">
+      <c r="B108" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C108" s="134"/>
-      <c r="D108" s="133" t="s">
+      <c r="C108" s="136"/>
+      <c r="D108" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E108" s="134"/>
-      <c r="F108" s="133" t="s">
+      <c r="E108" s="136"/>
+      <c r="F108" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G108" s="134"/>
-      <c r="H108" s="135" t="s">
+      <c r="G108" s="136"/>
+      <c r="H108" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I108" s="135"/>
+      <c r="I108" s="137"/>
       <c r="J108" s="130" t="s">
         <v>39</v>
       </c>
@@ -5156,35 +5192,35 @@
       <c r="A109" s="48">
         <v>17</v>
       </c>
-      <c r="B109" s="136" t="s">
+      <c r="B109" s="138" t="s">
         <v>123</v>
       </c>
-      <c r="C109" s="137"/>
-      <c r="D109" s="142" t="s">
+      <c r="C109" s="139"/>
+      <c r="D109" s="144" t="s">
         <v>127</v>
       </c>
-      <c r="E109" s="143"/>
-      <c r="F109" s="148" t="s">
+      <c r="E109" s="145"/>
+      <c r="F109" s="150" t="s">
         <v>128</v>
       </c>
-      <c r="G109" s="149"/>
-      <c r="H109" s="154" t="s">
+      <c r="G109" s="151"/>
+      <c r="H109" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I109" s="155"/>
+      <c r="I109" s="157"/>
       <c r="J109" s="52"/>
-      <c r="K109" s="156"/>
+      <c r="K109" s="158"/>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="138"/>
-      <c r="C110" s="139"/>
-      <c r="D110" s="144"/>
-      <c r="E110" s="145"/>
-      <c r="F110" s="150"/>
-      <c r="G110" s="151"/>
+      <c r="B110" s="140"/>
+      <c r="C110" s="141"/>
+      <c r="D110" s="146"/>
+      <c r="E110" s="147"/>
+      <c r="F110" s="152"/>
+      <c r="G110" s="153"/>
       <c r="H110" s="130" t="s">
         <v>42</v>
       </c>
@@ -5194,35 +5230,35 @@
       <c r="J110" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="K110" s="157"/>
+      <c r="K110" s="159"/>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="B111" s="138"/>
-      <c r="C111" s="139"/>
-      <c r="D111" s="144"/>
-      <c r="E111" s="145"/>
-      <c r="F111" s="150"/>
-      <c r="G111" s="151"/>
+      <c r="B111" s="140"/>
+      <c r="C111" s="141"/>
+      <c r="D111" s="146"/>
+      <c r="E111" s="147"/>
+      <c r="F111" s="152"/>
+      <c r="G111" s="153"/>
       <c r="H111" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I111" s="50"/>
       <c r="J111" s="48"/>
-      <c r="K111" s="157"/>
+      <c r="K111" s="159"/>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B112" s="138"/>
-      <c r="C112" s="139"/>
-      <c r="D112" s="144"/>
-      <c r="E112" s="145"/>
-      <c r="F112" s="150"/>
-      <c r="G112" s="151"/>
+      <c r="B112" s="140"/>
+      <c r="C112" s="141"/>
+      <c r="D112" s="146"/>
+      <c r="E112" s="147"/>
+      <c r="F112" s="152"/>
+      <c r="G112" s="153"/>
       <c r="H112" s="130" t="s">
         <v>46</v>
       </c>
@@ -5230,45 +5266,45 @@
         <v>47</v>
       </c>
       <c r="J112" s="130"/>
-      <c r="K112" s="157"/>
+      <c r="K112" s="159"/>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" s="51">
         <v>17</v>
       </c>
-      <c r="B113" s="140"/>
-      <c r="C113" s="141"/>
-      <c r="D113" s="146"/>
-      <c r="E113" s="147"/>
-      <c r="F113" s="152"/>
-      <c r="G113" s="153"/>
+      <c r="B113" s="142"/>
+      <c r="C113" s="143"/>
+      <c r="D113" s="148"/>
+      <c r="E113" s="149"/>
+      <c r="F113" s="154"/>
+      <c r="G113" s="155"/>
       <c r="H113" s="50">
         <v>43434</v>
       </c>
       <c r="I113" s="50"/>
       <c r="J113" s="48"/>
-      <c r="K113" s="158"/>
+      <c r="K113" s="160"/>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B114" s="133" t="s">
+      <c r="B114" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C114" s="134"/>
-      <c r="D114" s="133" t="s">
+      <c r="C114" s="136"/>
+      <c r="D114" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E114" s="134"/>
-      <c r="F114" s="133" t="s">
+      <c r="E114" s="136"/>
+      <c r="F114" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="G114" s="134"/>
-      <c r="H114" s="135" t="s">
+      <c r="G114" s="136"/>
+      <c r="H114" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I114" s="135"/>
+      <c r="I114" s="137"/>
       <c r="J114" s="130" t="s">
         <v>39</v>
       </c>
@@ -5280,35 +5316,35 @@
       <c r="A115" s="48">
         <v>18</v>
       </c>
-      <c r="B115" s="136" t="s">
+      <c r="B115" s="138" t="s">
         <v>124</v>
       </c>
-      <c r="C115" s="137"/>
-      <c r="D115" s="142" t="s">
+      <c r="C115" s="139"/>
+      <c r="D115" s="144" t="s">
         <v>129</v>
       </c>
-      <c r="E115" s="143"/>
-      <c r="F115" s="148" t="s">
+      <c r="E115" s="145"/>
+      <c r="F115" s="150" t="s">
         <v>130</v>
       </c>
-      <c r="G115" s="149"/>
-      <c r="H115" s="154" t="s">
+      <c r="G115" s="151"/>
+      <c r="H115" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="I115" s="155"/>
+      <c r="I115" s="157"/>
       <c r="J115" s="52"/>
-      <c r="K115" s="156"/>
+      <c r="K115" s="158"/>
     </row>
     <row r="116" spans="1:11">
       <c r="A116" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B116" s="138"/>
-      <c r="C116" s="139"/>
-      <c r="D116" s="144"/>
-      <c r="E116" s="145"/>
-      <c r="F116" s="150"/>
-      <c r="G116" s="151"/>
+      <c r="B116" s="140"/>
+      <c r="C116" s="141"/>
+      <c r="D116" s="146"/>
+      <c r="E116" s="147"/>
+      <c r="F116" s="152"/>
+      <c r="G116" s="153"/>
       <c r="H116" s="130" t="s">
         <v>42</v>
       </c>
@@ -5318,35 +5354,35 @@
       <c r="J116" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="K116" s="157"/>
+      <c r="K116" s="159"/>
     </row>
     <row r="117" spans="1:11">
       <c r="A117" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B117" s="138"/>
-      <c r="C117" s="139"/>
-      <c r="D117" s="144"/>
-      <c r="E117" s="145"/>
-      <c r="F117" s="150"/>
-      <c r="G117" s="151"/>
+      <c r="B117" s="140"/>
+      <c r="C117" s="141"/>
+      <c r="D117" s="146"/>
+      <c r="E117" s="147"/>
+      <c r="F117" s="152"/>
+      <c r="G117" s="153"/>
       <c r="H117" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I117" s="50"/>
       <c r="J117" s="48"/>
-      <c r="K117" s="157"/>
+      <c r="K117" s="159"/>
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B118" s="138"/>
-      <c r="C118" s="139"/>
-      <c r="D118" s="144"/>
-      <c r="E118" s="145"/>
-      <c r="F118" s="150"/>
-      <c r="G118" s="151"/>
+      <c r="B118" s="140"/>
+      <c r="C118" s="141"/>
+      <c r="D118" s="146"/>
+      <c r="E118" s="147"/>
+      <c r="F118" s="152"/>
+      <c r="G118" s="153"/>
       <c r="H118" s="130" t="s">
         <v>46</v>
       </c>
@@ -5354,83 +5390,440 @@
         <v>47</v>
       </c>
       <c r="J118" s="130"/>
-      <c r="K118" s="157"/>
+      <c r="K118" s="159"/>
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="51">
         <v>18</v>
       </c>
-      <c r="B119" s="140"/>
-      <c r="C119" s="141"/>
-      <c r="D119" s="146"/>
-      <c r="E119" s="147"/>
-      <c r="F119" s="152"/>
-      <c r="G119" s="153"/>
+      <c r="B119" s="142"/>
+      <c r="C119" s="143"/>
+      <c r="D119" s="148"/>
+      <c r="E119" s="149"/>
+      <c r="F119" s="154"/>
+      <c r="G119" s="155"/>
       <c r="H119" s="50">
         <v>43434</v>
       </c>
       <c r="I119" s="50"/>
       <c r="J119" s="48"/>
-      <c r="K119" s="158"/>
+      <c r="K119" s="160"/>
+    </row>
+    <row r="120" spans="1:11">
+      <c r="A120" s="98" t="s">
+        <v>131</v>
+      </c>
+      <c r="B120" s="165" t="s">
+        <v>132</v>
+      </c>
+      <c r="C120" s="165"/>
+      <c r="D120" s="166"/>
+      <c r="E120" s="166"/>
+      <c r="F120" s="166"/>
+      <c r="G120" s="166"/>
+      <c r="H120" s="166"/>
+      <c r="I120" s="166"/>
+      <c r="J120" s="166"/>
+      <c r="K120" s="166"/>
+    </row>
+    <row r="121" spans="1:11">
+      <c r="A121" s="132" t="s">
+        <v>34</v>
+      </c>
+      <c r="B121" s="135" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="136"/>
+      <c r="D121" s="135" t="s">
+        <v>36</v>
+      </c>
+      <c r="E121" s="136"/>
+      <c r="F121" s="135" t="s">
+        <v>37</v>
+      </c>
+      <c r="G121" s="136"/>
+      <c r="H121" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="I121" s="137"/>
+      <c r="J121" s="132" t="s">
+        <v>39</v>
+      </c>
+      <c r="K121" s="131" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
+      <c r="A122" s="48">
+        <v>19</v>
+      </c>
+      <c r="B122" s="138" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" s="139"/>
+      <c r="D122" s="144" t="s">
+        <v>136</v>
+      </c>
+      <c r="E122" s="145"/>
+      <c r="F122" s="150" t="s">
+        <v>137</v>
+      </c>
+      <c r="G122" s="151"/>
+      <c r="H122" s="156" t="s">
+        <v>9</v>
+      </c>
+      <c r="I122" s="157"/>
+      <c r="J122" s="52"/>
+      <c r="K122" s="158"/>
+    </row>
+    <row r="123" spans="1:11">
+      <c r="A123" s="132" t="s">
+        <v>41</v>
+      </c>
+      <c r="B123" s="140"/>
+      <c r="C123" s="141"/>
+      <c r="D123" s="146"/>
+      <c r="E123" s="147"/>
+      <c r="F123" s="152"/>
+      <c r="G123" s="153"/>
+      <c r="H123" s="132" t="s">
+        <v>42</v>
+      </c>
+      <c r="I123" s="132" t="s">
+        <v>43</v>
+      </c>
+      <c r="J123" s="132" t="s">
+        <v>44</v>
+      </c>
+      <c r="K123" s="159"/>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="A124" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="B124" s="140"/>
+      <c r="C124" s="141"/>
+      <c r="D124" s="146"/>
+      <c r="E124" s="147"/>
+      <c r="F124" s="152"/>
+      <c r="G124" s="153"/>
+      <c r="H124" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I124" s="50"/>
+      <c r="J124" s="48"/>
+      <c r="K124" s="159"/>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="132" t="s">
+        <v>45</v>
+      </c>
+      <c r="B125" s="140"/>
+      <c r="C125" s="141"/>
+      <c r="D125" s="146"/>
+      <c r="E125" s="147"/>
+      <c r="F125" s="152"/>
+      <c r="G125" s="153"/>
+      <c r="H125" s="132" t="s">
+        <v>46</v>
+      </c>
+      <c r="I125" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="J125" s="132"/>
+      <c r="K125" s="159"/>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" s="51">
+        <v>19</v>
+      </c>
+      <c r="B126" s="142"/>
+      <c r="C126" s="143"/>
+      <c r="D126" s="148"/>
+      <c r="E126" s="149"/>
+      <c r="F126" s="154"/>
+      <c r="G126" s="155"/>
+      <c r="H126" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I126" s="50"/>
+      <c r="J126" s="48"/>
+      <c r="K126" s="160"/>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="132" t="s">
+        <v>34</v>
+      </c>
+      <c r="B127" s="135" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="136"/>
+      <c r="D127" s="135" t="s">
+        <v>36</v>
+      </c>
+      <c r="E127" s="136"/>
+      <c r="F127" s="135" t="s">
+        <v>37</v>
+      </c>
+      <c r="G127" s="136"/>
+      <c r="H127" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="I127" s="137"/>
+      <c r="J127" s="132" t="s">
+        <v>39</v>
+      </c>
+      <c r="K127" s="131" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A128" s="48">
+        <v>20</v>
+      </c>
+      <c r="B128" s="138" t="s">
+        <v>138</v>
+      </c>
+      <c r="C128" s="139"/>
+      <c r="D128" s="144" t="s">
+        <v>139</v>
+      </c>
+      <c r="E128" s="145"/>
+      <c r="F128" s="150" t="s">
+        <v>140</v>
+      </c>
+      <c r="G128" s="151"/>
+      <c r="H128" s="156" t="s">
+        <v>9</v>
+      </c>
+      <c r="I128" s="157"/>
+      <c r="J128" s="52"/>
+      <c r="K128" s="158"/>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="132" t="s">
+        <v>41</v>
+      </c>
+      <c r="B129" s="140"/>
+      <c r="C129" s="141"/>
+      <c r="D129" s="146"/>
+      <c r="E129" s="147"/>
+      <c r="F129" s="152"/>
+      <c r="G129" s="153"/>
+      <c r="H129" s="132" t="s">
+        <v>42</v>
+      </c>
+      <c r="I129" s="132" t="s">
+        <v>43</v>
+      </c>
+      <c r="J129" s="132" t="s">
+        <v>44</v>
+      </c>
+      <c r="K129" s="159"/>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="B130" s="140"/>
+      <c r="C130" s="141"/>
+      <c r="D130" s="146"/>
+      <c r="E130" s="147"/>
+      <c r="F130" s="152"/>
+      <c r="G130" s="153"/>
+      <c r="H130" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I130" s="50"/>
+      <c r="J130" s="48"/>
+      <c r="K130" s="159"/>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="132" t="s">
+        <v>45</v>
+      </c>
+      <c r="B131" s="140"/>
+      <c r="C131" s="141"/>
+      <c r="D131" s="146"/>
+      <c r="E131" s="147"/>
+      <c r="F131" s="152"/>
+      <c r="G131" s="153"/>
+      <c r="H131" s="132" t="s">
+        <v>46</v>
+      </c>
+      <c r="I131" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="J131" s="132"/>
+      <c r="K131" s="159"/>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="51">
+        <v>20</v>
+      </c>
+      <c r="B132" s="142"/>
+      <c r="C132" s="143"/>
+      <c r="D132" s="148"/>
+      <c r="E132" s="149"/>
+      <c r="F132" s="154"/>
+      <c r="G132" s="155"/>
+      <c r="H132" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I132" s="50"/>
+      <c r="J132" s="48"/>
+      <c r="K132" s="160"/>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="A134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+    </row>
+    <row r="135" spans="1:11">
+      <c r="A135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+    </row>
+    <row r="136" spans="1:11">
+      <c r="A136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="A137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="A138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="167">
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="B115:C119"/>
-    <mergeCell ref="D115:E119"/>
-    <mergeCell ref="F115:G119"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="K115:K119"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="B109:C113"/>
-    <mergeCell ref="D109:E113"/>
-    <mergeCell ref="F109:G113"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="K109:K113"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="B103:C107"/>
-    <mergeCell ref="D103:E107"/>
-    <mergeCell ref="F103:G107"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="K103:K107"/>
-    <mergeCell ref="B95:K95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="B97:C101"/>
-    <mergeCell ref="D97:E101"/>
-    <mergeCell ref="F97:G101"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="K97:K101"/>
-    <mergeCell ref="B72:C76"/>
-    <mergeCell ref="D72:E76"/>
-    <mergeCell ref="F72:G76"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="K72:K76"/>
-    <mergeCell ref="B70:K70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="D46:E50"/>
-    <mergeCell ref="F46:G50"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="K46:K50"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
+  <mergeCells count="186">
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="F127:G127"/>
+    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="B128:C132"/>
+    <mergeCell ref="D128:E132"/>
+    <mergeCell ref="F128:G132"/>
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="K128:K132"/>
+    <mergeCell ref="B120:K120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="B122:C126"/>
+    <mergeCell ref="D122:E126"/>
+    <mergeCell ref="F122:G126"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="K122:K126"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="B90:C94"/>
+    <mergeCell ref="D90:E94"/>
+    <mergeCell ref="F90:G94"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="K90:K94"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="B84:C88"/>
+    <mergeCell ref="D84:E88"/>
+    <mergeCell ref="F84:G88"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="K84:K88"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="B78:C82"/>
+    <mergeCell ref="D78:E82"/>
+    <mergeCell ref="F78:G82"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="B65:C69"/>
+    <mergeCell ref="D65:E69"/>
+    <mergeCell ref="F65:G69"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="K65:K69"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B59:C63"/>
+    <mergeCell ref="D59:E63"/>
+    <mergeCell ref="F59:G63"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="K59:K63"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B53:C57"/>
+    <mergeCell ref="D53:E57"/>
+    <mergeCell ref="F53:G57"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:K57"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="K28:K32"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:C38"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="F34:G38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B40:C44"/>
+    <mergeCell ref="D40:E44"/>
+    <mergeCell ref="F40:G44"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F28:G32"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D28:E32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="F21:G25"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="H8:I8"/>
@@ -5454,94 +5847,63 @@
     <mergeCell ref="D15:E19"/>
     <mergeCell ref="B15:C19"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F28:G32"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="D28:E32"/>
     <mergeCell ref="K21:K25"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="B28:C32"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:E25"/>
-    <mergeCell ref="F21:G25"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="K34:K38"/>
-    <mergeCell ref="K28:K32"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B34:C38"/>
-    <mergeCell ref="D34:E38"/>
-    <mergeCell ref="F34:G38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B40:C44"/>
-    <mergeCell ref="D40:E44"/>
-    <mergeCell ref="F40:G44"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B46:C50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="B53:C57"/>
-    <mergeCell ref="D53:E57"/>
-    <mergeCell ref="F53:G57"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="K53:K57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="B59:C63"/>
-    <mergeCell ref="D59:E63"/>
-    <mergeCell ref="F59:G63"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="K59:K63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="B65:C69"/>
-    <mergeCell ref="D65:E69"/>
-    <mergeCell ref="F65:G69"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="K65:K69"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="B78:C82"/>
-    <mergeCell ref="D78:E82"/>
-    <mergeCell ref="F78:G82"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="B84:C88"/>
-    <mergeCell ref="D84:E88"/>
-    <mergeCell ref="F84:G88"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="K84:K88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="B90:C94"/>
-    <mergeCell ref="D90:E94"/>
-    <mergeCell ref="F90:G94"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="K90:K94"/>
+    <mergeCell ref="D46:E50"/>
+    <mergeCell ref="F46:G50"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="K46:K50"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B72:C76"/>
+    <mergeCell ref="D72:E76"/>
+    <mergeCell ref="F72:G76"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="K72:K76"/>
+    <mergeCell ref="B70:K70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="B95:K95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="B97:C101"/>
+    <mergeCell ref="D97:E101"/>
+    <mergeCell ref="F97:G101"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="K97:K101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="B103:C107"/>
+    <mergeCell ref="D103:E107"/>
+    <mergeCell ref="F103:G107"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="K103:K107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="B109:C113"/>
+    <mergeCell ref="D109:E113"/>
+    <mergeCell ref="F109:G113"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="K109:K113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="B115:C119"/>
+    <mergeCell ref="D115:E119"/>
+    <mergeCell ref="F115:G119"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="K115:K119"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H34:I34">

</xml_diff>

<commit_message>
Add DangBai test case continue
</commit_message>
<xml_diff>
--- a/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="145">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -470,6 +470,18 @@
   </si>
   <si>
     <t>Hệ thống thông báo lỗi cho người dùng,trường sai định dạng và nhập lại</t>
+  </si>
+  <si>
+    <t>6-3</t>
+  </si>
+  <si>
+    <t>DangBai_03</t>
+  </si>
+  <si>
+    <t>Kiểm tra xem bài post của người dùng có đúng với nội dung đã được nhập không</t>
+  </si>
+  <si>
+    <t>Hệ thống hiển thị đúng nội dung đã được nhập ,theo định dạng của một bài viết được định trước</t>
   </si>
 </sst>
 </file>
@@ -968,7 +980,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1284,6 +1296,12 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1369,6 +1387,12 @@
     <xf numFmtId="49" fontId="18" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1381,11 +1405,44 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1404,45 +1461,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1553,7 +1571,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0730E54B-906F-483C-AE30-73A046308AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2020,13 +2038,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="133" t="s">
+      <c r="O6" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="133"/>
-      <c r="Q6" s="133"/>
-      <c r="R6" s="133"/>
-      <c r="S6" s="133"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -2036,11 +2054,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="133"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="133"/>
-      <c r="R7" s="133"/>
-      <c r="S7" s="133"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="135"/>
+      <c r="R7" s="135"/>
+      <c r="S7" s="135"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -2095,12 +2113,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="134">
+      <c r="E11" s="136">
         <f ca="1">TODAY()</f>
         <v>43431</v>
       </c>
-      <c r="F11" s="134"/>
-      <c r="G11" s="134"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
       <c r="H11" s="71"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -2961,7 +2979,7 @@
   <dimension ref="A1:K138"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A115" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2993,7 +3011,7 @@
       </c>
       <c r="I1" s="99">
         <f>COUNTIF(H1:H761,"OK")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J1" s="81" t="s">
         <v>23</v>
@@ -3061,7 +3079,7 @@
       <c r="H4" s="84"/>
       <c r="I4" s="100">
         <f>COUNTIF(H3:H763,"Result")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J4" s="88"/>
       <c r="K4" s="89"/>
@@ -3096,39 +3114,39 @@
       <c r="A7" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="166" t="s">
+      <c r="B7" s="164" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="166"/>
-      <c r="H7" s="166"/>
-      <c r="I7" s="166"/>
-      <c r="J7" s="166"/>
-      <c r="K7" s="166"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="164"/>
+      <c r="I7" s="164"/>
+      <c r="J7" s="164"/>
+      <c r="K7" s="164"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="136"/>
-      <c r="D8" s="135" t="s">
+      <c r="C8" s="138"/>
+      <c r="D8" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="136"/>
-      <c r="F8" s="135" t="s">
+      <c r="E8" s="138"/>
+      <c r="F8" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="136"/>
-      <c r="H8" s="173" t="s">
+      <c r="G8" s="138"/>
+      <c r="H8" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="173"/>
+      <c r="I8" s="169"/>
       <c r="J8" s="116" t="s">
         <v>39</v>
       </c>
@@ -3140,35 +3158,35 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="138" t="s">
+      <c r="B9" s="140" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="139"/>
-      <c r="D9" s="144" t="s">
+      <c r="C9" s="141"/>
+      <c r="D9" s="146" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="145"/>
-      <c r="F9" s="174" t="s">
+      <c r="E9" s="147"/>
+      <c r="F9" s="176" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="175"/>
-      <c r="H9" s="163" t="s">
+      <c r="G9" s="177"/>
+      <c r="H9" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="164"/>
+      <c r="I9" s="168"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="158"/>
+      <c r="K9" s="160"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="140"/>
-      <c r="C10" s="141"/>
-      <c r="D10" s="146"/>
-      <c r="E10" s="147"/>
-      <c r="F10" s="176"/>
-      <c r="G10" s="177"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="148"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="179"/>
       <c r="H10" s="115" t="s">
         <v>42</v>
       </c>
@@ -3178,35 +3196,35 @@
       <c r="J10" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="159"/>
+      <c r="K10" s="161"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="140"/>
-      <c r="C11" s="141"/>
-      <c r="D11" s="146"/>
-      <c r="E11" s="147"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="177"/>
+      <c r="B11" s="142"/>
+      <c r="C11" s="143"/>
+      <c r="D11" s="148"/>
+      <c r="E11" s="149"/>
+      <c r="F11" s="178"/>
+      <c r="G11" s="179"/>
       <c r="H11" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="159"/>
+      <c r="K11" s="161"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="140"/>
-      <c r="C12" s="141"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="147"/>
-      <c r="F12" s="176"/>
-      <c r="G12" s="177"/>
+      <c r="B12" s="142"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="148"/>
+      <c r="E12" s="149"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="179"/>
       <c r="H12" s="115" t="s">
         <v>46</v>
       </c>
@@ -3214,45 +3232,45 @@
         <v>47</v>
       </c>
       <c r="J12" s="115"/>
-      <c r="K12" s="159"/>
+      <c r="K12" s="161"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>1</v>
       </c>
-      <c r="B13" s="142"/>
-      <c r="C13" s="143"/>
-      <c r="D13" s="148"/>
-      <c r="E13" s="149"/>
-      <c r="F13" s="178"/>
-      <c r="G13" s="179"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="145"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="181"/>
       <c r="H13" s="53">
         <v>43434</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="160"/>
+      <c r="K13" s="162"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="161" t="s">
+      <c r="B14" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="162"/>
-      <c r="D14" s="161" t="s">
+      <c r="C14" s="166"/>
+      <c r="D14" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="162"/>
-      <c r="F14" s="161" t="s">
+      <c r="E14" s="166"/>
+      <c r="F14" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="162"/>
-      <c r="H14" s="161" t="s">
+      <c r="G14" s="166"/>
+      <c r="H14" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="162"/>
+      <c r="I14" s="166"/>
       <c r="J14" s="119" t="s">
         <v>39</v>
       </c>
@@ -3264,35 +3282,35 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="140" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="139"/>
-      <c r="D15" s="144" t="s">
+      <c r="C15" s="141"/>
+      <c r="D15" s="146" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="145"/>
-      <c r="F15" s="150" t="s">
+      <c r="E15" s="147"/>
+      <c r="F15" s="152" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="151"/>
-      <c r="H15" s="163" t="s">
+      <c r="G15" s="153"/>
+      <c r="H15" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="164"/>
+      <c r="I15" s="168"/>
       <c r="J15" s="52"/>
-      <c r="K15" s="158"/>
+      <c r="K15" s="160"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="140"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="146"/>
-      <c r="E16" s="147"/>
-      <c r="F16" s="152"/>
-      <c r="G16" s="153"/>
+      <c r="B16" s="142"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="148"/>
+      <c r="E16" s="149"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="155"/>
       <c r="H16" s="119" t="s">
         <v>42</v>
       </c>
@@ -3302,35 +3320,35 @@
       <c r="J16" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="159"/>
+      <c r="K16" s="161"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="140"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="147"/>
-      <c r="F17" s="152"/>
-      <c r="G17" s="153"/>
+      <c r="B17" s="142"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="148"/>
+      <c r="E17" s="149"/>
+      <c r="F17" s="154"/>
+      <c r="G17" s="155"/>
       <c r="H17" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48"/>
-      <c r="K17" s="159"/>
+      <c r="K17" s="161"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="140"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="146"/>
-      <c r="E18" s="147"/>
-      <c r="F18" s="152"/>
-      <c r="G18" s="153"/>
+      <c r="B18" s="142"/>
+      <c r="C18" s="143"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="149"/>
+      <c r="F18" s="154"/>
+      <c r="G18" s="155"/>
       <c r="H18" s="119" t="s">
         <v>46</v>
       </c>
@@ -3338,45 +3356,45 @@
         <v>47</v>
       </c>
       <c r="J18" s="119"/>
-      <c r="K18" s="159"/>
+      <c r="K18" s="161"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>2</v>
       </c>
-      <c r="B19" s="142"/>
-      <c r="C19" s="143"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="149"/>
-      <c r="F19" s="154"/>
-      <c r="G19" s="155"/>
+      <c r="B19" s="144"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="156"/>
+      <c r="G19" s="157"/>
       <c r="H19" s="50">
         <v>43434</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="159"/>
+      <c r="K19" s="161"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="136"/>
-      <c r="D20" s="135" t="s">
+      <c r="C20" s="138"/>
+      <c r="D20" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="136"/>
-      <c r="F20" s="135" t="s">
+      <c r="E20" s="138"/>
+      <c r="F20" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="136"/>
-      <c r="H20" s="173" t="s">
+      <c r="G20" s="138"/>
+      <c r="H20" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="173"/>
+      <c r="I20" s="169"/>
       <c r="J20" s="120" t="s">
         <v>39</v>
       </c>
@@ -3388,35 +3406,35 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="140" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="139"/>
-      <c r="D21" s="144" t="s">
+      <c r="C21" s="141"/>
+      <c r="D21" s="146" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="145"/>
-      <c r="F21" s="180" t="s">
+      <c r="E21" s="147"/>
+      <c r="F21" s="170" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="181"/>
-      <c r="H21" s="163" t="s">
+      <c r="G21" s="171"/>
+      <c r="H21" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="164"/>
+      <c r="I21" s="168"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="158"/>
+      <c r="K21" s="160"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="140"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="147"/>
-      <c r="F22" s="182"/>
-      <c r="G22" s="183"/>
+      <c r="B22" s="142"/>
+      <c r="C22" s="143"/>
+      <c r="D22" s="148"/>
+      <c r="E22" s="149"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="173"/>
       <c r="H22" s="118" t="s">
         <v>42</v>
       </c>
@@ -3426,35 +3444,35 @@
       <c r="J22" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="159"/>
+      <c r="K22" s="161"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="140"/>
-      <c r="C23" s="141"/>
-      <c r="D23" s="146"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="182"/>
-      <c r="G23" s="183"/>
+      <c r="B23" s="142"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="148"/>
+      <c r="E23" s="149"/>
+      <c r="F23" s="172"/>
+      <c r="G23" s="173"/>
       <c r="H23" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="159"/>
+      <c r="K23" s="161"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="140"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="146"/>
-      <c r="E24" s="147"/>
-      <c r="F24" s="182"/>
-      <c r="G24" s="183"/>
+      <c r="B24" s="142"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="149"/>
+      <c r="F24" s="172"/>
+      <c r="G24" s="173"/>
       <c r="H24" s="118" t="s">
         <v>46</v>
       </c>
@@ -3462,62 +3480,62 @@
         <v>47</v>
       </c>
       <c r="J24" s="118"/>
-      <c r="K24" s="159"/>
+      <c r="K24" s="161"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>3</v>
       </c>
-      <c r="B25" s="142"/>
-      <c r="C25" s="143"/>
-      <c r="D25" s="148"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="184"/>
-      <c r="G25" s="185"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="174"/>
+      <c r="G25" s="175"/>
       <c r="H25" s="53">
         <v>43434</v>
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="54"/>
-      <c r="K25" s="160"/>
+      <c r="K25" s="162"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="165" t="s">
+      <c r="B26" s="163" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="165"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
-      <c r="H26" s="166"/>
-      <c r="I26" s="166"/>
-      <c r="J26" s="166"/>
-      <c r="K26" s="166"/>
+      <c r="C26" s="163"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="164"/>
+      <c r="H26" s="164"/>
+      <c r="I26" s="164"/>
+      <c r="J26" s="164"/>
+      <c r="K26" s="164"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="135" t="s">
+      <c r="B27" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="136"/>
-      <c r="D27" s="135" t="s">
+      <c r="C27" s="138"/>
+      <c r="D27" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="136"/>
-      <c r="F27" s="135" t="s">
+      <c r="E27" s="138"/>
+      <c r="F27" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="136"/>
-      <c r="H27" s="137" t="s">
+      <c r="G27" s="138"/>
+      <c r="H27" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="137"/>
+      <c r="I27" s="139"/>
       <c r="J27" s="115" t="s">
         <v>39</v>
       </c>
@@ -3529,35 +3547,35 @@
       <c r="A28" s="48">
         <v>4</v>
       </c>
-      <c r="B28" s="138" t="s">
+      <c r="B28" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="139"/>
-      <c r="D28" s="144" t="s">
+      <c r="C28" s="141"/>
+      <c r="D28" s="146" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="145"/>
-      <c r="F28" s="150" t="s">
+      <c r="E28" s="147"/>
+      <c r="F28" s="152" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="151"/>
-      <c r="H28" s="156" t="s">
+      <c r="G28" s="153"/>
+      <c r="H28" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="157"/>
+      <c r="I28" s="159"/>
       <c r="J28" s="52"/>
-      <c r="K28" s="158"/>
+      <c r="K28" s="160"/>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="140"/>
-      <c r="C29" s="141"/>
-      <c r="D29" s="146"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="153"/>
+      <c r="B29" s="142"/>
+      <c r="C29" s="143"/>
+      <c r="D29" s="148"/>
+      <c r="E29" s="149"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="155"/>
       <c r="H29" s="115" t="s">
         <v>42</v>
       </c>
@@ -3567,35 +3585,35 @@
       <c r="J29" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="159"/>
+      <c r="K29" s="161"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="140"/>
-      <c r="C30" s="141"/>
-      <c r="D30" s="146"/>
-      <c r="E30" s="147"/>
-      <c r="F30" s="152"/>
-      <c r="G30" s="153"/>
+      <c r="B30" s="142"/>
+      <c r="C30" s="143"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="149"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="155"/>
       <c r="H30" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I30" s="50"/>
       <c r="J30" s="48"/>
-      <c r="K30" s="159"/>
+      <c r="K30" s="161"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="140"/>
-      <c r="C31" s="141"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="147"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="153"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="143"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="154"/>
+      <c r="G31" s="155"/>
       <c r="H31" s="115" t="s">
         <v>46</v>
       </c>
@@ -3603,45 +3621,45 @@
         <v>47</v>
       </c>
       <c r="J31" s="115"/>
-      <c r="K31" s="159"/>
+      <c r="K31" s="161"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="51">
         <v>4</v>
       </c>
-      <c r="B32" s="142"/>
-      <c r="C32" s="143"/>
-      <c r="D32" s="148"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="154"/>
-      <c r="G32" s="155"/>
+      <c r="B32" s="144"/>
+      <c r="C32" s="145"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="156"/>
+      <c r="G32" s="157"/>
       <c r="H32" s="50">
         <v>43434</v>
       </c>
       <c r="I32" s="50"/>
       <c r="J32" s="48"/>
-      <c r="K32" s="160"/>
+      <c r="K32" s="162"/>
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A33" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="135" t="s">
+      <c r="B33" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="136"/>
-      <c r="D33" s="135" t="s">
+      <c r="C33" s="138"/>
+      <c r="D33" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="136"/>
-      <c r="F33" s="135" t="s">
+      <c r="E33" s="138"/>
+      <c r="F33" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="136"/>
-      <c r="H33" s="137" t="s">
+      <c r="G33" s="138"/>
+      <c r="H33" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="137"/>
+      <c r="I33" s="139"/>
       <c r="J33" s="115" t="s">
         <v>39</v>
       </c>
@@ -3653,35 +3671,35 @@
       <c r="A34" s="48">
         <v>5</v>
       </c>
-      <c r="B34" s="138" t="s">
+      <c r="B34" s="140" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="139"/>
-      <c r="D34" s="144" t="s">
+      <c r="C34" s="141"/>
+      <c r="D34" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="145"/>
-      <c r="F34" s="150" t="s">
+      <c r="E34" s="147"/>
+      <c r="F34" s="152" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="151"/>
-      <c r="H34" s="156" t="s">
+      <c r="G34" s="153"/>
+      <c r="H34" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I34" s="157"/>
+      <c r="I34" s="159"/>
       <c r="J34" s="52"/>
-      <c r="K34" s="158"/>
+      <c r="K34" s="160"/>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="140"/>
-      <c r="C35" s="141"/>
-      <c r="D35" s="146"/>
-      <c r="E35" s="147"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="153"/>
+      <c r="B35" s="142"/>
+      <c r="C35" s="143"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="149"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="155"/>
       <c r="H35" s="115" t="s">
         <v>42</v>
       </c>
@@ -3691,35 +3709,35 @@
       <c r="J35" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="159"/>
+      <c r="K35" s="161"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="140"/>
-      <c r="C36" s="141"/>
-      <c r="D36" s="146"/>
-      <c r="E36" s="147"/>
-      <c r="F36" s="152"/>
-      <c r="G36" s="153"/>
+      <c r="B36" s="142"/>
+      <c r="C36" s="143"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="149"/>
+      <c r="F36" s="154"/>
+      <c r="G36" s="155"/>
       <c r="H36" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I36" s="50"/>
       <c r="J36" s="48"/>
-      <c r="K36" s="159"/>
+      <c r="K36" s="161"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="140"/>
-      <c r="C37" s="141"/>
-      <c r="D37" s="146"/>
-      <c r="E37" s="147"/>
-      <c r="F37" s="152"/>
-      <c r="G37" s="153"/>
+      <c r="B37" s="142"/>
+      <c r="C37" s="143"/>
+      <c r="D37" s="148"/>
+      <c r="E37" s="149"/>
+      <c r="F37" s="154"/>
+      <c r="G37" s="155"/>
       <c r="H37" s="115" t="s">
         <v>46</v>
       </c>
@@ -3727,45 +3745,45 @@
         <v>47</v>
       </c>
       <c r="J37" s="115"/>
-      <c r="K37" s="159"/>
+      <c r="K37" s="161"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="51">
         <v>5</v>
       </c>
-      <c r="B38" s="142"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="148"/>
-      <c r="E38" s="149"/>
-      <c r="F38" s="154"/>
-      <c r="G38" s="155"/>
+      <c r="B38" s="144"/>
+      <c r="C38" s="145"/>
+      <c r="D38" s="150"/>
+      <c r="E38" s="151"/>
+      <c r="F38" s="156"/>
+      <c r="G38" s="157"/>
       <c r="H38" s="50">
         <v>43434</v>
       </c>
       <c r="I38" s="50"/>
       <c r="J38" s="48"/>
-      <c r="K38" s="160"/>
+      <c r="K38" s="162"/>
     </row>
     <row r="39" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A39" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="135" t="s">
+      <c r="B39" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="136"/>
-      <c r="D39" s="135" t="s">
+      <c r="C39" s="138"/>
+      <c r="D39" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="136"/>
-      <c r="F39" s="135" t="s">
+      <c r="E39" s="138"/>
+      <c r="F39" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="136"/>
-      <c r="H39" s="137" t="s">
+      <c r="G39" s="138"/>
+      <c r="H39" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="137"/>
+      <c r="I39" s="139"/>
       <c r="J39" s="121" t="s">
         <v>39</v>
       </c>
@@ -3777,35 +3795,35 @@
       <c r="A40" s="48">
         <v>6</v>
       </c>
-      <c r="B40" s="138" t="s">
+      <c r="B40" s="140" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="139"/>
-      <c r="D40" s="144" t="s">
+      <c r="C40" s="141"/>
+      <c r="D40" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="145"/>
-      <c r="F40" s="150" t="s">
+      <c r="E40" s="147"/>
+      <c r="F40" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="151"/>
-      <c r="H40" s="156" t="s">
+      <c r="G40" s="153"/>
+      <c r="H40" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="157"/>
+      <c r="I40" s="159"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="158"/>
+      <c r="K40" s="160"/>
     </row>
     <row r="41" spans="1:11" ht="10.5" customHeight="1">
       <c r="A41" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="140"/>
-      <c r="C41" s="141"/>
-      <c r="D41" s="146"/>
-      <c r="E41" s="147"/>
-      <c r="F41" s="152"/>
-      <c r="G41" s="153"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="143"/>
+      <c r="D41" s="148"/>
+      <c r="E41" s="149"/>
+      <c r="F41" s="154"/>
+      <c r="G41" s="155"/>
       <c r="H41" s="121" t="s">
         <v>42</v>
       </c>
@@ -3815,35 +3833,35 @@
       <c r="J41" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="159"/>
+      <c r="K41" s="161"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="140"/>
-      <c r="C42" s="141"/>
-      <c r="D42" s="146"/>
-      <c r="E42" s="147"/>
-      <c r="F42" s="152"/>
-      <c r="G42" s="153"/>
+      <c r="B42" s="142"/>
+      <c r="C42" s="143"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="149"/>
+      <c r="F42" s="154"/>
+      <c r="G42" s="155"/>
       <c r="H42" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I42" s="50"/>
       <c r="J42" s="48"/>
-      <c r="K42" s="159"/>
+      <c r="K42" s="161"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="140"/>
-      <c r="C43" s="141"/>
-      <c r="D43" s="146"/>
-      <c r="E43" s="147"/>
-      <c r="F43" s="152"/>
-      <c r="G43" s="153"/>
+      <c r="B43" s="142"/>
+      <c r="C43" s="143"/>
+      <c r="D43" s="148"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="154"/>
+      <c r="G43" s="155"/>
       <c r="H43" s="121" t="s">
         <v>46</v>
       </c>
@@ -3851,45 +3869,45 @@
         <v>47</v>
       </c>
       <c r="J43" s="121"/>
-      <c r="K43" s="159"/>
+      <c r="K43" s="161"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="51">
         <v>6</v>
       </c>
-      <c r="B44" s="142"/>
-      <c r="C44" s="143"/>
-      <c r="D44" s="148"/>
-      <c r="E44" s="149"/>
-      <c r="F44" s="154"/>
-      <c r="G44" s="155"/>
+      <c r="B44" s="144"/>
+      <c r="C44" s="145"/>
+      <c r="D44" s="150"/>
+      <c r="E44" s="151"/>
+      <c r="F44" s="156"/>
+      <c r="G44" s="157"/>
       <c r="H44" s="50">
         <v>43434</v>
       </c>
       <c r="I44" s="50"/>
       <c r="J44" s="48"/>
-      <c r="K44" s="160"/>
+      <c r="K44" s="162"/>
     </row>
     <row r="45" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A45" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="135" t="s">
+      <c r="B45" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="136"/>
-      <c r="D45" s="135" t="s">
+      <c r="C45" s="138"/>
+      <c r="D45" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="136"/>
-      <c r="F45" s="135" t="s">
+      <c r="E45" s="138"/>
+      <c r="F45" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="136"/>
-      <c r="H45" s="137" t="s">
+      <c r="G45" s="138"/>
+      <c r="H45" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="137"/>
+      <c r="I45" s="139"/>
       <c r="J45" s="121" t="s">
         <v>39</v>
       </c>
@@ -3901,35 +3919,35 @@
       <c r="A46" s="48">
         <v>7</v>
       </c>
-      <c r="B46" s="138" t="s">
+      <c r="B46" s="140" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="139"/>
-      <c r="D46" s="144" t="s">
+      <c r="C46" s="141"/>
+      <c r="D46" s="146" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="145"/>
-      <c r="F46" s="167" t="s">
+      <c r="E46" s="147"/>
+      <c r="F46" s="182" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="168"/>
-      <c r="H46" s="156" t="s">
+      <c r="G46" s="183"/>
+      <c r="H46" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I46" s="157"/>
+      <c r="I46" s="159"/>
       <c r="J46" s="52"/>
-      <c r="K46" s="158"/>
+      <c r="K46" s="160"/>
     </row>
     <row r="47" spans="1:11" ht="10.5" customHeight="1">
       <c r="A47" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="140"/>
-      <c r="C47" s="141"/>
-      <c r="D47" s="146"/>
-      <c r="E47" s="147"/>
-      <c r="F47" s="169"/>
-      <c r="G47" s="170"/>
+      <c r="B47" s="142"/>
+      <c r="C47" s="143"/>
+      <c r="D47" s="148"/>
+      <c r="E47" s="149"/>
+      <c r="F47" s="184"/>
+      <c r="G47" s="185"/>
       <c r="H47" s="121" t="s">
         <v>42</v>
       </c>
@@ -3939,35 +3957,35 @@
       <c r="J47" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="K47" s="159"/>
+      <c r="K47" s="161"/>
     </row>
     <row r="48" spans="1:11" ht="10.5" customHeight="1">
       <c r="A48" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="140"/>
-      <c r="C48" s="141"/>
-      <c r="D48" s="146"/>
-      <c r="E48" s="147"/>
-      <c r="F48" s="169"/>
-      <c r="G48" s="170"/>
+      <c r="B48" s="142"/>
+      <c r="C48" s="143"/>
+      <c r="D48" s="148"/>
+      <c r="E48" s="149"/>
+      <c r="F48" s="184"/>
+      <c r="G48" s="185"/>
       <c r="H48" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I48" s="50"/>
       <c r="J48" s="48"/>
-      <c r="K48" s="159"/>
+      <c r="K48" s="161"/>
     </row>
     <row r="49" spans="1:11" ht="10.5" customHeight="1">
       <c r="A49" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="140"/>
-      <c r="C49" s="141"/>
-      <c r="D49" s="146"/>
-      <c r="E49" s="147"/>
-      <c r="F49" s="169"/>
-      <c r="G49" s="170"/>
+      <c r="B49" s="142"/>
+      <c r="C49" s="143"/>
+      <c r="D49" s="148"/>
+      <c r="E49" s="149"/>
+      <c r="F49" s="184"/>
+      <c r="G49" s="185"/>
       <c r="H49" s="121" t="s">
         <v>46</v>
       </c>
@@ -3975,62 +3993,62 @@
         <v>47</v>
       </c>
       <c r="J49" s="121"/>
-      <c r="K49" s="159"/>
+      <c r="K49" s="161"/>
     </row>
     <row r="50" spans="1:11" ht="10.5" customHeight="1">
       <c r="A50" s="51">
         <v>7</v>
       </c>
-      <c r="B50" s="142"/>
-      <c r="C50" s="143"/>
-      <c r="D50" s="148"/>
-      <c r="E50" s="149"/>
-      <c r="F50" s="171"/>
-      <c r="G50" s="172"/>
+      <c r="B50" s="144"/>
+      <c r="C50" s="145"/>
+      <c r="D50" s="150"/>
+      <c r="E50" s="151"/>
+      <c r="F50" s="186"/>
+      <c r="G50" s="187"/>
       <c r="H50" s="50">
         <v>43434</v>
       </c>
       <c r="I50" s="50"/>
       <c r="J50" s="48"/>
-      <c r="K50" s="160"/>
+      <c r="K50" s="162"/>
     </row>
     <row r="51" spans="1:11" s="58" customFormat="1">
       <c r="A51" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="165" t="s">
+      <c r="B51" s="163" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="165"/>
-      <c r="D51" s="166"/>
-      <c r="E51" s="166"/>
-      <c r="F51" s="166"/>
-      <c r="G51" s="166"/>
-      <c r="H51" s="166"/>
-      <c r="I51" s="166"/>
-      <c r="J51" s="166"/>
-      <c r="K51" s="166"/>
+      <c r="C51" s="163"/>
+      <c r="D51" s="164"/>
+      <c r="E51" s="164"/>
+      <c r="F51" s="164"/>
+      <c r="G51" s="164"/>
+      <c r="H51" s="164"/>
+      <c r="I51" s="164"/>
+      <c r="J51" s="164"/>
+      <c r="K51" s="164"/>
     </row>
     <row r="52" spans="1:11" s="58" customFormat="1">
       <c r="A52" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="135" t="s">
+      <c r="B52" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="136"/>
-      <c r="D52" s="135" t="s">
+      <c r="C52" s="138"/>
+      <c r="D52" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="136"/>
-      <c r="F52" s="135" t="s">
+      <c r="E52" s="138"/>
+      <c r="F52" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G52" s="136"/>
-      <c r="H52" s="137" t="s">
+      <c r="G52" s="138"/>
+      <c r="H52" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I52" s="137"/>
+      <c r="I52" s="139"/>
       <c r="J52" s="124" t="s">
         <v>39</v>
       </c>
@@ -4042,35 +4060,35 @@
       <c r="A53" s="48">
         <v>8</v>
       </c>
-      <c r="B53" s="138" t="s">
+      <c r="B53" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="139"/>
-      <c r="D53" s="144" t="s">
+      <c r="C53" s="141"/>
+      <c r="D53" s="146" t="s">
         <v>89</v>
       </c>
-      <c r="E53" s="145"/>
-      <c r="F53" s="150" t="s">
+      <c r="E53" s="147"/>
+      <c r="F53" s="152" t="s">
         <v>90</v>
       </c>
-      <c r="G53" s="151"/>
-      <c r="H53" s="156" t="s">
+      <c r="G53" s="153"/>
+      <c r="H53" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I53" s="157"/>
+      <c r="I53" s="159"/>
       <c r="J53" s="52"/>
-      <c r="K53" s="158"/>
+      <c r="K53" s="160"/>
     </row>
     <row r="54" spans="1:11" s="58" customFormat="1">
       <c r="A54" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="140"/>
-      <c r="C54" s="141"/>
-      <c r="D54" s="146"/>
-      <c r="E54" s="147"/>
-      <c r="F54" s="152"/>
-      <c r="G54" s="153"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="143"/>
+      <c r="D54" s="148"/>
+      <c r="E54" s="149"/>
+      <c r="F54" s="154"/>
+      <c r="G54" s="155"/>
       <c r="H54" s="124" t="s">
         <v>42</v>
       </c>
@@ -4080,35 +4098,35 @@
       <c r="J54" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K54" s="159"/>
+      <c r="K54" s="161"/>
     </row>
     <row r="55" spans="1:11" s="58" customFormat="1">
       <c r="A55" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="140"/>
-      <c r="C55" s="141"/>
-      <c r="D55" s="146"/>
-      <c r="E55" s="147"/>
-      <c r="F55" s="152"/>
-      <c r="G55" s="153"/>
+      <c r="B55" s="142"/>
+      <c r="C55" s="143"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="149"/>
+      <c r="F55" s="154"/>
+      <c r="G55" s="155"/>
       <c r="H55" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I55" s="50"/>
       <c r="J55" s="48"/>
-      <c r="K55" s="159"/>
+      <c r="K55" s="161"/>
     </row>
     <row r="56" spans="1:11" s="58" customFormat="1">
       <c r="A56" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="140"/>
-      <c r="C56" s="141"/>
-      <c r="D56" s="146"/>
-      <c r="E56" s="147"/>
-      <c r="F56" s="152"/>
-      <c r="G56" s="153"/>
+      <c r="B56" s="142"/>
+      <c r="C56" s="143"/>
+      <c r="D56" s="148"/>
+      <c r="E56" s="149"/>
+      <c r="F56" s="154"/>
+      <c r="G56" s="155"/>
       <c r="H56" s="124" t="s">
         <v>46</v>
       </c>
@@ -4116,45 +4134,45 @@
         <v>47</v>
       </c>
       <c r="J56" s="124"/>
-      <c r="K56" s="159"/>
+      <c r="K56" s="161"/>
     </row>
     <row r="57" spans="1:11" s="58" customFormat="1">
       <c r="A57" s="51">
         <v>8</v>
       </c>
-      <c r="B57" s="142"/>
-      <c r="C57" s="143"/>
-      <c r="D57" s="148"/>
-      <c r="E57" s="149"/>
-      <c r="F57" s="154"/>
-      <c r="G57" s="155"/>
+      <c r="B57" s="144"/>
+      <c r="C57" s="145"/>
+      <c r="D57" s="150"/>
+      <c r="E57" s="151"/>
+      <c r="F57" s="156"/>
+      <c r="G57" s="157"/>
       <c r="H57" s="50">
         <v>43434</v>
       </c>
       <c r="I57" s="50"/>
       <c r="J57" s="48"/>
-      <c r="K57" s="160"/>
+      <c r="K57" s="162"/>
     </row>
     <row r="58" spans="1:11" s="58" customFormat="1">
       <c r="A58" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="135" t="s">
+      <c r="B58" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="136"/>
-      <c r="D58" s="135" t="s">
+      <c r="C58" s="138"/>
+      <c r="D58" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="136"/>
-      <c r="F58" s="135" t="s">
+      <c r="E58" s="138"/>
+      <c r="F58" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G58" s="136"/>
-      <c r="H58" s="137" t="s">
+      <c r="G58" s="138"/>
+      <c r="H58" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I58" s="137"/>
+      <c r="I58" s="139"/>
       <c r="J58" s="124" t="s">
         <v>39</v>
       </c>
@@ -4166,35 +4184,35 @@
       <c r="A59" s="48">
         <v>9</v>
       </c>
-      <c r="B59" s="138" t="s">
+      <c r="B59" s="140" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="139"/>
-      <c r="D59" s="144" t="s">
+      <c r="C59" s="141"/>
+      <c r="D59" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="145"/>
-      <c r="F59" s="150" t="s">
+      <c r="E59" s="147"/>
+      <c r="F59" s="152" t="s">
         <v>92</v>
       </c>
-      <c r="G59" s="151"/>
-      <c r="H59" s="156" t="s">
+      <c r="G59" s="153"/>
+      <c r="H59" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I59" s="157"/>
+      <c r="I59" s="159"/>
       <c r="J59" s="52"/>
-      <c r="K59" s="158"/>
+      <c r="K59" s="160"/>
     </row>
     <row r="60" spans="1:11" s="58" customFormat="1">
       <c r="A60" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="140"/>
-      <c r="C60" s="141"/>
-      <c r="D60" s="146"/>
-      <c r="E60" s="147"/>
-      <c r="F60" s="152"/>
-      <c r="G60" s="153"/>
+      <c r="B60" s="142"/>
+      <c r="C60" s="143"/>
+      <c r="D60" s="148"/>
+      <c r="E60" s="149"/>
+      <c r="F60" s="154"/>
+      <c r="G60" s="155"/>
       <c r="H60" s="124" t="s">
         <v>42</v>
       </c>
@@ -4204,35 +4222,35 @@
       <c r="J60" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K60" s="159"/>
+      <c r="K60" s="161"/>
     </row>
     <row r="61" spans="1:11" s="58" customFormat="1">
       <c r="A61" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B61" s="140"/>
-      <c r="C61" s="141"/>
-      <c r="D61" s="146"/>
-      <c r="E61" s="147"/>
-      <c r="F61" s="152"/>
-      <c r="G61" s="153"/>
+      <c r="B61" s="142"/>
+      <c r="C61" s="143"/>
+      <c r="D61" s="148"/>
+      <c r="E61" s="149"/>
+      <c r="F61" s="154"/>
+      <c r="G61" s="155"/>
       <c r="H61" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I61" s="50"/>
       <c r="J61" s="48"/>
-      <c r="K61" s="159"/>
+      <c r="K61" s="161"/>
     </row>
     <row r="62" spans="1:11" s="58" customFormat="1">
       <c r="A62" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="140"/>
-      <c r="C62" s="141"/>
-      <c r="D62" s="146"/>
-      <c r="E62" s="147"/>
-      <c r="F62" s="152"/>
-      <c r="G62" s="153"/>
+      <c r="B62" s="142"/>
+      <c r="C62" s="143"/>
+      <c r="D62" s="148"/>
+      <c r="E62" s="149"/>
+      <c r="F62" s="154"/>
+      <c r="G62" s="155"/>
       <c r="H62" s="124" t="s">
         <v>46</v>
       </c>
@@ -4240,45 +4258,45 @@
         <v>47</v>
       </c>
       <c r="J62" s="124"/>
-      <c r="K62" s="159"/>
+      <c r="K62" s="161"/>
     </row>
     <row r="63" spans="1:11" s="58" customFormat="1">
       <c r="A63" s="51">
         <v>9</v>
       </c>
-      <c r="B63" s="142"/>
-      <c r="C63" s="143"/>
-      <c r="D63" s="148"/>
-      <c r="E63" s="149"/>
-      <c r="F63" s="154"/>
-      <c r="G63" s="155"/>
+      <c r="B63" s="144"/>
+      <c r="C63" s="145"/>
+      <c r="D63" s="150"/>
+      <c r="E63" s="151"/>
+      <c r="F63" s="156"/>
+      <c r="G63" s="157"/>
       <c r="H63" s="50">
         <v>43434</v>
       </c>
       <c r="I63" s="50"/>
       <c r="J63" s="48"/>
-      <c r="K63" s="160"/>
+      <c r="K63" s="162"/>
     </row>
     <row r="64" spans="1:11" s="58" customFormat="1">
       <c r="A64" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="135" t="s">
+      <c r="B64" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="136"/>
-      <c r="D64" s="135" t="s">
+      <c r="C64" s="138"/>
+      <c r="D64" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E64" s="136"/>
-      <c r="F64" s="135" t="s">
+      <c r="E64" s="138"/>
+      <c r="F64" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G64" s="136"/>
-      <c r="H64" s="137" t="s">
+      <c r="G64" s="138"/>
+      <c r="H64" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I64" s="137"/>
+      <c r="I64" s="139"/>
       <c r="J64" s="124" t="s">
         <v>39</v>
       </c>
@@ -4290,35 +4308,35 @@
       <c r="A65" s="48">
         <v>10</v>
       </c>
-      <c r="B65" s="138" t="s">
+      <c r="B65" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="C65" s="139"/>
-      <c r="D65" s="144" t="s">
+      <c r="C65" s="141"/>
+      <c r="D65" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="E65" s="145"/>
-      <c r="F65" s="150" t="s">
+      <c r="E65" s="147"/>
+      <c r="F65" s="152" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="151"/>
-      <c r="H65" s="156" t="s">
+      <c r="G65" s="153"/>
+      <c r="H65" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I65" s="157"/>
+      <c r="I65" s="159"/>
       <c r="J65" s="52"/>
-      <c r="K65" s="158"/>
+      <c r="K65" s="160"/>
     </row>
     <row r="66" spans="1:11" s="58" customFormat="1">
       <c r="A66" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="140"/>
-      <c r="C66" s="141"/>
-      <c r="D66" s="146"/>
-      <c r="E66" s="147"/>
-      <c r="F66" s="152"/>
-      <c r="G66" s="153"/>
+      <c r="B66" s="142"/>
+      <c r="C66" s="143"/>
+      <c r="D66" s="148"/>
+      <c r="E66" s="149"/>
+      <c r="F66" s="154"/>
+      <c r="G66" s="155"/>
       <c r="H66" s="124" t="s">
         <v>42</v>
       </c>
@@ -4328,35 +4346,35 @@
       <c r="J66" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="K66" s="159"/>
+      <c r="K66" s="161"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B67" s="140"/>
-      <c r="C67" s="141"/>
-      <c r="D67" s="146"/>
-      <c r="E67" s="147"/>
-      <c r="F67" s="152"/>
-      <c r="G67" s="153"/>
+      <c r="B67" s="142"/>
+      <c r="C67" s="143"/>
+      <c r="D67" s="148"/>
+      <c r="E67" s="149"/>
+      <c r="F67" s="154"/>
+      <c r="G67" s="155"/>
       <c r="H67" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I67" s="50"/>
       <c r="J67" s="48"/>
-      <c r="K67" s="159"/>
+      <c r="K67" s="161"/>
     </row>
     <row r="68" spans="1:11" s="58" customFormat="1">
       <c r="A68" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="140"/>
-      <c r="C68" s="141"/>
-      <c r="D68" s="146"/>
-      <c r="E68" s="147"/>
-      <c r="F68" s="152"/>
-      <c r="G68" s="153"/>
+      <c r="B68" s="142"/>
+      <c r="C68" s="143"/>
+      <c r="D68" s="148"/>
+      <c r="E68" s="149"/>
+      <c r="F68" s="154"/>
+      <c r="G68" s="155"/>
       <c r="H68" s="124" t="s">
         <v>46</v>
       </c>
@@ -4364,62 +4382,62 @@
         <v>47</v>
       </c>
       <c r="J68" s="124"/>
-      <c r="K68" s="159"/>
+      <c r="K68" s="161"/>
     </row>
     <row r="69" spans="1:11" s="58" customFormat="1">
       <c r="A69" s="51">
         <v>10</v>
       </c>
-      <c r="B69" s="142"/>
-      <c r="C69" s="143"/>
-      <c r="D69" s="148"/>
-      <c r="E69" s="149"/>
-      <c r="F69" s="154"/>
-      <c r="G69" s="155"/>
+      <c r="B69" s="144"/>
+      <c r="C69" s="145"/>
+      <c r="D69" s="150"/>
+      <c r="E69" s="151"/>
+      <c r="F69" s="156"/>
+      <c r="G69" s="157"/>
       <c r="H69" s="50">
         <v>43434</v>
       </c>
       <c r="I69" s="50"/>
       <c r="J69" s="48"/>
-      <c r="K69" s="160"/>
+      <c r="K69" s="162"/>
     </row>
     <row r="70" spans="1:11" s="58" customFormat="1">
       <c r="A70" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="B70" s="165" t="s">
+      <c r="B70" s="163" t="s">
         <v>96</v>
       </c>
-      <c r="C70" s="165"/>
-      <c r="D70" s="166"/>
-      <c r="E70" s="166"/>
-      <c r="F70" s="166"/>
-      <c r="G70" s="166"/>
-      <c r="H70" s="166"/>
-      <c r="I70" s="166"/>
-      <c r="J70" s="166"/>
-      <c r="K70" s="166"/>
+      <c r="C70" s="163"/>
+      <c r="D70" s="164"/>
+      <c r="E70" s="164"/>
+      <c r="F70" s="164"/>
+      <c r="G70" s="164"/>
+      <c r="H70" s="164"/>
+      <c r="I70" s="164"/>
+      <c r="J70" s="164"/>
+      <c r="K70" s="164"/>
     </row>
     <row r="71" spans="1:11" s="58" customFormat="1">
       <c r="A71" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B71" s="135" t="s">
+      <c r="B71" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C71" s="136"/>
-      <c r="D71" s="135" t="s">
+      <c r="C71" s="138"/>
+      <c r="D71" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E71" s="136"/>
-      <c r="F71" s="135" t="s">
+      <c r="E71" s="138"/>
+      <c r="F71" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G71" s="136"/>
-      <c r="H71" s="137" t="s">
+      <c r="G71" s="138"/>
+      <c r="H71" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I71" s="137"/>
+      <c r="I71" s="139"/>
       <c r="J71" s="126" t="s">
         <v>39</v>
       </c>
@@ -4431,35 +4449,35 @@
       <c r="A72" s="48">
         <v>11</v>
       </c>
-      <c r="B72" s="138" t="s">
+      <c r="B72" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="C72" s="139"/>
-      <c r="D72" s="144" t="s">
+      <c r="C72" s="141"/>
+      <c r="D72" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="145"/>
-      <c r="F72" s="150" t="s">
+      <c r="E72" s="147"/>
+      <c r="F72" s="152" t="s">
         <v>107</v>
       </c>
-      <c r="G72" s="151"/>
-      <c r="H72" s="156" t="s">
+      <c r="G72" s="153"/>
+      <c r="H72" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I72" s="157"/>
+      <c r="I72" s="159"/>
       <c r="J72" s="52"/>
-      <c r="K72" s="158"/>
+      <c r="K72" s="160"/>
     </row>
     <row r="73" spans="1:11" s="58" customFormat="1">
       <c r="A73" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="140"/>
-      <c r="C73" s="141"/>
-      <c r="D73" s="146"/>
-      <c r="E73" s="147"/>
-      <c r="F73" s="152"/>
-      <c r="G73" s="153"/>
+      <c r="B73" s="142"/>
+      <c r="C73" s="143"/>
+      <c r="D73" s="148"/>
+      <c r="E73" s="149"/>
+      <c r="F73" s="154"/>
+      <c r="G73" s="155"/>
       <c r="H73" s="126" t="s">
         <v>42</v>
       </c>
@@ -4469,35 +4487,35 @@
       <c r="J73" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K73" s="159"/>
+      <c r="K73" s="161"/>
     </row>
     <row r="74" spans="1:11" s="58" customFormat="1">
       <c r="A74" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="140"/>
-      <c r="C74" s="141"/>
-      <c r="D74" s="146"/>
-      <c r="E74" s="147"/>
-      <c r="F74" s="152"/>
-      <c r="G74" s="153"/>
+      <c r="B74" s="142"/>
+      <c r="C74" s="143"/>
+      <c r="D74" s="148"/>
+      <c r="E74" s="149"/>
+      <c r="F74" s="154"/>
+      <c r="G74" s="155"/>
       <c r="H74" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I74" s="50"/>
       <c r="J74" s="48"/>
-      <c r="K74" s="159"/>
+      <c r="K74" s="161"/>
     </row>
     <row r="75" spans="1:11" s="58" customFormat="1">
       <c r="A75" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="B75" s="140"/>
-      <c r="C75" s="141"/>
-      <c r="D75" s="146"/>
-      <c r="E75" s="147"/>
-      <c r="F75" s="152"/>
-      <c r="G75" s="153"/>
+      <c r="B75" s="142"/>
+      <c r="C75" s="143"/>
+      <c r="D75" s="148"/>
+      <c r="E75" s="149"/>
+      <c r="F75" s="154"/>
+      <c r="G75" s="155"/>
       <c r="H75" s="126" t="s">
         <v>46</v>
       </c>
@@ -4505,45 +4523,45 @@
         <v>47</v>
       </c>
       <c r="J75" s="126"/>
-      <c r="K75" s="159"/>
+      <c r="K75" s="161"/>
     </row>
     <row r="76" spans="1:11" s="58" customFormat="1">
       <c r="A76" s="51">
         <v>11</v>
       </c>
-      <c r="B76" s="142"/>
-      <c r="C76" s="143"/>
-      <c r="D76" s="148"/>
-      <c r="E76" s="149"/>
-      <c r="F76" s="154"/>
-      <c r="G76" s="155"/>
+      <c r="B76" s="144"/>
+      <c r="C76" s="145"/>
+      <c r="D76" s="150"/>
+      <c r="E76" s="151"/>
+      <c r="F76" s="156"/>
+      <c r="G76" s="157"/>
       <c r="H76" s="50">
         <v>43434</v>
       </c>
       <c r="I76" s="50"/>
       <c r="J76" s="48"/>
-      <c r="K76" s="160"/>
+      <c r="K76" s="162"/>
     </row>
     <row r="77" spans="1:11" s="58" customFormat="1">
       <c r="A77" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B77" s="161" t="s">
+      <c r="B77" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="C77" s="162"/>
-      <c r="D77" s="161" t="s">
+      <c r="C77" s="166"/>
+      <c r="D77" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E77" s="162"/>
-      <c r="F77" s="161" t="s">
+      <c r="E77" s="166"/>
+      <c r="F77" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="G77" s="162"/>
-      <c r="H77" s="161" t="s">
+      <c r="G77" s="166"/>
+      <c r="H77" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="I77" s="162"/>
+      <c r="I77" s="166"/>
       <c r="J77" s="119" t="s">
         <v>39</v>
       </c>
@@ -4555,35 +4573,35 @@
       <c r="A78" s="48">
         <v>12</v>
       </c>
-      <c r="B78" s="138" t="s">
+      <c r="B78" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="C78" s="139"/>
-      <c r="D78" s="144" t="s">
+      <c r="C78" s="141"/>
+      <c r="D78" s="146" t="s">
         <v>99</v>
       </c>
-      <c r="E78" s="145"/>
-      <c r="F78" s="150" t="s">
+      <c r="E78" s="147"/>
+      <c r="F78" s="152" t="s">
         <v>108</v>
       </c>
-      <c r="G78" s="151"/>
-      <c r="H78" s="163" t="s">
+      <c r="G78" s="153"/>
+      <c r="H78" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="I78" s="164"/>
+      <c r="I78" s="168"/>
       <c r="J78" s="52"/>
-      <c r="K78" s="158"/>
+      <c r="K78" s="160"/>
     </row>
     <row r="79" spans="1:11" s="58" customFormat="1">
       <c r="A79" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="140"/>
-      <c r="C79" s="141"/>
-      <c r="D79" s="146"/>
-      <c r="E79" s="147"/>
-      <c r="F79" s="152"/>
-      <c r="G79" s="153"/>
+      <c r="B79" s="142"/>
+      <c r="C79" s="143"/>
+      <c r="D79" s="148"/>
+      <c r="E79" s="149"/>
+      <c r="F79" s="154"/>
+      <c r="G79" s="155"/>
       <c r="H79" s="119" t="s">
         <v>42</v>
       </c>
@@ -4593,35 +4611,35 @@
       <c r="J79" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K79" s="159"/>
+      <c r="K79" s="161"/>
     </row>
     <row r="80" spans="1:11" s="58" customFormat="1">
       <c r="A80" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="140"/>
-      <c r="C80" s="141"/>
-      <c r="D80" s="146"/>
-      <c r="E80" s="147"/>
-      <c r="F80" s="152"/>
-      <c r="G80" s="153"/>
+      <c r="B80" s="142"/>
+      <c r="C80" s="143"/>
+      <c r="D80" s="148"/>
+      <c r="E80" s="149"/>
+      <c r="F80" s="154"/>
+      <c r="G80" s="155"/>
       <c r="H80" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I80" s="50"/>
       <c r="J80" s="48"/>
-      <c r="K80" s="159"/>
+      <c r="K80" s="161"/>
     </row>
     <row r="81" spans="1:11" s="58" customFormat="1">
       <c r="A81" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B81" s="140"/>
-      <c r="C81" s="141"/>
-      <c r="D81" s="146"/>
-      <c r="E81" s="147"/>
-      <c r="F81" s="152"/>
-      <c r="G81" s="153"/>
+      <c r="B81" s="142"/>
+      <c r="C81" s="143"/>
+      <c r="D81" s="148"/>
+      <c r="E81" s="149"/>
+      <c r="F81" s="154"/>
+      <c r="G81" s="155"/>
       <c r="H81" s="119" t="s">
         <v>46</v>
       </c>
@@ -4629,45 +4647,45 @@
         <v>47</v>
       </c>
       <c r="J81" s="119"/>
-      <c r="K81" s="159"/>
+      <c r="K81" s="161"/>
     </row>
     <row r="82" spans="1:11" s="58" customFormat="1">
       <c r="A82" s="51">
         <v>12</v>
       </c>
-      <c r="B82" s="142"/>
-      <c r="C82" s="143"/>
-      <c r="D82" s="148"/>
-      <c r="E82" s="149"/>
-      <c r="F82" s="154"/>
-      <c r="G82" s="155"/>
+      <c r="B82" s="144"/>
+      <c r="C82" s="145"/>
+      <c r="D82" s="150"/>
+      <c r="E82" s="151"/>
+      <c r="F82" s="156"/>
+      <c r="G82" s="157"/>
       <c r="H82" s="50">
         <v>43434</v>
       </c>
       <c r="I82" s="50"/>
       <c r="J82" s="48"/>
-      <c r="K82" s="159"/>
+      <c r="K82" s="161"/>
     </row>
     <row r="83" spans="1:11" s="58" customFormat="1">
       <c r="A83" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="B83" s="135" t="s">
+      <c r="B83" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="136"/>
-      <c r="D83" s="135" t="s">
+      <c r="C83" s="138"/>
+      <c r="D83" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E83" s="136"/>
-      <c r="F83" s="135" t="s">
+      <c r="E83" s="138"/>
+      <c r="F83" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G83" s="136"/>
-      <c r="H83" s="137" t="s">
+      <c r="G83" s="138"/>
+      <c r="H83" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I83" s="137"/>
+      <c r="I83" s="139"/>
       <c r="J83" s="128" t="s">
         <v>39</v>
       </c>
@@ -4679,35 +4697,35 @@
       <c r="A84" s="48">
         <v>13</v>
       </c>
-      <c r="B84" s="138" t="s">
+      <c r="B84" s="140" t="s">
         <v>104</v>
       </c>
-      <c r="C84" s="139"/>
-      <c r="D84" s="144" t="s">
+      <c r="C84" s="141"/>
+      <c r="D84" s="146" t="s">
         <v>109</v>
       </c>
-      <c r="E84" s="145"/>
-      <c r="F84" s="150" t="s">
+      <c r="E84" s="147"/>
+      <c r="F84" s="152" t="s">
         <v>110</v>
       </c>
-      <c r="G84" s="151"/>
-      <c r="H84" s="156" t="s">
+      <c r="G84" s="153"/>
+      <c r="H84" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I84" s="157"/>
+      <c r="I84" s="159"/>
       <c r="J84" s="52"/>
-      <c r="K84" s="158"/>
+      <c r="K84" s="160"/>
     </row>
     <row r="85" spans="1:11" s="58" customFormat="1">
       <c r="A85" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="140"/>
-      <c r="C85" s="141"/>
-      <c r="D85" s="146"/>
-      <c r="E85" s="147"/>
-      <c r="F85" s="152"/>
-      <c r="G85" s="153"/>
+      <c r="B85" s="142"/>
+      <c r="C85" s="143"/>
+      <c r="D85" s="148"/>
+      <c r="E85" s="149"/>
+      <c r="F85" s="154"/>
+      <c r="G85" s="155"/>
       <c r="H85" s="128" t="s">
         <v>42</v>
       </c>
@@ -4717,35 +4735,35 @@
       <c r="J85" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="K85" s="159"/>
+      <c r="K85" s="161"/>
     </row>
     <row r="86" spans="1:11" s="58" customFormat="1">
       <c r="A86" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="B86" s="140"/>
-      <c r="C86" s="141"/>
-      <c r="D86" s="146"/>
-      <c r="E86" s="147"/>
-      <c r="F86" s="152"/>
-      <c r="G86" s="153"/>
+      <c r="B86" s="142"/>
+      <c r="C86" s="143"/>
+      <c r="D86" s="148"/>
+      <c r="E86" s="149"/>
+      <c r="F86" s="154"/>
+      <c r="G86" s="155"/>
       <c r="H86" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I86" s="50"/>
       <c r="J86" s="48"/>
-      <c r="K86" s="159"/>
+      <c r="K86" s="161"/>
     </row>
     <row r="87" spans="1:11" s="58" customFormat="1">
       <c r="A87" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="B87" s="140"/>
-      <c r="C87" s="141"/>
-      <c r="D87" s="146"/>
-      <c r="E87" s="147"/>
-      <c r="F87" s="152"/>
-      <c r="G87" s="153"/>
+      <c r="B87" s="142"/>
+      <c r="C87" s="143"/>
+      <c r="D87" s="148"/>
+      <c r="E87" s="149"/>
+      <c r="F87" s="154"/>
+      <c r="G87" s="155"/>
       <c r="H87" s="128" t="s">
         <v>46</v>
       </c>
@@ -4753,45 +4771,45 @@
         <v>47</v>
       </c>
       <c r="J87" s="128"/>
-      <c r="K87" s="159"/>
+      <c r="K87" s="161"/>
     </row>
     <row r="88" spans="1:11" s="58" customFormat="1">
       <c r="A88" s="51">
         <v>13</v>
       </c>
-      <c r="B88" s="142"/>
-      <c r="C88" s="143"/>
-      <c r="D88" s="148"/>
-      <c r="E88" s="149"/>
-      <c r="F88" s="154"/>
-      <c r="G88" s="155"/>
+      <c r="B88" s="144"/>
+      <c r="C88" s="145"/>
+      <c r="D88" s="150"/>
+      <c r="E88" s="151"/>
+      <c r="F88" s="156"/>
+      <c r="G88" s="157"/>
       <c r="H88" s="50">
         <v>43434</v>
       </c>
       <c r="I88" s="50"/>
       <c r="J88" s="48"/>
-      <c r="K88" s="160"/>
+      <c r="K88" s="162"/>
     </row>
     <row r="89" spans="1:11" s="58" customFormat="1">
       <c r="A89" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="B89" s="135" t="s">
+      <c r="B89" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="136"/>
-      <c r="D89" s="135" t="s">
+      <c r="C89" s="138"/>
+      <c r="D89" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E89" s="136"/>
-      <c r="F89" s="135" t="s">
+      <c r="E89" s="138"/>
+      <c r="F89" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G89" s="136"/>
-      <c r="H89" s="137" t="s">
+      <c r="G89" s="138"/>
+      <c r="H89" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I89" s="137"/>
+      <c r="I89" s="139"/>
       <c r="J89" s="128" t="s">
         <v>39</v>
       </c>
@@ -4803,35 +4821,35 @@
       <c r="A90" s="48">
         <v>14</v>
       </c>
-      <c r="B90" s="138" t="s">
+      <c r="B90" s="140" t="s">
         <v>105</v>
       </c>
-      <c r="C90" s="139"/>
-      <c r="D90" s="144" t="s">
+      <c r="C90" s="141"/>
+      <c r="D90" s="146" t="s">
         <v>111</v>
       </c>
-      <c r="E90" s="145"/>
-      <c r="F90" s="150" t="s">
+      <c r="E90" s="147"/>
+      <c r="F90" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="G90" s="151"/>
-      <c r="H90" s="156" t="s">
+      <c r="G90" s="153"/>
+      <c r="H90" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I90" s="157"/>
+      <c r="I90" s="159"/>
       <c r="J90" s="52"/>
-      <c r="K90" s="158"/>
+      <c r="K90" s="160"/>
     </row>
     <row r="91" spans="1:11" s="58" customFormat="1">
       <c r="A91" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B91" s="140"/>
-      <c r="C91" s="141"/>
-      <c r="D91" s="146"/>
-      <c r="E91" s="147"/>
-      <c r="F91" s="152"/>
-      <c r="G91" s="153"/>
+      <c r="B91" s="142"/>
+      <c r="C91" s="143"/>
+      <c r="D91" s="148"/>
+      <c r="E91" s="149"/>
+      <c r="F91" s="154"/>
+      <c r="G91" s="155"/>
       <c r="H91" s="128" t="s">
         <v>42</v>
       </c>
@@ -4841,35 +4859,35 @@
       <c r="J91" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="K91" s="159"/>
+      <c r="K91" s="161"/>
     </row>
     <row r="92" spans="1:11" s="58" customFormat="1">
       <c r="A92" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B92" s="140"/>
-      <c r="C92" s="141"/>
-      <c r="D92" s="146"/>
-      <c r="E92" s="147"/>
-      <c r="F92" s="152"/>
-      <c r="G92" s="153"/>
+      <c r="B92" s="142"/>
+      <c r="C92" s="143"/>
+      <c r="D92" s="148"/>
+      <c r="E92" s="149"/>
+      <c r="F92" s="154"/>
+      <c r="G92" s="155"/>
       <c r="H92" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I92" s="50"/>
       <c r="J92" s="48"/>
-      <c r="K92" s="159"/>
+      <c r="K92" s="161"/>
     </row>
     <row r="93" spans="1:11" s="58" customFormat="1">
       <c r="A93" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="B93" s="140"/>
-      <c r="C93" s="141"/>
-      <c r="D93" s="146"/>
-      <c r="E93" s="147"/>
-      <c r="F93" s="152"/>
-      <c r="G93" s="153"/>
+      <c r="B93" s="142"/>
+      <c r="C93" s="143"/>
+      <c r="D93" s="148"/>
+      <c r="E93" s="149"/>
+      <c r="F93" s="154"/>
+      <c r="G93" s="155"/>
       <c r="H93" s="128" t="s">
         <v>46</v>
       </c>
@@ -4877,62 +4895,62 @@
         <v>47</v>
       </c>
       <c r="J93" s="128"/>
-      <c r="K93" s="159"/>
+      <c r="K93" s="161"/>
     </row>
     <row r="94" spans="1:11" s="58" customFormat="1">
       <c r="A94" s="51">
         <v>14</v>
       </c>
-      <c r="B94" s="142"/>
-      <c r="C94" s="143"/>
-      <c r="D94" s="148"/>
-      <c r="E94" s="149"/>
-      <c r="F94" s="154"/>
-      <c r="G94" s="155"/>
+      <c r="B94" s="144"/>
+      <c r="C94" s="145"/>
+      <c r="D94" s="150"/>
+      <c r="E94" s="151"/>
+      <c r="F94" s="156"/>
+      <c r="G94" s="157"/>
       <c r="H94" s="50">
         <v>43434</v>
       </c>
       <c r="I94" s="50"/>
       <c r="J94" s="48"/>
-      <c r="K94" s="160"/>
+      <c r="K94" s="162"/>
     </row>
     <row r="95" spans="1:11" s="58" customFormat="1">
       <c r="A95" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="B95" s="165" t="s">
+      <c r="B95" s="163" t="s">
         <v>114</v>
       </c>
-      <c r="C95" s="165"/>
-      <c r="D95" s="166"/>
-      <c r="E95" s="166"/>
-      <c r="F95" s="166"/>
-      <c r="G95" s="166"/>
-      <c r="H95" s="166"/>
-      <c r="I95" s="166"/>
-      <c r="J95" s="166"/>
-      <c r="K95" s="166"/>
+      <c r="C95" s="163"/>
+      <c r="D95" s="164"/>
+      <c r="E95" s="164"/>
+      <c r="F95" s="164"/>
+      <c r="G95" s="164"/>
+      <c r="H95" s="164"/>
+      <c r="I95" s="164"/>
+      <c r="J95" s="164"/>
+      <c r="K95" s="164"/>
     </row>
     <row r="96" spans="1:11" s="58" customFormat="1">
       <c r="A96" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B96" s="135" t="s">
+      <c r="B96" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C96" s="136"/>
-      <c r="D96" s="135" t="s">
+      <c r="C96" s="138"/>
+      <c r="D96" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E96" s="136"/>
-      <c r="F96" s="135" t="s">
+      <c r="E96" s="138"/>
+      <c r="F96" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G96" s="136"/>
-      <c r="H96" s="137" t="s">
+      <c r="G96" s="138"/>
+      <c r="H96" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I96" s="137"/>
+      <c r="I96" s="139"/>
       <c r="J96" s="130" t="s">
         <v>39</v>
       </c>
@@ -4944,35 +4962,35 @@
       <c r="A97" s="48">
         <v>15</v>
       </c>
-      <c r="B97" s="138" t="s">
+      <c r="B97" s="140" t="s">
         <v>119</v>
       </c>
-      <c r="C97" s="139"/>
-      <c r="D97" s="144" t="s">
+      <c r="C97" s="141"/>
+      <c r="D97" s="146" t="s">
         <v>120</v>
       </c>
-      <c r="E97" s="145"/>
-      <c r="F97" s="150" t="s">
+      <c r="E97" s="147"/>
+      <c r="F97" s="152" t="s">
         <v>121</v>
       </c>
-      <c r="G97" s="151"/>
-      <c r="H97" s="156" t="s">
+      <c r="G97" s="153"/>
+      <c r="H97" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I97" s="157"/>
+      <c r="I97" s="159"/>
       <c r="J97" s="52"/>
-      <c r="K97" s="158"/>
+      <c r="K97" s="160"/>
     </row>
     <row r="98" spans="1:11" s="58" customFormat="1">
       <c r="A98" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B98" s="140"/>
-      <c r="C98" s="141"/>
-      <c r="D98" s="146"/>
-      <c r="E98" s="147"/>
-      <c r="F98" s="152"/>
-      <c r="G98" s="153"/>
+      <c r="B98" s="142"/>
+      <c r="C98" s="143"/>
+      <c r="D98" s="148"/>
+      <c r="E98" s="149"/>
+      <c r="F98" s="154"/>
+      <c r="G98" s="155"/>
       <c r="H98" s="130" t="s">
         <v>42</v>
       </c>
@@ -4982,35 +5000,35 @@
       <c r="J98" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="K98" s="159"/>
+      <c r="K98" s="161"/>
     </row>
     <row r="99" spans="1:11" s="58" customFormat="1">
       <c r="A99" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="B99" s="140"/>
-      <c r="C99" s="141"/>
-      <c r="D99" s="146"/>
-      <c r="E99" s="147"/>
-      <c r="F99" s="152"/>
-      <c r="G99" s="153"/>
+      <c r="B99" s="142"/>
+      <c r="C99" s="143"/>
+      <c r="D99" s="148"/>
+      <c r="E99" s="149"/>
+      <c r="F99" s="154"/>
+      <c r="G99" s="155"/>
       <c r="H99" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I99" s="50"/>
       <c r="J99" s="48"/>
-      <c r="K99" s="159"/>
+      <c r="K99" s="161"/>
     </row>
     <row r="100" spans="1:11" s="58" customFormat="1">
       <c r="A100" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B100" s="140"/>
-      <c r="C100" s="141"/>
-      <c r="D100" s="146"/>
-      <c r="E100" s="147"/>
-      <c r="F100" s="152"/>
-      <c r="G100" s="153"/>
+      <c r="B100" s="142"/>
+      <c r="C100" s="143"/>
+      <c r="D100" s="148"/>
+      <c r="E100" s="149"/>
+      <c r="F100" s="154"/>
+      <c r="G100" s="155"/>
       <c r="H100" s="130" t="s">
         <v>46</v>
       </c>
@@ -5018,45 +5036,45 @@
         <v>47</v>
       </c>
       <c r="J100" s="130"/>
-      <c r="K100" s="159"/>
+      <c r="K100" s="161"/>
     </row>
     <row r="101" spans="1:11" s="58" customFormat="1">
       <c r="A101" s="51">
         <v>15</v>
       </c>
-      <c r="B101" s="142"/>
-      <c r="C101" s="143"/>
-      <c r="D101" s="148"/>
-      <c r="E101" s="149"/>
-      <c r="F101" s="154"/>
-      <c r="G101" s="155"/>
+      <c r="B101" s="144"/>
+      <c r="C101" s="145"/>
+      <c r="D101" s="150"/>
+      <c r="E101" s="151"/>
+      <c r="F101" s="156"/>
+      <c r="G101" s="157"/>
       <c r="H101" s="50">
         <v>43434</v>
       </c>
       <c r="I101" s="50"/>
       <c r="J101" s="48"/>
-      <c r="K101" s="160"/>
+      <c r="K101" s="162"/>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B102" s="161" t="s">
+      <c r="B102" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="C102" s="162"/>
-      <c r="D102" s="161" t="s">
+      <c r="C102" s="166"/>
+      <c r="D102" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E102" s="162"/>
-      <c r="F102" s="161" t="s">
+      <c r="E102" s="166"/>
+      <c r="F102" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="G102" s="162"/>
-      <c r="H102" s="161" t="s">
+      <c r="G102" s="166"/>
+      <c r="H102" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="I102" s="162"/>
+      <c r="I102" s="166"/>
       <c r="J102" s="119" t="s">
         <v>39</v>
       </c>
@@ -5068,35 +5086,35 @@
       <c r="A103" s="48">
         <v>16</v>
       </c>
-      <c r="B103" s="138" t="s">
+      <c r="B103" s="140" t="s">
         <v>122</v>
       </c>
-      <c r="C103" s="139"/>
-      <c r="D103" s="144" t="s">
+      <c r="C103" s="141"/>
+      <c r="D103" s="146" t="s">
         <v>125</v>
       </c>
-      <c r="E103" s="145"/>
-      <c r="F103" s="150" t="s">
+      <c r="E103" s="147"/>
+      <c r="F103" s="152" t="s">
         <v>126</v>
       </c>
-      <c r="G103" s="151"/>
-      <c r="H103" s="163" t="s">
+      <c r="G103" s="153"/>
+      <c r="H103" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="I103" s="164"/>
+      <c r="I103" s="168"/>
       <c r="J103" s="52"/>
-      <c r="K103" s="158"/>
+      <c r="K103" s="160"/>
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B104" s="140"/>
-      <c r="C104" s="141"/>
-      <c r="D104" s="146"/>
-      <c r="E104" s="147"/>
-      <c r="F104" s="152"/>
-      <c r="G104" s="153"/>
+      <c r="B104" s="142"/>
+      <c r="C104" s="143"/>
+      <c r="D104" s="148"/>
+      <c r="E104" s="149"/>
+      <c r="F104" s="154"/>
+      <c r="G104" s="155"/>
       <c r="H104" s="119" t="s">
         <v>42</v>
       </c>
@@ -5106,35 +5124,35 @@
       <c r="J104" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="K104" s="159"/>
+      <c r="K104" s="161"/>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="B105" s="140"/>
-      <c r="C105" s="141"/>
-      <c r="D105" s="146"/>
-      <c r="E105" s="147"/>
-      <c r="F105" s="152"/>
-      <c r="G105" s="153"/>
+      <c r="B105" s="142"/>
+      <c r="C105" s="143"/>
+      <c r="D105" s="148"/>
+      <c r="E105" s="149"/>
+      <c r="F105" s="154"/>
+      <c r="G105" s="155"/>
       <c r="H105" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I105" s="50"/>
       <c r="J105" s="48"/>
-      <c r="K105" s="159"/>
+      <c r="K105" s="161"/>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B106" s="140"/>
-      <c r="C106" s="141"/>
-      <c r="D106" s="146"/>
-      <c r="E106" s="147"/>
-      <c r="F106" s="152"/>
-      <c r="G106" s="153"/>
+      <c r="B106" s="142"/>
+      <c r="C106" s="143"/>
+      <c r="D106" s="148"/>
+      <c r="E106" s="149"/>
+      <c r="F106" s="154"/>
+      <c r="G106" s="155"/>
       <c r="H106" s="119" t="s">
         <v>46</v>
       </c>
@@ -5142,45 +5160,45 @@
         <v>47</v>
       </c>
       <c r="J106" s="119"/>
-      <c r="K106" s="159"/>
+      <c r="K106" s="161"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="51">
         <v>16</v>
       </c>
-      <c r="B107" s="142"/>
-      <c r="C107" s="143"/>
-      <c r="D107" s="148"/>
-      <c r="E107" s="149"/>
-      <c r="F107" s="154"/>
-      <c r="G107" s="155"/>
+      <c r="B107" s="144"/>
+      <c r="C107" s="145"/>
+      <c r="D107" s="150"/>
+      <c r="E107" s="151"/>
+      <c r="F107" s="156"/>
+      <c r="G107" s="157"/>
       <c r="H107" s="50">
         <v>43434</v>
       </c>
       <c r="I107" s="50"/>
       <c r="J107" s="48"/>
-      <c r="K107" s="159"/>
+      <c r="K107" s="161"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B108" s="135" t="s">
+      <c r="B108" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C108" s="136"/>
-      <c r="D108" s="135" t="s">
+      <c r="C108" s="138"/>
+      <c r="D108" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E108" s="136"/>
-      <c r="F108" s="135" t="s">
+      <c r="E108" s="138"/>
+      <c r="F108" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G108" s="136"/>
-      <c r="H108" s="137" t="s">
+      <c r="G108" s="138"/>
+      <c r="H108" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I108" s="137"/>
+      <c r="I108" s="139"/>
       <c r="J108" s="130" t="s">
         <v>39</v>
       </c>
@@ -5192,35 +5210,35 @@
       <c r="A109" s="48">
         <v>17</v>
       </c>
-      <c r="B109" s="138" t="s">
+      <c r="B109" s="140" t="s">
         <v>123</v>
       </c>
-      <c r="C109" s="139"/>
-      <c r="D109" s="144" t="s">
+      <c r="C109" s="141"/>
+      <c r="D109" s="146" t="s">
         <v>127</v>
       </c>
-      <c r="E109" s="145"/>
-      <c r="F109" s="150" t="s">
+      <c r="E109" s="147"/>
+      <c r="F109" s="152" t="s">
         <v>128</v>
       </c>
-      <c r="G109" s="151"/>
-      <c r="H109" s="156" t="s">
+      <c r="G109" s="153"/>
+      <c r="H109" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I109" s="157"/>
+      <c r="I109" s="159"/>
       <c r="J109" s="52"/>
-      <c r="K109" s="158"/>
+      <c r="K109" s="160"/>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="140"/>
-      <c r="C110" s="141"/>
-      <c r="D110" s="146"/>
-      <c r="E110" s="147"/>
-      <c r="F110" s="152"/>
-      <c r="G110" s="153"/>
+      <c r="B110" s="142"/>
+      <c r="C110" s="143"/>
+      <c r="D110" s="148"/>
+      <c r="E110" s="149"/>
+      <c r="F110" s="154"/>
+      <c r="G110" s="155"/>
       <c r="H110" s="130" t="s">
         <v>42</v>
       </c>
@@ -5230,35 +5248,35 @@
       <c r="J110" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="K110" s="159"/>
+      <c r="K110" s="161"/>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="B111" s="140"/>
-      <c r="C111" s="141"/>
-      <c r="D111" s="146"/>
-      <c r="E111" s="147"/>
-      <c r="F111" s="152"/>
-      <c r="G111" s="153"/>
+      <c r="B111" s="142"/>
+      <c r="C111" s="143"/>
+      <c r="D111" s="148"/>
+      <c r="E111" s="149"/>
+      <c r="F111" s="154"/>
+      <c r="G111" s="155"/>
       <c r="H111" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I111" s="50"/>
       <c r="J111" s="48"/>
-      <c r="K111" s="159"/>
+      <c r="K111" s="161"/>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B112" s="140"/>
-      <c r="C112" s="141"/>
-      <c r="D112" s="146"/>
-      <c r="E112" s="147"/>
-      <c r="F112" s="152"/>
-      <c r="G112" s="153"/>
+      <c r="B112" s="142"/>
+      <c r="C112" s="143"/>
+      <c r="D112" s="148"/>
+      <c r="E112" s="149"/>
+      <c r="F112" s="154"/>
+      <c r="G112" s="155"/>
       <c r="H112" s="130" t="s">
         <v>46</v>
       </c>
@@ -5266,45 +5284,45 @@
         <v>47</v>
       </c>
       <c r="J112" s="130"/>
-      <c r="K112" s="159"/>
+      <c r="K112" s="161"/>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" s="51">
         <v>17</v>
       </c>
-      <c r="B113" s="142"/>
-      <c r="C113" s="143"/>
-      <c r="D113" s="148"/>
-      <c r="E113" s="149"/>
-      <c r="F113" s="154"/>
-      <c r="G113" s="155"/>
+      <c r="B113" s="144"/>
+      <c r="C113" s="145"/>
+      <c r="D113" s="150"/>
+      <c r="E113" s="151"/>
+      <c r="F113" s="156"/>
+      <c r="G113" s="157"/>
       <c r="H113" s="50">
         <v>43434</v>
       </c>
       <c r="I113" s="50"/>
       <c r="J113" s="48"/>
-      <c r="K113" s="160"/>
+      <c r="K113" s="162"/>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B114" s="135" t="s">
+      <c r="B114" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C114" s="136"/>
-      <c r="D114" s="135" t="s">
+      <c r="C114" s="138"/>
+      <c r="D114" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E114" s="136"/>
-      <c r="F114" s="135" t="s">
+      <c r="E114" s="138"/>
+      <c r="F114" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G114" s="136"/>
-      <c r="H114" s="137" t="s">
+      <c r="G114" s="138"/>
+      <c r="H114" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I114" s="137"/>
+      <c r="I114" s="139"/>
       <c r="J114" s="130" t="s">
         <v>39</v>
       </c>
@@ -5316,35 +5334,35 @@
       <c r="A115" s="48">
         <v>18</v>
       </c>
-      <c r="B115" s="138" t="s">
+      <c r="B115" s="140" t="s">
         <v>124</v>
       </c>
-      <c r="C115" s="139"/>
-      <c r="D115" s="144" t="s">
+      <c r="C115" s="141"/>
+      <c r="D115" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="E115" s="145"/>
-      <c r="F115" s="150" t="s">
+      <c r="E115" s="147"/>
+      <c r="F115" s="152" t="s">
         <v>130</v>
       </c>
-      <c r="G115" s="151"/>
-      <c r="H115" s="156" t="s">
+      <c r="G115" s="153"/>
+      <c r="H115" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I115" s="157"/>
+      <c r="I115" s="159"/>
       <c r="J115" s="52"/>
-      <c r="K115" s="158"/>
+      <c r="K115" s="160"/>
     </row>
     <row r="116" spans="1:11">
       <c r="A116" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B116" s="140"/>
-      <c r="C116" s="141"/>
-      <c r="D116" s="146"/>
-      <c r="E116" s="147"/>
-      <c r="F116" s="152"/>
-      <c r="G116" s="153"/>
+      <c r="B116" s="142"/>
+      <c r="C116" s="143"/>
+      <c r="D116" s="148"/>
+      <c r="E116" s="149"/>
+      <c r="F116" s="154"/>
+      <c r="G116" s="155"/>
       <c r="H116" s="130" t="s">
         <v>42</v>
       </c>
@@ -5354,35 +5372,35 @@
       <c r="J116" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="K116" s="159"/>
+      <c r="K116" s="161"/>
     </row>
     <row r="117" spans="1:11">
       <c r="A117" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B117" s="140"/>
-      <c r="C117" s="141"/>
-      <c r="D117" s="146"/>
-      <c r="E117" s="147"/>
-      <c r="F117" s="152"/>
-      <c r="G117" s="153"/>
+      <c r="B117" s="142"/>
+      <c r="C117" s="143"/>
+      <c r="D117" s="148"/>
+      <c r="E117" s="149"/>
+      <c r="F117" s="154"/>
+      <c r="G117" s="155"/>
       <c r="H117" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I117" s="50"/>
       <c r="J117" s="48"/>
-      <c r="K117" s="159"/>
+      <c r="K117" s="161"/>
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B118" s="140"/>
-      <c r="C118" s="141"/>
-      <c r="D118" s="146"/>
-      <c r="E118" s="147"/>
-      <c r="F118" s="152"/>
-      <c r="G118" s="153"/>
+      <c r="B118" s="142"/>
+      <c r="C118" s="143"/>
+      <c r="D118" s="148"/>
+      <c r="E118" s="149"/>
+      <c r="F118" s="154"/>
+      <c r="G118" s="155"/>
       <c r="H118" s="130" t="s">
         <v>46</v>
       </c>
@@ -5390,62 +5408,62 @@
         <v>47</v>
       </c>
       <c r="J118" s="130"/>
-      <c r="K118" s="159"/>
+      <c r="K118" s="161"/>
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="51">
         <v>18</v>
       </c>
-      <c r="B119" s="142"/>
-      <c r="C119" s="143"/>
-      <c r="D119" s="148"/>
-      <c r="E119" s="149"/>
-      <c r="F119" s="154"/>
-      <c r="G119" s="155"/>
+      <c r="B119" s="144"/>
+      <c r="C119" s="145"/>
+      <c r="D119" s="150"/>
+      <c r="E119" s="151"/>
+      <c r="F119" s="156"/>
+      <c r="G119" s="157"/>
       <c r="H119" s="50">
         <v>43434</v>
       </c>
       <c r="I119" s="50"/>
       <c r="J119" s="48"/>
-      <c r="K119" s="160"/>
+      <c r="K119" s="162"/>
     </row>
     <row r="120" spans="1:11">
       <c r="A120" s="98" t="s">
         <v>131</v>
       </c>
-      <c r="B120" s="165" t="s">
+      <c r="B120" s="163" t="s">
         <v>132</v>
       </c>
-      <c r="C120" s="165"/>
-      <c r="D120" s="166"/>
-      <c r="E120" s="166"/>
-      <c r="F120" s="166"/>
-      <c r="G120" s="166"/>
-      <c r="H120" s="166"/>
-      <c r="I120" s="166"/>
-      <c r="J120" s="166"/>
-      <c r="K120" s="166"/>
+      <c r="C120" s="163"/>
+      <c r="D120" s="164"/>
+      <c r="E120" s="164"/>
+      <c r="F120" s="164"/>
+      <c r="G120" s="164"/>
+      <c r="H120" s="164"/>
+      <c r="I120" s="164"/>
+      <c r="J120" s="164"/>
+      <c r="K120" s="164"/>
     </row>
     <row r="121" spans="1:11">
       <c r="A121" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="B121" s="135" t="s">
+      <c r="B121" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C121" s="136"/>
-      <c r="D121" s="135" t="s">
+      <c r="C121" s="138"/>
+      <c r="D121" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E121" s="136"/>
-      <c r="F121" s="135" t="s">
+      <c r="E121" s="138"/>
+      <c r="F121" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G121" s="136"/>
-      <c r="H121" s="137" t="s">
+      <c r="G121" s="138"/>
+      <c r="H121" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I121" s="137"/>
+      <c r="I121" s="139"/>
       <c r="J121" s="132" t="s">
         <v>39</v>
       </c>
@@ -5457,35 +5475,35 @@
       <c r="A122" s="48">
         <v>19</v>
       </c>
-      <c r="B122" s="138" t="s">
+      <c r="B122" s="140" t="s">
         <v>135</v>
       </c>
-      <c r="C122" s="139"/>
-      <c r="D122" s="144" t="s">
+      <c r="C122" s="141"/>
+      <c r="D122" s="146" t="s">
         <v>136</v>
       </c>
-      <c r="E122" s="145"/>
-      <c r="F122" s="150" t="s">
+      <c r="E122" s="147"/>
+      <c r="F122" s="152" t="s">
         <v>137</v>
       </c>
-      <c r="G122" s="151"/>
-      <c r="H122" s="156" t="s">
+      <c r="G122" s="153"/>
+      <c r="H122" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I122" s="157"/>
+      <c r="I122" s="159"/>
       <c r="J122" s="52"/>
-      <c r="K122" s="158"/>
+      <c r="K122" s="160"/>
     </row>
     <row r="123" spans="1:11">
       <c r="A123" s="132" t="s">
         <v>41</v>
       </c>
-      <c r="B123" s="140"/>
-      <c r="C123" s="141"/>
-      <c r="D123" s="146"/>
-      <c r="E123" s="147"/>
-      <c r="F123" s="152"/>
-      <c r="G123" s="153"/>
+      <c r="B123" s="142"/>
+      <c r="C123" s="143"/>
+      <c r="D123" s="148"/>
+      <c r="E123" s="149"/>
+      <c r="F123" s="154"/>
+      <c r="G123" s="155"/>
       <c r="H123" s="132" t="s">
         <v>42</v>
       </c>
@@ -5495,35 +5513,35 @@
       <c r="J123" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K123" s="159"/>
+      <c r="K123" s="161"/>
     </row>
     <row r="124" spans="1:11">
       <c r="A124" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="B124" s="140"/>
-      <c r="C124" s="141"/>
-      <c r="D124" s="146"/>
-      <c r="E124" s="147"/>
-      <c r="F124" s="152"/>
-      <c r="G124" s="153"/>
+      <c r="B124" s="142"/>
+      <c r="C124" s="143"/>
+      <c r="D124" s="148"/>
+      <c r="E124" s="149"/>
+      <c r="F124" s="154"/>
+      <c r="G124" s="155"/>
       <c r="H124" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I124" s="50"/>
       <c r="J124" s="48"/>
-      <c r="K124" s="159"/>
+      <c r="K124" s="161"/>
     </row>
     <row r="125" spans="1:11">
       <c r="A125" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="B125" s="140"/>
-      <c r="C125" s="141"/>
-      <c r="D125" s="146"/>
-      <c r="E125" s="147"/>
-      <c r="F125" s="152"/>
-      <c r="G125" s="153"/>
+      <c r="B125" s="142"/>
+      <c r="C125" s="143"/>
+      <c r="D125" s="148"/>
+      <c r="E125" s="149"/>
+      <c r="F125" s="154"/>
+      <c r="G125" s="155"/>
       <c r="H125" s="132" t="s">
         <v>46</v>
       </c>
@@ -5531,45 +5549,45 @@
         <v>47</v>
       </c>
       <c r="J125" s="132"/>
-      <c r="K125" s="159"/>
+      <c r="K125" s="161"/>
     </row>
     <row r="126" spans="1:11">
       <c r="A126" s="51">
         <v>19</v>
       </c>
-      <c r="B126" s="142"/>
-      <c r="C126" s="143"/>
-      <c r="D126" s="148"/>
-      <c r="E126" s="149"/>
-      <c r="F126" s="154"/>
-      <c r="G126" s="155"/>
+      <c r="B126" s="144"/>
+      <c r="C126" s="145"/>
+      <c r="D126" s="150"/>
+      <c r="E126" s="151"/>
+      <c r="F126" s="156"/>
+      <c r="G126" s="157"/>
       <c r="H126" s="50">
         <v>43434</v>
       </c>
       <c r="I126" s="50"/>
       <c r="J126" s="48"/>
-      <c r="K126" s="160"/>
+      <c r="K126" s="162"/>
     </row>
     <row r="127" spans="1:11">
       <c r="A127" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="B127" s="135" t="s">
+      <c r="B127" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C127" s="136"/>
-      <c r="D127" s="135" t="s">
+      <c r="C127" s="138"/>
+      <c r="D127" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E127" s="136"/>
-      <c r="F127" s="135" t="s">
+      <c r="E127" s="138"/>
+      <c r="F127" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G127" s="136"/>
-      <c r="H127" s="137" t="s">
+      <c r="G127" s="138"/>
+      <c r="H127" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I127" s="137"/>
+      <c r="I127" s="139"/>
       <c r="J127" s="132" t="s">
         <v>39</v>
       </c>
@@ -5581,35 +5599,35 @@
       <c r="A128" s="48">
         <v>20</v>
       </c>
-      <c r="B128" s="138" t="s">
+      <c r="B128" s="140" t="s">
         <v>138</v>
       </c>
-      <c r="C128" s="139"/>
-      <c r="D128" s="144" t="s">
+      <c r="C128" s="141"/>
+      <c r="D128" s="146" t="s">
         <v>139</v>
       </c>
-      <c r="E128" s="145"/>
-      <c r="F128" s="150" t="s">
+      <c r="E128" s="147"/>
+      <c r="F128" s="152" t="s">
         <v>140</v>
       </c>
-      <c r="G128" s="151"/>
-      <c r="H128" s="156" t="s">
+      <c r="G128" s="153"/>
+      <c r="H128" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I128" s="157"/>
+      <c r="I128" s="159"/>
       <c r="J128" s="52"/>
-      <c r="K128" s="158"/>
+      <c r="K128" s="160"/>
     </row>
     <row r="129" spans="1:11">
       <c r="A129" s="132" t="s">
         <v>41</v>
       </c>
-      <c r="B129" s="140"/>
-      <c r="C129" s="141"/>
-      <c r="D129" s="146"/>
-      <c r="E129" s="147"/>
-      <c r="F129" s="152"/>
-      <c r="G129" s="153"/>
+      <c r="B129" s="142"/>
+      <c r="C129" s="143"/>
+      <c r="D129" s="148"/>
+      <c r="E129" s="149"/>
+      <c r="F129" s="154"/>
+      <c r="G129" s="155"/>
       <c r="H129" s="132" t="s">
         <v>42</v>
       </c>
@@ -5619,35 +5637,35 @@
       <c r="J129" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K129" s="159"/>
+      <c r="K129" s="161"/>
     </row>
     <row r="130" spans="1:11">
       <c r="A130" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="140"/>
-      <c r="C130" s="141"/>
-      <c r="D130" s="146"/>
-      <c r="E130" s="147"/>
-      <c r="F130" s="152"/>
-      <c r="G130" s="153"/>
+      <c r="B130" s="142"/>
+      <c r="C130" s="143"/>
+      <c r="D130" s="148"/>
+      <c r="E130" s="149"/>
+      <c r="F130" s="154"/>
+      <c r="G130" s="155"/>
       <c r="H130" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I130" s="50"/>
       <c r="J130" s="48"/>
-      <c r="K130" s="159"/>
+      <c r="K130" s="161"/>
     </row>
     <row r="131" spans="1:11">
       <c r="A131" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="B131" s="140"/>
-      <c r="C131" s="141"/>
-      <c r="D131" s="146"/>
-      <c r="E131" s="147"/>
-      <c r="F131" s="152"/>
-      <c r="G131" s="153"/>
+      <c r="B131" s="142"/>
+      <c r="C131" s="143"/>
+      <c r="D131" s="148"/>
+      <c r="E131" s="149"/>
+      <c r="F131" s="154"/>
+      <c r="G131" s="155"/>
       <c r="H131" s="132" t="s">
         <v>46</v>
       </c>
@@ -5655,175 +5673,212 @@
         <v>47</v>
       </c>
       <c r="J131" s="132"/>
-      <c r="K131" s="159"/>
+      <c r="K131" s="161"/>
     </row>
     <row r="132" spans="1:11">
       <c r="A132" s="51">
         <v>20</v>
       </c>
-      <c r="B132" s="142"/>
-      <c r="C132" s="143"/>
-      <c r="D132" s="148"/>
-      <c r="E132" s="149"/>
-      <c r="F132" s="154"/>
-      <c r="G132" s="155"/>
+      <c r="B132" s="144"/>
+      <c r="C132" s="145"/>
+      <c r="D132" s="150"/>
+      <c r="E132" s="151"/>
+      <c r="F132" s="156"/>
+      <c r="G132" s="157"/>
       <c r="H132" s="50">
         <v>43434</v>
       </c>
       <c r="I132" s="50"/>
       <c r="J132" s="48"/>
-      <c r="K132" s="160"/>
+      <c r="K132" s="162"/>
     </row>
     <row r="133" spans="1:11">
-      <c r="A133" s="1"/>
-      <c r="H133" s="1"/>
-      <c r="I133" s="1"/>
-      <c r="J133" s="1"/>
-      <c r="K133" s="1"/>
+      <c r="A133" s="134" t="s">
+        <v>34</v>
+      </c>
+      <c r="B133" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C133" s="138"/>
+      <c r="D133" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="E133" s="138"/>
+      <c r="F133" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="G133" s="138"/>
+      <c r="H133" s="139" t="s">
+        <v>38</v>
+      </c>
+      <c r="I133" s="139"/>
+      <c r="J133" s="134" t="s">
+        <v>39</v>
+      </c>
+      <c r="K133" s="133" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="134" spans="1:11">
-      <c r="A134" s="1"/>
-      <c r="H134" s="1"/>
-      <c r="I134" s="1"/>
-      <c r="J134" s="1"/>
-      <c r="K134" s="1"/>
+      <c r="A134" s="48">
+        <v>21</v>
+      </c>
+      <c r="B134" s="140" t="s">
+        <v>142</v>
+      </c>
+      <c r="C134" s="141"/>
+      <c r="D134" s="146" t="s">
+        <v>143</v>
+      </c>
+      <c r="E134" s="147"/>
+      <c r="F134" s="152" t="s">
+        <v>144</v>
+      </c>
+      <c r="G134" s="153"/>
+      <c r="H134" s="158" t="s">
+        <v>9</v>
+      </c>
+      <c r="I134" s="159"/>
+      <c r="J134" s="52"/>
+      <c r="K134" s="160"/>
     </row>
     <row r="135" spans="1:11">
-      <c r="A135" s="1"/>
-      <c r="H135" s="1"/>
-      <c r="I135" s="1"/>
-      <c r="J135" s="1"/>
-      <c r="K135" s="1"/>
+      <c r="A135" s="134" t="s">
+        <v>41</v>
+      </c>
+      <c r="B135" s="142"/>
+      <c r="C135" s="143"/>
+      <c r="D135" s="148"/>
+      <c r="E135" s="149"/>
+      <c r="F135" s="154"/>
+      <c r="G135" s="155"/>
+      <c r="H135" s="134" t="s">
+        <v>42</v>
+      </c>
+      <c r="I135" s="134" t="s">
+        <v>43</v>
+      </c>
+      <c r="J135" s="134" t="s">
+        <v>44</v>
+      </c>
+      <c r="K135" s="161"/>
     </row>
     <row r="136" spans="1:11">
-      <c r="A136" s="1"/>
-      <c r="H136" s="1"/>
-      <c r="I136" s="1"/>
-      <c r="J136" s="1"/>
-      <c r="K136" s="1"/>
+      <c r="A136" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B136" s="142"/>
+      <c r="C136" s="143"/>
+      <c r="D136" s="148"/>
+      <c r="E136" s="149"/>
+      <c r="F136" s="154"/>
+      <c r="G136" s="155"/>
+      <c r="H136" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I136" s="50"/>
+      <c r="J136" s="48"/>
+      <c r="K136" s="161"/>
     </row>
     <row r="137" spans="1:11">
-      <c r="A137" s="1"/>
-      <c r="H137" s="1"/>
-      <c r="I137" s="1"/>
-      <c r="J137" s="1"/>
-      <c r="K137" s="1"/>
+      <c r="A137" s="134" t="s">
+        <v>45</v>
+      </c>
+      <c r="B137" s="142"/>
+      <c r="C137" s="143"/>
+      <c r="D137" s="148"/>
+      <c r="E137" s="149"/>
+      <c r="F137" s="154"/>
+      <c r="G137" s="155"/>
+      <c r="H137" s="134" t="s">
+        <v>46</v>
+      </c>
+      <c r="I137" s="134" t="s">
+        <v>47</v>
+      </c>
+      <c r="J137" s="134"/>
+      <c r="K137" s="161"/>
     </row>
     <row r="138" spans="1:11">
-      <c r="A138" s="1"/>
-      <c r="H138" s="1"/>
-      <c r="I138" s="1"/>
-      <c r="J138" s="1"/>
-      <c r="K138" s="1"/>
+      <c r="A138" s="51">
+        <v>21</v>
+      </c>
+      <c r="B138" s="144"/>
+      <c r="C138" s="145"/>
+      <c r="D138" s="150"/>
+      <c r="E138" s="151"/>
+      <c r="F138" s="156"/>
+      <c r="G138" s="157"/>
+      <c r="H138" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I138" s="50"/>
+      <c r="J138" s="48"/>
+      <c r="K138" s="162"/>
     </row>
   </sheetData>
-  <mergeCells count="186">
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="F127:G127"/>
-    <mergeCell ref="H127:I127"/>
-    <mergeCell ref="B128:C132"/>
-    <mergeCell ref="D128:E132"/>
-    <mergeCell ref="F128:G132"/>
-    <mergeCell ref="H128:I128"/>
-    <mergeCell ref="K128:K132"/>
-    <mergeCell ref="B120:K120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="H121:I121"/>
-    <mergeCell ref="B122:C126"/>
-    <mergeCell ref="D122:E126"/>
-    <mergeCell ref="F122:G126"/>
-    <mergeCell ref="H122:I122"/>
-    <mergeCell ref="K122:K126"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="B90:C94"/>
-    <mergeCell ref="D90:E94"/>
-    <mergeCell ref="F90:G94"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="K90:K94"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="B84:C88"/>
-    <mergeCell ref="D84:E88"/>
-    <mergeCell ref="F84:G88"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="K84:K88"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="B78:C82"/>
-    <mergeCell ref="D78:E82"/>
-    <mergeCell ref="F78:G82"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="B65:C69"/>
-    <mergeCell ref="D65:E69"/>
-    <mergeCell ref="F65:G69"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="K65:K69"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="B59:C63"/>
-    <mergeCell ref="D59:E63"/>
-    <mergeCell ref="F59:G63"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="K59:K63"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="B53:C57"/>
-    <mergeCell ref="D53:E57"/>
-    <mergeCell ref="F53:G57"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="K53:K57"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="K34:K38"/>
-    <mergeCell ref="K28:K32"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B34:C38"/>
-    <mergeCell ref="D34:E38"/>
-    <mergeCell ref="F34:G38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B40:C44"/>
-    <mergeCell ref="D40:E44"/>
-    <mergeCell ref="F40:G44"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B46:C50"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F28:G32"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="D28:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="B28:C32"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:E25"/>
-    <mergeCell ref="F21:G25"/>
+  <mergeCells count="195">
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="F133:G133"/>
+    <mergeCell ref="H133:I133"/>
+    <mergeCell ref="B134:C138"/>
+    <mergeCell ref="D134:E138"/>
+    <mergeCell ref="F134:G138"/>
+    <mergeCell ref="H134:I134"/>
+    <mergeCell ref="K134:K138"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="B115:C119"/>
+    <mergeCell ref="D115:E119"/>
+    <mergeCell ref="F115:G119"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="K115:K119"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="B109:C113"/>
+    <mergeCell ref="D109:E113"/>
+    <mergeCell ref="F109:G113"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="K109:K113"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="B103:C107"/>
+    <mergeCell ref="D103:E107"/>
+    <mergeCell ref="F103:G107"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="K103:K107"/>
+    <mergeCell ref="B95:K95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="B97:C101"/>
+    <mergeCell ref="D97:E101"/>
+    <mergeCell ref="F97:G101"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="K97:K101"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B72:C76"/>
+    <mergeCell ref="D72:E76"/>
+    <mergeCell ref="F72:G76"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="K72:K76"/>
+    <mergeCell ref="B70:K70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="H8:I8"/>
@@ -5848,62 +5903,116 @@
     <mergeCell ref="B15:C19"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="K21:K25"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F28:G32"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D28:E32"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="F21:G25"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="K34:K38"/>
+    <mergeCell ref="K28:K32"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:C38"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="F34:G38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B40:C44"/>
+    <mergeCell ref="D40:E44"/>
+    <mergeCell ref="F40:G44"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="D46:E50"/>
     <mergeCell ref="F46:G50"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="K46:K50"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B72:C76"/>
-    <mergeCell ref="D72:E76"/>
-    <mergeCell ref="F72:G76"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="K72:K76"/>
-    <mergeCell ref="B70:K70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="B95:K95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="B97:C101"/>
-    <mergeCell ref="D97:E101"/>
-    <mergeCell ref="F97:G101"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="K97:K101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="B103:C107"/>
-    <mergeCell ref="D103:E107"/>
-    <mergeCell ref="F103:G107"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="K103:K107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="B109:C113"/>
-    <mergeCell ref="D109:E113"/>
-    <mergeCell ref="F109:G113"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="K109:K113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="B115:C119"/>
-    <mergeCell ref="D115:E119"/>
-    <mergeCell ref="F115:G119"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="K115:K119"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B53:C57"/>
+    <mergeCell ref="D53:E57"/>
+    <mergeCell ref="F53:G57"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:K57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B59:C63"/>
+    <mergeCell ref="D59:E63"/>
+    <mergeCell ref="F59:G63"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="K59:K63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="B65:C69"/>
+    <mergeCell ref="D65:E69"/>
+    <mergeCell ref="F65:G69"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="K65:K69"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="B78:C82"/>
+    <mergeCell ref="D78:E82"/>
+    <mergeCell ref="F78:G82"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="B84:C88"/>
+    <mergeCell ref="D84:E88"/>
+    <mergeCell ref="F84:G88"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="K84:K88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="B90:C94"/>
+    <mergeCell ref="D90:E94"/>
+    <mergeCell ref="F90:G94"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="K90:K94"/>
+    <mergeCell ref="B120:K120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="B122:C126"/>
+    <mergeCell ref="D122:E126"/>
+    <mergeCell ref="F122:G126"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="K122:K126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="F127:G127"/>
+    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="B128:C132"/>
+    <mergeCell ref="D128:E132"/>
+    <mergeCell ref="F128:G132"/>
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="K128:K132"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H34:I34">

</xml_diff>

<commit_message>
Add Timkiem test case
</commit_message>
<xml_diff>
--- a/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/Btl/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="154">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -482,6 +482,33 @@
   </si>
   <si>
     <t>Hệ thống hiển thị đúng nội dung đã được nhập ,theo định dạng của một bài viết được định trước</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>TimKiem_01</t>
+  </si>
+  <si>
+    <t>7-1</t>
+  </si>
+  <si>
+    <t>7-2</t>
+  </si>
+  <si>
+    <t>TimKiem_02</t>
+  </si>
+  <si>
+    <t>Tìm kiếm theo từ khoá</t>
+  </si>
+  <si>
+    <t>Tìm kiếm món ăn</t>
+  </si>
+  <si>
+    <t>danh sách các món ăn nếu có, ngược lại thông báo "không có kết quả nào được tìm thấy"</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nâng cao</t>
   </si>
 </sst>
 </file>
@@ -2976,10 +3003,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K138"/>
+  <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A115" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A128" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147:E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3011,7 +3038,7 @@
       </c>
       <c r="I1" s="99">
         <f>COUNTIF(H1:H761,"OK")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J1" s="81" t="s">
         <v>23</v>
@@ -3079,7 +3106,7 @@
       <c r="H4" s="84"/>
       <c r="I4" s="100">
         <f>COUNTIF(H3:H763,"Result")</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J4" s="88"/>
       <c r="K4" s="89"/>
@@ -5816,8 +5843,292 @@
       <c r="J138" s="48"/>
       <c r="K138" s="162"/>
     </row>
+    <row r="139" spans="1:11">
+      <c r="A139" s="98" t="s">
+        <v>145</v>
+      </c>
+      <c r="B139" s="163" t="s">
+        <v>151</v>
+      </c>
+      <c r="C139" s="163"/>
+      <c r="D139" s="164"/>
+      <c r="E139" s="164"/>
+      <c r="F139" s="164"/>
+      <c r="G139" s="164"/>
+      <c r="H139" s="164"/>
+      <c r="I139" s="164"/>
+      <c r="J139" s="164"/>
+      <c r="K139" s="164"/>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="A140" s="134" t="s">
+        <v>34</v>
+      </c>
+      <c r="B140" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C140" s="138"/>
+      <c r="D140" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="E140" s="138"/>
+      <c r="F140" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="G140" s="138"/>
+      <c r="H140" s="139" t="s">
+        <v>38</v>
+      </c>
+      <c r="I140" s="139"/>
+      <c r="J140" s="134" t="s">
+        <v>39</v>
+      </c>
+      <c r="K140" s="133" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" s="48">
+        <v>22</v>
+      </c>
+      <c r="B141" s="140" t="s">
+        <v>146</v>
+      </c>
+      <c r="C141" s="141"/>
+      <c r="D141" s="146" t="s">
+        <v>150</v>
+      </c>
+      <c r="E141" s="147"/>
+      <c r="F141" s="152" t="s">
+        <v>152</v>
+      </c>
+      <c r="G141" s="153"/>
+      <c r="H141" s="158" t="s">
+        <v>9</v>
+      </c>
+      <c r="I141" s="159"/>
+      <c r="J141" s="52"/>
+      <c r="K141" s="160"/>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" s="134" t="s">
+        <v>41</v>
+      </c>
+      <c r="B142" s="142"/>
+      <c r="C142" s="143"/>
+      <c r="D142" s="148"/>
+      <c r="E142" s="149"/>
+      <c r="F142" s="154"/>
+      <c r="G142" s="155"/>
+      <c r="H142" s="134" t="s">
+        <v>42</v>
+      </c>
+      <c r="I142" s="134" t="s">
+        <v>43</v>
+      </c>
+      <c r="J142" s="134" t="s">
+        <v>44</v>
+      </c>
+      <c r="K142" s="161"/>
+    </row>
+    <row r="143" spans="1:11">
+      <c r="A143" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="B143" s="142"/>
+      <c r="C143" s="143"/>
+      <c r="D143" s="148"/>
+      <c r="E143" s="149"/>
+      <c r="F143" s="154"/>
+      <c r="G143" s="155"/>
+      <c r="H143" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I143" s="50"/>
+      <c r="J143" s="48"/>
+      <c r="K143" s="161"/>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" s="134" t="s">
+        <v>45</v>
+      </c>
+      <c r="B144" s="142"/>
+      <c r="C144" s="143"/>
+      <c r="D144" s="148"/>
+      <c r="E144" s="149"/>
+      <c r="F144" s="154"/>
+      <c r="G144" s="155"/>
+      <c r="H144" s="134" t="s">
+        <v>46</v>
+      </c>
+      <c r="I144" s="134" t="s">
+        <v>47</v>
+      </c>
+      <c r="J144" s="134"/>
+      <c r="K144" s="161"/>
+    </row>
+    <row r="145" spans="1:11">
+      <c r="A145" s="51">
+        <v>22</v>
+      </c>
+      <c r="B145" s="144"/>
+      <c r="C145" s="145"/>
+      <c r="D145" s="150"/>
+      <c r="E145" s="151"/>
+      <c r="F145" s="156"/>
+      <c r="G145" s="157"/>
+      <c r="H145" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I145" s="50"/>
+      <c r="J145" s="48"/>
+      <c r="K145" s="162"/>
+    </row>
+    <row r="146" spans="1:11">
+      <c r="A146" s="134" t="s">
+        <v>34</v>
+      </c>
+      <c r="B146" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="138"/>
+      <c r="D146" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="E146" s="138"/>
+      <c r="F146" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="G146" s="138"/>
+      <c r="H146" s="139" t="s">
+        <v>38</v>
+      </c>
+      <c r="I146" s="139"/>
+      <c r="J146" s="134" t="s">
+        <v>39</v>
+      </c>
+      <c r="K146" s="133" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11">
+      <c r="A147" s="48">
+        <v>23</v>
+      </c>
+      <c r="B147" s="140" t="s">
+        <v>149</v>
+      </c>
+      <c r="C147" s="141"/>
+      <c r="D147" s="146" t="s">
+        <v>153</v>
+      </c>
+      <c r="E147" s="147"/>
+      <c r="F147" s="152" t="s">
+        <v>152</v>
+      </c>
+      <c r="G147" s="153"/>
+      <c r="H147" s="158" t="s">
+        <v>9</v>
+      </c>
+      <c r="I147" s="159"/>
+      <c r="J147" s="52"/>
+      <c r="K147" s="160"/>
+    </row>
+    <row r="148" spans="1:11">
+      <c r="A148" s="134" t="s">
+        <v>41</v>
+      </c>
+      <c r="B148" s="142"/>
+      <c r="C148" s="143"/>
+      <c r="D148" s="148"/>
+      <c r="E148" s="149"/>
+      <c r="F148" s="154"/>
+      <c r="G148" s="155"/>
+      <c r="H148" s="134" t="s">
+        <v>42</v>
+      </c>
+      <c r="I148" s="134" t="s">
+        <v>43</v>
+      </c>
+      <c r="J148" s="134" t="s">
+        <v>44</v>
+      </c>
+      <c r="K148" s="161"/>
+    </row>
+    <row r="149" spans="1:11">
+      <c r="A149" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B149" s="142"/>
+      <c r="C149" s="143"/>
+      <c r="D149" s="148"/>
+      <c r="E149" s="149"/>
+      <c r="F149" s="154"/>
+      <c r="G149" s="155"/>
+      <c r="H149" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I149" s="50"/>
+      <c r="J149" s="48"/>
+      <c r="K149" s="161"/>
+    </row>
+    <row r="150" spans="1:11">
+      <c r="A150" s="134" t="s">
+        <v>45</v>
+      </c>
+      <c r="B150" s="142"/>
+      <c r="C150" s="143"/>
+      <c r="D150" s="148"/>
+      <c r="E150" s="149"/>
+      <c r="F150" s="154"/>
+      <c r="G150" s="155"/>
+      <c r="H150" s="134" t="s">
+        <v>46</v>
+      </c>
+      <c r="I150" s="134" t="s">
+        <v>47</v>
+      </c>
+      <c r="J150" s="134"/>
+      <c r="K150" s="161"/>
+    </row>
+    <row r="151" spans="1:11">
+      <c r="A151" s="51">
+        <v>23</v>
+      </c>
+      <c r="B151" s="144"/>
+      <c r="C151" s="145"/>
+      <c r="D151" s="150"/>
+      <c r="E151" s="151"/>
+      <c r="F151" s="156"/>
+      <c r="G151" s="157"/>
+      <c r="H151" s="50">
+        <v>43434</v>
+      </c>
+      <c r="I151" s="50"/>
+      <c r="J151" s="48"/>
+      <c r="K151" s="162"/>
+    </row>
   </sheetData>
-  <mergeCells count="195">
+  <mergeCells count="214">
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="F146:G146"/>
+    <mergeCell ref="H146:I146"/>
+    <mergeCell ref="B147:C151"/>
+    <mergeCell ref="D147:E151"/>
+    <mergeCell ref="F147:G151"/>
+    <mergeCell ref="H147:I147"/>
+    <mergeCell ref="K147:K151"/>
+    <mergeCell ref="B139:K139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="F140:G140"/>
+    <mergeCell ref="H140:I140"/>
+    <mergeCell ref="B141:C145"/>
+    <mergeCell ref="D141:E145"/>
+    <mergeCell ref="F141:G145"/>
+    <mergeCell ref="H141:I141"/>
+    <mergeCell ref="K141:K145"/>
     <mergeCell ref="B133:C133"/>
     <mergeCell ref="D133:E133"/>
     <mergeCell ref="F133:G133"/>

</xml_diff>